<commit_message>
Update Team 3  - Del 6 CRUD Matrix
</commit_message>
<xml_diff>
--- a/Documentation/Team 3  - Del 6 CRUD Matrix.xlsx
+++ b/Documentation/Team 3  - Del 6 CRUD Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Team-3-Orion\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50471EB6-CC04-4979-B025-F17457A9C125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7054B26-6B95-418D-B4A5-58C32F262665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Table 1'!$A$1:$DF$238</definedName>
   </definedNames>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="435">
   <si>
     <r>
       <rPr>
@@ -2086,13 +2086,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2101,56 +2095,14 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -2167,13 +2119,61 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2516,11 +2516,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DF238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="AC139" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="BA115" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AQ141" sqref="AQ141"/>
+      <selection pane="bottomRight" activeCell="BF2" sqref="BF2:BH2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="6" x14ac:dyDescent="0.2"/>
@@ -2580,141 +2580,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="23"/>
+      <c r="A1" s="44"/>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="28" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="28" t="s">
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="28" t="s">
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="45" t="s">
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+      <c r="AE1" s="28"/>
+      <c r="AF1" s="28"/>
+      <c r="AG1" s="28"/>
+      <c r="AH1" s="28"/>
+      <c r="AI1" s="28"/>
+      <c r="AJ1" s="28"/>
+      <c r="AK1" s="28"/>
+      <c r="AL1" s="28"/>
+      <c r="AM1" s="28"/>
+      <c r="AN1" s="28"/>
+      <c r="AO1" s="28"/>
+      <c r="AP1" s="28"/>
+      <c r="AQ1" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="47"/>
-      <c r="BB1" s="45" t="s">
+      <c r="AR1" s="30"/>
+      <c r="AS1" s="30"/>
+      <c r="AT1" s="30"/>
+      <c r="AU1" s="30"/>
+      <c r="AV1" s="30"/>
+      <c r="AW1" s="30"/>
+      <c r="AX1" s="30"/>
+      <c r="AY1" s="30"/>
+      <c r="AZ1" s="30"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="46"/>
-      <c r="BE1" s="46"/>
-      <c r="BF1" s="46"/>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="47"/>
-      <c r="BQ1" s="48" t="s">
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30"/>
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30"/>
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
+      <c r="BO1" s="30"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" s="49"/>
-      <c r="BS1" s="49"/>
-      <c r="BT1" s="49"/>
-      <c r="BU1" s="44" t="s">
+      <c r="BR1" s="33"/>
+      <c r="BS1" s="33"/>
+      <c r="BT1" s="33"/>
+      <c r="BU1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BV1" s="26"/>
-      <c r="BW1" s="26"/>
-      <c r="BX1" s="26"/>
-      <c r="BY1" s="26"/>
-      <c r="BZ1" s="26"/>
-      <c r="CA1" s="26"/>
-      <c r="CB1" s="26"/>
-      <c r="CC1" s="26"/>
-      <c r="CD1" s="26"/>
-      <c r="CE1" s="26"/>
-      <c r="CF1" s="26"/>
-      <c r="CG1" s="26"/>
-      <c r="CH1" s="26"/>
-      <c r="CI1" s="26"/>
-      <c r="CJ1" s="26"/>
-      <c r="CK1" s="26"/>
-      <c r="CL1" s="27"/>
-      <c r="CM1" s="44" t="s">
+      <c r="BV1" s="24"/>
+      <c r="BW1" s="24"/>
+      <c r="BX1" s="24"/>
+      <c r="BY1" s="24"/>
+      <c r="BZ1" s="24"/>
+      <c r="CA1" s="24"/>
+      <c r="CB1" s="24"/>
+      <c r="CC1" s="24"/>
+      <c r="CD1" s="24"/>
+      <c r="CE1" s="24"/>
+      <c r="CF1" s="24"/>
+      <c r="CG1" s="24"/>
+      <c r="CH1" s="24"/>
+      <c r="CI1" s="24"/>
+      <c r="CJ1" s="24"/>
+      <c r="CK1" s="24"/>
+      <c r="CL1" s="25"/>
+      <c r="CM1" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="CN1" s="26"/>
-      <c r="CO1" s="26"/>
-      <c r="CP1" s="26"/>
-      <c r="CQ1" s="26"/>
-      <c r="CR1" s="26"/>
-      <c r="CS1" s="26"/>
-      <c r="CT1" s="26"/>
-      <c r="CU1" s="26"/>
-      <c r="CV1" s="27"/>
-      <c r="CW1" s="44" t="s">
+      <c r="CN1" s="24"/>
+      <c r="CO1" s="24"/>
+      <c r="CP1" s="24"/>
+      <c r="CQ1" s="24"/>
+      <c r="CR1" s="24"/>
+      <c r="CS1" s="24"/>
+      <c r="CT1" s="24"/>
+      <c r="CU1" s="24"/>
+      <c r="CV1" s="25"/>
+      <c r="CW1" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="CX1" s="26"/>
-      <c r="CY1" s="26"/>
-      <c r="CZ1" s="26"/>
-      <c r="DA1" s="26"/>
-      <c r="DB1" s="26"/>
-      <c r="DC1" s="26"/>
-      <c r="DD1" s="26"/>
-      <c r="DE1" s="26"/>
-      <c r="DF1" s="27"/>
+      <c r="CX1" s="24"/>
+      <c r="CY1" s="24"/>
+      <c r="CZ1" s="24"/>
+      <c r="DA1" s="24"/>
+      <c r="DB1" s="24"/>
+      <c r="DC1" s="24"/>
+      <c r="DD1" s="24"/>
+      <c r="DE1" s="24"/>
+      <c r="DF1" s="25"/>
     </row>
     <row r="2" spans="1:110" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="24"/>
+      <c r="A2" s="45"/>
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -3376,7 +3376,7 @@
       </c>
     </row>
     <row r="4" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="48" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3496,7 +3496,7 @@
       <c r="DF4" s="20"/>
     </row>
     <row r="5" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="36"/>
+      <c r="A5" s="49"/>
       <c r="B5" s="2" t="s">
         <v>134</v>
       </c>
@@ -3614,7 +3614,7 @@
       <c r="DF5" s="20"/>
     </row>
     <row r="6" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="36"/>
+      <c r="A6" s="49"/>
       <c r="B6" s="2" t="s">
         <v>135</v>
       </c>
@@ -3728,7 +3728,7 @@
       <c r="DF6" s="20"/>
     </row>
     <row r="7" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="37"/>
+      <c r="A7" s="50"/>
       <c r="B7" s="2" t="s">
         <v>136</v>
       </c>
@@ -3842,7 +3842,7 @@
       <c r="DF7" s="20"/>
     </row>
     <row r="8" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="34" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3962,7 +3962,7 @@
       <c r="DF8" s="21"/>
     </row>
     <row r="9" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="31"/>
+      <c r="A9" s="35"/>
       <c r="B9" s="3" t="s">
         <v>138</v>
       </c>
@@ -4076,7 +4076,7 @@
       <c r="DF9" s="21"/>
     </row>
     <row r="10" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="31"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="3" t="s">
         <v>139</v>
       </c>
@@ -4190,7 +4190,7 @@
       <c r="DF10" s="21"/>
     </row>
     <row r="11" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="32" t="s">
+      <c r="A11" s="37" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4312,7 +4312,7 @@
       <c r="DF11" s="20"/>
     </row>
     <row r="12" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="33"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="2" t="s">
         <v>137</v>
       </c>
@@ -4428,7 +4428,7 @@
       <c r="DF12" s="20"/>
     </row>
     <row r="13" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="33"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="2" t="s">
         <v>141</v>
       </c>
@@ -4544,7 +4544,7 @@
       <c r="DF13" s="20"/>
     </row>
     <row r="14" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="33"/>
+      <c r="A14" s="38"/>
       <c r="B14" s="2" t="s">
         <v>142</v>
       </c>
@@ -4662,7 +4662,7 @@
       <c r="DF14" s="20"/>
     </row>
     <row r="15" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="41" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4778,7 +4778,7 @@
       <c r="DF15" s="21"/>
     </row>
     <row r="16" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="39"/>
+      <c r="A16" s="42"/>
       <c r="B16" s="3" t="s">
         <v>144</v>
       </c>
@@ -4892,7 +4892,7 @@
       <c r="DF16" s="21"/>
     </row>
     <row r="17" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="39"/>
+      <c r="A17" s="42"/>
       <c r="B17" s="3" t="s">
         <v>133</v>
       </c>
@@ -5006,7 +5006,7 @@
       <c r="DF17" s="21"/>
     </row>
     <row r="18" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="37" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -5128,7 +5128,7 @@
       <c r="DF18" s="20"/>
     </row>
     <row r="19" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="33"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="2" t="s">
         <v>146</v>
       </c>
@@ -5248,7 +5248,7 @@
       <c r="DF19" s="20"/>
     </row>
     <row r="20" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="33"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="2" t="s">
         <v>147</v>
       </c>
@@ -5362,7 +5362,7 @@
       <c r="DF20" s="20"/>
     </row>
     <row r="21" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="34" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -5478,7 +5478,7 @@
       <c r="DF21" s="21"/>
     </row>
     <row r="22" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="31"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="3" t="s">
         <v>139</v>
       </c>
@@ -5592,7 +5592,7 @@
       <c r="DF22" s="21"/>
     </row>
     <row r="23" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="31"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="3" t="s">
         <v>149</v>
       </c>
@@ -5706,7 +5706,7 @@
       <c r="DF23" s="21"/>
     </row>
     <row r="24" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="37" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5830,7 +5830,7 @@
       <c r="DF24" s="20"/>
     </row>
     <row r="25" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="33"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="2" t="s">
         <v>151</v>
       </c>
@@ -5950,7 +5950,7 @@
       <c r="DF25" s="20"/>
     </row>
     <row r="26" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="33"/>
+      <c r="A26" s="38"/>
       <c r="B26" s="2" t="s">
         <v>152</v>
       </c>
@@ -6070,7 +6070,7 @@
       <c r="DF26" s="20"/>
     </row>
     <row r="27" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="33"/>
+      <c r="A27" s="38"/>
       <c r="B27" s="2" t="s">
         <v>153</v>
       </c>
@@ -6188,7 +6188,7 @@
       <c r="DF27" s="20"/>
     </row>
     <row r="28" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="33"/>
+      <c r="A28" s="38"/>
       <c r="B28" s="2" t="s">
         <v>154</v>
       </c>
@@ -6306,7 +6306,7 @@
       <c r="DF28" s="20"/>
     </row>
     <row r="29" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="33"/>
+      <c r="A29" s="38"/>
       <c r="B29" s="2" t="s">
         <v>155</v>
       </c>
@@ -6424,7 +6424,7 @@
       <c r="DF29" s="20"/>
     </row>
     <row r="30" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="33"/>
+      <c r="A30" s="38"/>
       <c r="B30" s="2" t="s">
         <v>156</v>
       </c>
@@ -6542,7 +6542,7 @@
       <c r="DF30" s="20"/>
     </row>
     <row r="31" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="33"/>
+      <c r="A31" s="38"/>
       <c r="B31" s="2" t="s">
         <v>150</v>
       </c>
@@ -6660,7 +6660,7 @@
       <c r="DF31" s="20"/>
     </row>
     <row r="32" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="33"/>
+      <c r="A32" s="38"/>
       <c r="B32" s="2" t="s">
         <v>138</v>
       </c>
@@ -6774,7 +6774,7 @@
       <c r="DF32" s="20"/>
     </row>
     <row r="33" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="34" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -6890,7 +6890,7 @@
       <c r="DF33" s="21"/>
     </row>
     <row r="34" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="31"/>
+      <c r="A34" s="35"/>
       <c r="B34" s="3" t="s">
         <v>157</v>
       </c>
@@ -7004,7 +7004,7 @@
       <c r="DF34" s="21"/>
     </row>
     <row r="35" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="34"/>
+      <c r="A35" s="40"/>
       <c r="B35" s="3" t="s">
         <v>158</v>
       </c>
@@ -7118,7 +7118,7 @@
       <c r="DF35" s="21"/>
     </row>
     <row r="36" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="32" t="s">
+      <c r="A36" s="37" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -7238,7 +7238,7 @@
       <c r="DF36" s="18"/>
     </row>
     <row r="37" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="33"/>
+      <c r="A37" s="38"/>
       <c r="B37" s="2" t="s">
         <v>160</v>
       </c>
@@ -7356,7 +7356,7 @@
       <c r="DF37" s="18"/>
     </row>
     <row r="38" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="34" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -7472,7 +7472,7 @@
       <c r="DF38" s="15"/>
     </row>
     <row r="39" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="31"/>
+      <c r="A39" s="35"/>
       <c r="B39" s="3" t="s">
         <v>162</v>
       </c>
@@ -7586,7 +7586,7 @@
       <c r="DF39" s="15"/>
     </row>
     <row r="40" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="31"/>
+      <c r="A40" s="35"/>
       <c r="B40" s="3" t="s">
         <v>163</v>
       </c>
@@ -7700,7 +7700,7 @@
       <c r="DF40" s="15"/>
     </row>
     <row r="41" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="31"/>
+      <c r="A41" s="35"/>
       <c r="B41" s="3" t="s">
         <v>159</v>
       </c>
@@ -7814,7 +7814,7 @@
       <c r="DF41" s="15"/>
     </row>
     <row r="42" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="32" t="s">
+      <c r="A42" s="37" t="s">
         <v>79</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -7930,7 +7930,7 @@
       <c r="DF42" s="20"/>
     </row>
     <row r="43" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="33"/>
+      <c r="A43" s="38"/>
       <c r="B43" s="2" t="s">
         <v>164</v>
       </c>
@@ -8044,7 +8044,7 @@
       <c r="DF43" s="20"/>
     </row>
     <row r="44" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="33"/>
+      <c r="A44" s="38"/>
       <c r="B44" s="2" t="s">
         <v>165</v>
       </c>
@@ -8158,7 +8158,7 @@
       <c r="DF44" s="20"/>
     </row>
     <row r="45" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="42"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="2" t="s">
         <v>166</v>
       </c>
@@ -8272,7 +8272,7 @@
       <c r="DF45" s="20"/>
     </row>
     <row r="46" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="34" t="s">
         <v>80</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -8388,7 +8388,7 @@
       <c r="DF46" s="21"/>
     </row>
     <row r="47" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="31"/>
+      <c r="A47" s="35"/>
       <c r="B47" s="3" t="s">
         <v>168</v>
       </c>
@@ -8502,7 +8502,7 @@
       <c r="DF47" s="21"/>
     </row>
     <row r="48" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="31"/>
+      <c r="A48" s="35"/>
       <c r="B48" s="3" t="s">
         <v>169</v>
       </c>
@@ -8616,7 +8616,7 @@
       <c r="DF48" s="21"/>
     </row>
     <row r="49" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="31"/>
+      <c r="A49" s="35"/>
       <c r="B49" s="3" t="s">
         <v>170</v>
       </c>
@@ -8730,7 +8730,7 @@
       <c r="DF49" s="21"/>
     </row>
     <row r="50" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="31"/>
+      <c r="A50" s="35"/>
       <c r="B50" s="3" t="s">
         <v>171</v>
       </c>
@@ -8844,7 +8844,7 @@
       <c r="DF50" s="21"/>
     </row>
     <row r="51" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="31"/>
+      <c r="A51" s="35"/>
       <c r="B51" s="3" t="s">
         <v>172</v>
       </c>
@@ -8958,7 +8958,7 @@
       <c r="DF51" s="21"/>
     </row>
     <row r="52" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="34"/>
+      <c r="A52" s="40"/>
       <c r="B52" s="3" t="s">
         <v>138</v>
       </c>
@@ -9072,7 +9072,7 @@
       <c r="DF52" s="21"/>
     </row>
     <row r="53" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="37" t="s">
         <v>81</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -9188,7 +9188,7 @@
       <c r="DF53" s="20"/>
     </row>
     <row r="54" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="33"/>
+      <c r="A54" s="38"/>
       <c r="B54" s="2" t="s">
         <v>173</v>
       </c>
@@ -9302,7 +9302,7 @@
       <c r="DF54" s="20"/>
     </row>
     <row r="55" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="30" t="s">
+      <c r="A55" s="34" t="s">
         <v>82</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -9418,7 +9418,7 @@
       <c r="DF55" s="21"/>
     </row>
     <row r="56" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="31"/>
+      <c r="A56" s="35"/>
       <c r="B56" s="3" t="s">
         <v>175</v>
       </c>
@@ -9532,7 +9532,7 @@
       <c r="DF56" s="21"/>
     </row>
     <row r="57" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="31"/>
+      <c r="A57" s="35"/>
       <c r="B57" s="3" t="s">
         <v>176</v>
       </c>
@@ -9646,7 +9646,7 @@
       <c r="DF57" s="21"/>
     </row>
     <row r="58" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="31"/>
+      <c r="A58" s="35"/>
       <c r="B58" s="3" t="s">
         <v>141</v>
       </c>
@@ -9760,7 +9760,7 @@
       <c r="DF58" s="21"/>
     </row>
     <row r="59" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="37" t="s">
         <v>83</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -9876,7 +9876,7 @@
       <c r="DF59" s="20"/>
     </row>
     <row r="60" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="33"/>
+      <c r="A60" s="38"/>
       <c r="B60" s="2" t="s">
         <v>178</v>
       </c>
@@ -9990,7 +9990,7 @@
       <c r="DF60" s="20"/>
     </row>
     <row r="61" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="33"/>
+      <c r="A61" s="38"/>
       <c r="B61" s="2" t="s">
         <v>179</v>
       </c>
@@ -10104,7 +10104,7 @@
       <c r="DF61" s="20"/>
     </row>
     <row r="62" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="30" t="s">
+      <c r="A62" s="34" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -10220,7 +10220,7 @@
       <c r="DF62" s="21"/>
     </row>
     <row r="63" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="31"/>
+      <c r="A63" s="35"/>
       <c r="B63" s="3" t="s">
         <v>178</v>
       </c>
@@ -10334,7 +10334,7 @@
       <c r="DF63" s="21"/>
     </row>
     <row r="64" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="31"/>
+      <c r="A64" s="35"/>
       <c r="B64" s="3" t="s">
         <v>177</v>
       </c>
@@ -10448,7 +10448,7 @@
       <c r="DF64" s="21"/>
     </row>
     <row r="65" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="31"/>
+      <c r="A65" s="35"/>
       <c r="B65" s="3" t="s">
         <v>182</v>
       </c>
@@ -10562,7 +10562,7 @@
       <c r="DF65" s="21"/>
     </row>
     <row r="66" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="34"/>
+      <c r="A66" s="40"/>
       <c r="B66" s="3" t="s">
         <v>181</v>
       </c>
@@ -10676,7 +10676,7 @@
       <c r="DF66" s="21"/>
     </row>
     <row r="67" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="32" t="s">
+      <c r="A67" s="37" t="s">
         <v>85</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -10792,7 +10792,7 @@
       <c r="DF67" s="20"/>
     </row>
     <row r="68" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="33"/>
+      <c r="A68" s="38"/>
       <c r="B68" s="2" t="s">
         <v>183</v>
       </c>
@@ -10906,7 +10906,7 @@
       <c r="DF68" s="20"/>
     </row>
     <row r="69" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="30" t="s">
+      <c r="A69" s="34" t="s">
         <v>86</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -11022,7 +11022,7 @@
       <c r="DF69" s="21"/>
     </row>
     <row r="70" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="31"/>
+      <c r="A70" s="35"/>
       <c r="B70" s="3" t="s">
         <v>174</v>
       </c>
@@ -11136,7 +11136,7 @@
       <c r="DF70" s="21"/>
     </row>
     <row r="71" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="31"/>
+      <c r="A71" s="35"/>
       <c r="B71" s="3" t="s">
         <v>184</v>
       </c>
@@ -11250,7 +11250,7 @@
       <c r="DF71" s="21"/>
     </row>
     <row r="72" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="31"/>
+      <c r="A72" s="35"/>
       <c r="B72" s="3" t="s">
         <v>185</v>
       </c>
@@ -11370,140 +11370,140 @@
       <c r="DF72" s="21"/>
     </row>
     <row r="73" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="31"/>
+      <c r="A73" s="35"/>
       <c r="B73" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="25" t="s">
+      <c r="C73" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="26"/>
-      <c r="E73" s="26"/>
-      <c r="F73" s="27"/>
-      <c r="G73" s="28" t="s">
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="25"/>
+      <c r="G73" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H73" s="29"/>
-      <c r="I73" s="29"/>
-      <c r="J73" s="28" t="s">
+      <c r="H73" s="28"/>
+      <c r="I73" s="28"/>
+      <c r="J73" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="K73" s="29"/>
-      <c r="L73" s="29"/>
-      <c r="M73" s="29"/>
-      <c r="N73" s="29"/>
-      <c r="O73" s="29"/>
-      <c r="P73" s="29"/>
-      <c r="Q73" s="29"/>
-      <c r="R73" s="29"/>
-      <c r="S73" s="29"/>
-      <c r="T73" s="29"/>
-      <c r="U73" s="29"/>
-      <c r="V73" s="29"/>
-      <c r="W73" s="29"/>
-      <c r="X73" s="29"/>
-      <c r="Y73" s="28" t="s">
+      <c r="K73" s="28"/>
+      <c r="L73" s="28"/>
+      <c r="M73" s="28"/>
+      <c r="N73" s="28"/>
+      <c r="O73" s="28"/>
+      <c r="P73" s="28"/>
+      <c r="Q73" s="28"/>
+      <c r="R73" s="28"/>
+      <c r="S73" s="28"/>
+      <c r="T73" s="28"/>
+      <c r="U73" s="28"/>
+      <c r="V73" s="28"/>
+      <c r="W73" s="28"/>
+      <c r="X73" s="28"/>
+      <c r="Y73" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="Z73" s="29"/>
-      <c r="AA73" s="29"/>
-      <c r="AB73" s="29"/>
-      <c r="AC73" s="29"/>
-      <c r="AD73" s="29"/>
-      <c r="AE73" s="29"/>
-      <c r="AF73" s="29"/>
-      <c r="AG73" s="29"/>
-      <c r="AH73" s="29"/>
-      <c r="AI73" s="29"/>
-      <c r="AJ73" s="29"/>
-      <c r="AK73" s="29"/>
-      <c r="AL73" s="29"/>
-      <c r="AM73" s="29"/>
-      <c r="AN73" s="29"/>
-      <c r="AO73" s="29"/>
-      <c r="AP73" s="29"/>
-      <c r="AQ73" s="45" t="s">
+      <c r="Z73" s="28"/>
+      <c r="AA73" s="28"/>
+      <c r="AB73" s="28"/>
+      <c r="AC73" s="28"/>
+      <c r="AD73" s="28"/>
+      <c r="AE73" s="28"/>
+      <c r="AF73" s="28"/>
+      <c r="AG73" s="28"/>
+      <c r="AH73" s="28"/>
+      <c r="AI73" s="28"/>
+      <c r="AJ73" s="28"/>
+      <c r="AK73" s="28"/>
+      <c r="AL73" s="28"/>
+      <c r="AM73" s="28"/>
+      <c r="AN73" s="28"/>
+      <c r="AO73" s="28"/>
+      <c r="AP73" s="28"/>
+      <c r="AQ73" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="AR73" s="46"/>
-      <c r="AS73" s="46"/>
-      <c r="AT73" s="46"/>
-      <c r="AU73" s="46"/>
-      <c r="AV73" s="46"/>
-      <c r="AW73" s="46"/>
-      <c r="AX73" s="46"/>
-      <c r="AY73" s="46"/>
-      <c r="AZ73" s="46"/>
-      <c r="BA73" s="47"/>
-      <c r="BB73" s="45" t="s">
+      <c r="AR73" s="30"/>
+      <c r="AS73" s="30"/>
+      <c r="AT73" s="30"/>
+      <c r="AU73" s="30"/>
+      <c r="AV73" s="30"/>
+      <c r="AW73" s="30"/>
+      <c r="AX73" s="30"/>
+      <c r="AY73" s="30"/>
+      <c r="AZ73" s="30"/>
+      <c r="BA73" s="31"/>
+      <c r="BB73" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="BC73" s="46"/>
-      <c r="BD73" s="46"/>
-      <c r="BE73" s="46"/>
-      <c r="BF73" s="46"/>
-      <c r="BG73" s="46"/>
-      <c r="BH73" s="46"/>
-      <c r="BI73" s="46"/>
-      <c r="BJ73" s="46"/>
-      <c r="BK73" s="46"/>
-      <c r="BL73" s="46"/>
-      <c r="BM73" s="46"/>
-      <c r="BN73" s="46"/>
-      <c r="BO73" s="46"/>
-      <c r="BP73" s="47"/>
-      <c r="BQ73" s="48" t="s">
+      <c r="BC73" s="30"/>
+      <c r="BD73" s="30"/>
+      <c r="BE73" s="30"/>
+      <c r="BF73" s="30"/>
+      <c r="BG73" s="30"/>
+      <c r="BH73" s="30"/>
+      <c r="BI73" s="30"/>
+      <c r="BJ73" s="30"/>
+      <c r="BK73" s="30"/>
+      <c r="BL73" s="30"/>
+      <c r="BM73" s="30"/>
+      <c r="BN73" s="30"/>
+      <c r="BO73" s="30"/>
+      <c r="BP73" s="31"/>
+      <c r="BQ73" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="BR73" s="49"/>
-      <c r="BS73" s="49"/>
-      <c r="BT73" s="49"/>
-      <c r="BU73" s="44" t="s">
+      <c r="BR73" s="33"/>
+      <c r="BS73" s="33"/>
+      <c r="BT73" s="33"/>
+      <c r="BU73" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BV73" s="26"/>
-      <c r="BW73" s="26"/>
-      <c r="BX73" s="26"/>
-      <c r="BY73" s="26"/>
-      <c r="BZ73" s="26"/>
-      <c r="CA73" s="26"/>
-      <c r="CB73" s="26"/>
-      <c r="CC73" s="26"/>
-      <c r="CD73" s="26"/>
-      <c r="CE73" s="26"/>
-      <c r="CF73" s="26"/>
-      <c r="CG73" s="26"/>
-      <c r="CH73" s="26"/>
-      <c r="CI73" s="26"/>
-      <c r="CJ73" s="26"/>
-      <c r="CK73" s="26"/>
-      <c r="CL73" s="27"/>
-      <c r="CM73" s="44" t="s">
+      <c r="BV73" s="24"/>
+      <c r="BW73" s="24"/>
+      <c r="BX73" s="24"/>
+      <c r="BY73" s="24"/>
+      <c r="BZ73" s="24"/>
+      <c r="CA73" s="24"/>
+      <c r="CB73" s="24"/>
+      <c r="CC73" s="24"/>
+      <c r="CD73" s="24"/>
+      <c r="CE73" s="24"/>
+      <c r="CF73" s="24"/>
+      <c r="CG73" s="24"/>
+      <c r="CH73" s="24"/>
+      <c r="CI73" s="24"/>
+      <c r="CJ73" s="24"/>
+      <c r="CK73" s="24"/>
+      <c r="CL73" s="25"/>
+      <c r="CM73" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="CN73" s="26"/>
-      <c r="CO73" s="26"/>
-      <c r="CP73" s="26"/>
-      <c r="CQ73" s="26"/>
-      <c r="CR73" s="26"/>
-      <c r="CS73" s="26"/>
-      <c r="CT73" s="26"/>
-      <c r="CU73" s="26"/>
-      <c r="CV73" s="27"/>
-      <c r="CW73" s="44" t="s">
+      <c r="CN73" s="24"/>
+      <c r="CO73" s="24"/>
+      <c r="CP73" s="24"/>
+      <c r="CQ73" s="24"/>
+      <c r="CR73" s="24"/>
+      <c r="CS73" s="24"/>
+      <c r="CT73" s="24"/>
+      <c r="CU73" s="24"/>
+      <c r="CV73" s="25"/>
+      <c r="CW73" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="CX73" s="26"/>
-      <c r="CY73" s="26"/>
-      <c r="CZ73" s="26"/>
-      <c r="DA73" s="26"/>
-      <c r="DB73" s="26"/>
-      <c r="DC73" s="26"/>
-      <c r="DD73" s="26"/>
-      <c r="DE73" s="26"/>
-      <c r="DF73" s="27"/>
+      <c r="CX73" s="24"/>
+      <c r="CY73" s="24"/>
+      <c r="CZ73" s="24"/>
+      <c r="DA73" s="24"/>
+      <c r="DB73" s="24"/>
+      <c r="DC73" s="24"/>
+      <c r="DD73" s="24"/>
+      <c r="DE73" s="24"/>
+      <c r="DF73" s="25"/>
     </row>
-    <row r="74" spans="1:110" ht="120" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:110" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="22"/>
       <c r="B74" s="12" t="s">
         <v>2</v>
@@ -12166,7 +12166,7 @@
       </c>
     </row>
     <row r="76" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="40" t="s">
+      <c r="A76" s="51" t="s">
         <v>87</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -12286,7 +12286,7 @@
       <c r="DF76" s="21"/>
     </row>
     <row r="77" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="41"/>
+      <c r="A77" s="52"/>
       <c r="B77" s="3" t="s">
         <v>187</v>
       </c>
@@ -12400,7 +12400,7 @@
       <c r="DF77" s="21"/>
     </row>
     <row r="78" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="32" t="s">
+      <c r="A78" s="37" t="s">
         <v>88</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -12516,7 +12516,7 @@
       <c r="DF78" s="20"/>
     </row>
     <row r="79" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="33"/>
+      <c r="A79" s="38"/>
       <c r="B79" s="2" t="s">
         <v>188</v>
       </c>
@@ -12630,7 +12630,7 @@
       <c r="DF79" s="20"/>
     </row>
     <row r="80" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="38" t="s">
+      <c r="A80" s="41" t="s">
         <v>89</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -12749,7 +12749,9 @@
       <c r="CS80" s="21"/>
       <c r="CT80" s="21"/>
       <c r="CU80" s="21"/>
-      <c r="CV80" s="21"/>
+      <c r="CV80" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="CW80" s="21"/>
       <c r="CX80" s="21"/>
       <c r="CY80" s="21"/>
@@ -12762,7 +12764,7 @@
       <c r="DF80" s="21"/>
     </row>
     <row r="81" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="39"/>
+      <c r="A81" s="42"/>
       <c r="B81" s="3" t="s">
         <v>190</v>
       </c>
@@ -12873,7 +12875,9 @@
       <c r="CS81" s="21"/>
       <c r="CT81" s="21"/>
       <c r="CU81" s="21"/>
-      <c r="CV81" s="21"/>
+      <c r="CV81" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="CW81" s="21"/>
       <c r="CX81" s="21"/>
       <c r="CY81" s="21"/>
@@ -12886,7 +12890,7 @@
       <c r="DF81" s="21"/>
     </row>
     <row r="82" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="39"/>
+      <c r="A82" s="42"/>
       <c r="B82" s="3" t="s">
         <v>191</v>
       </c>
@@ -13004,7 +13008,7 @@
       <c r="DF82" s="21"/>
     </row>
     <row r="83" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="39"/>
+      <c r="A83" s="42"/>
       <c r="B83" s="3" t="s">
         <v>192</v>
       </c>
@@ -13124,7 +13128,7 @@
       <c r="DF83" s="21"/>
     </row>
     <row r="84" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="39"/>
+      <c r="A84" s="42"/>
       <c r="B84" s="3" t="s">
         <v>139</v>
       </c>
@@ -13238,7 +13242,7 @@
       <c r="DF84" s="21"/>
     </row>
     <row r="85" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="39"/>
+      <c r="A85" s="42"/>
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -13472,7 +13476,7 @@
       <c r="DF86" s="21"/>
     </row>
     <row r="87" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="32" t="s">
+      <c r="A87" s="37" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -13585,7 +13589,9 @@
       <c r="CS87" s="20"/>
       <c r="CT87" s="20"/>
       <c r="CU87" s="20"/>
-      <c r="CV87" s="20"/>
+      <c r="CV87" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CW87" s="20"/>
       <c r="CX87" s="20"/>
       <c r="CY87" s="20"/>
@@ -13598,7 +13604,7 @@
       <c r="DF87" s="20"/>
     </row>
     <row r="88" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="33"/>
+      <c r="A88" s="38"/>
       <c r="B88" s="2" t="s">
         <v>189</v>
       </c>
@@ -13712,7 +13718,7 @@
       <c r="DF88" s="20"/>
     </row>
     <row r="89" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="33"/>
+      <c r="A89" s="38"/>
       <c r="B89" s="2" t="s">
         <v>141</v>
       </c>
@@ -13826,7 +13832,7 @@
       <c r="DF89" s="20"/>
     </row>
     <row r="90" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="33"/>
+      <c r="A90" s="38"/>
       <c r="B90" s="2" t="s">
         <v>142</v>
       </c>
@@ -13937,7 +13943,9 @@
       <c r="CS90" s="20"/>
       <c r="CT90" s="20"/>
       <c r="CU90" s="20"/>
-      <c r="CV90" s="20"/>
+      <c r="CV90" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CW90" s="20"/>
       <c r="CX90" s="20"/>
       <c r="CY90" s="20"/>
@@ -13950,7 +13958,7 @@
       <c r="DF90" s="20"/>
     </row>
     <row r="91" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="30" t="s">
+      <c r="A91" s="34" t="s">
         <v>91</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -14068,7 +14076,7 @@
       <c r="DF91" s="21"/>
     </row>
     <row r="92" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="31"/>
+      <c r="A92" s="35"/>
       <c r="B92" s="3" t="s">
         <v>196</v>
       </c>
@@ -14184,7 +14192,7 @@
       <c r="DF92" s="21"/>
     </row>
     <row r="93" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="31"/>
+      <c r="A93" s="35"/>
       <c r="B93" s="3" t="s">
         <v>197</v>
       </c>
@@ -14300,7 +14308,7 @@
       <c r="DF93" s="21"/>
     </row>
     <row r="94" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="31"/>
+      <c r="A94" s="35"/>
       <c r="B94" s="3" t="s">
         <v>198</v>
       </c>
@@ -14414,7 +14422,7 @@
       <c r="DF94" s="21"/>
     </row>
     <row r="95" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="31"/>
+      <c r="A95" s="35"/>
       <c r="B95" s="3" t="s">
         <v>199</v>
       </c>
@@ -14530,7 +14538,7 @@
       <c r="DF95" s="21"/>
     </row>
     <row r="96" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="34"/>
+      <c r="A96" s="40"/>
       <c r="B96" s="3" t="s">
         <v>189</v>
       </c>
@@ -14644,7 +14652,7 @@
       <c r="DF96" s="21"/>
     </row>
     <row r="97" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="32" t="s">
+      <c r="A97" s="37" t="s">
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -14766,7 +14774,7 @@
       <c r="DF97" s="20"/>
     </row>
     <row r="98" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="33"/>
+      <c r="A98" s="38"/>
       <c r="B98" s="2" t="s">
         <v>200</v>
       </c>
@@ -14886,7 +14894,7 @@
       <c r="DF98" s="20"/>
     </row>
     <row r="99" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="30" t="s">
+      <c r="A99" s="34" t="s">
         <v>93</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -15022,7 +15030,7 @@
       <c r="DF99" s="21"/>
     </row>
     <row r="100" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="34"/>
+      <c r="A100" s="40"/>
       <c r="B100" s="3" t="s">
         <v>201</v>
       </c>
@@ -15156,7 +15164,7 @@
       <c r="DF100" s="21"/>
     </row>
     <row r="101" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="32" t="s">
+      <c r="A101" s="37" t="s">
         <v>94</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -15274,7 +15282,7 @@
       <c r="DF101" s="20"/>
     </row>
     <row r="102" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="33"/>
+      <c r="A102" s="38"/>
       <c r="B102" s="2" t="s">
         <v>202</v>
       </c>
@@ -15390,7 +15398,7 @@
       <c r="DF102" s="20"/>
     </row>
     <row r="103" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="33"/>
+      <c r="A103" s="38"/>
       <c r="B103" s="2" t="s">
         <v>203</v>
       </c>
@@ -15506,7 +15514,7 @@
       <c r="DF103" s="20"/>
     </row>
     <row r="104" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="30" t="s">
+      <c r="A104" s="34" t="s">
         <v>95</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -15632,7 +15640,7 @@
       <c r="DF104" s="21"/>
     </row>
     <row r="105" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="31"/>
+      <c r="A105" s="35"/>
       <c r="B105" s="3" t="s">
         <v>205</v>
       </c>
@@ -15756,7 +15764,7 @@
       <c r="DF105" s="21"/>
     </row>
     <row r="106" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="31"/>
+      <c r="A106" s="35"/>
       <c r="B106" s="3" t="s">
         <v>206</v>
       </c>
@@ -15874,7 +15882,7 @@
       <c r="DF106" s="21"/>
     </row>
     <row r="107" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="31"/>
+      <c r="A107" s="35"/>
       <c r="B107" s="3" t="s">
         <v>431</v>
       </c>
@@ -15988,7 +15996,7 @@
       <c r="DF107" s="21"/>
     </row>
     <row r="108" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="34"/>
+      <c r="A108" s="40"/>
       <c r="B108" s="3" t="s">
         <v>77</v>
       </c>
@@ -16102,7 +16110,7 @@
       <c r="DF108" s="21"/>
     </row>
     <row r="109" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="32" t="s">
+      <c r="A109" s="37" t="s">
         <v>96</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -16167,10 +16175,18 @@
       <c r="AY109" s="20"/>
       <c r="AZ109" s="20"/>
       <c r="BA109" s="20"/>
-      <c r="BB109" s="20"/>
-      <c r="BC109" s="20"/>
-      <c r="BD109" s="20"/>
-      <c r="BE109" s="20"/>
+      <c r="BB109" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BC109" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BD109" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BE109" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="BF109" s="20"/>
       <c r="BG109" s="20"/>
       <c r="BH109" s="20"/>
@@ -16207,12 +16223,20 @@
       <c r="CM109" s="20"/>
       <c r="CN109" s="20"/>
       <c r="CO109" s="20"/>
-      <c r="CP109" s="20"/>
-      <c r="CQ109" s="20"/>
+      <c r="CP109" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="CQ109" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CR109" s="20"/>
       <c r="CS109" s="20"/>
-      <c r="CT109" s="20"/>
-      <c r="CU109" s="20"/>
+      <c r="CT109" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="CU109" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CV109" s="20"/>
       <c r="CW109" s="20"/>
       <c r="CX109" s="20"/>
@@ -16226,7 +16250,7 @@
       <c r="DF109" s="20"/>
     </row>
     <row r="110" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="33"/>
+      <c r="A110" s="38"/>
       <c r="B110" s="2" t="s">
         <v>207</v>
       </c>
@@ -16297,9 +16321,15 @@
       <c r="AY110" s="20"/>
       <c r="AZ110" s="20"/>
       <c r="BA110" s="20"/>
-      <c r="BB110" s="20"/>
-      <c r="BC110" s="20"/>
-      <c r="BD110" s="20"/>
+      <c r="BB110" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BC110" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BD110" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BE110" s="20"/>
       <c r="BF110" s="20"/>
       <c r="BG110" s="20"/>
@@ -16337,11 +16367,17 @@
       <c r="CM110" s="20"/>
       <c r="CN110" s="20"/>
       <c r="CO110" s="20"/>
-      <c r="CP110" s="20"/>
-      <c r="CQ110" s="20"/>
+      <c r="CP110" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="CQ110" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CR110" s="20"/>
       <c r="CS110" s="20"/>
-      <c r="CT110" s="20"/>
+      <c r="CT110" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CU110" s="20"/>
       <c r="CV110" s="20"/>
       <c r="CW110" s="20"/>
@@ -16356,7 +16392,7 @@
       <c r="DF110" s="20"/>
     </row>
     <row r="111" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="33"/>
+      <c r="A111" s="38"/>
       <c r="B111" s="2" t="s">
         <v>208</v>
       </c>
@@ -16414,8 +16450,12 @@
       <c r="AZ111" s="20"/>
       <c r="BA111" s="20"/>
       <c r="BB111" s="20"/>
-      <c r="BC111" s="20"/>
-      <c r="BD111" s="20"/>
+      <c r="BC111" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BD111" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BE111" s="20"/>
       <c r="BF111" s="20"/>
       <c r="BG111" s="20"/>
@@ -16453,7 +16493,9 @@
       <c r="CM111" s="20"/>
       <c r="CN111" s="20"/>
       <c r="CO111" s="20"/>
-      <c r="CP111" s="20"/>
+      <c r="CP111" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CQ111" s="20"/>
       <c r="CR111" s="20"/>
       <c r="CS111" s="20"/>
@@ -16472,7 +16514,7 @@
       <c r="DF111" s="20"/>
     </row>
     <row r="112" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="33"/>
+      <c r="A112" s="38"/>
       <c r="B112" s="2" t="s">
         <v>209</v>
       </c>
@@ -16540,8 +16582,12 @@
       <c r="AZ112" s="20"/>
       <c r="BA112" s="20"/>
       <c r="BB112" s="20"/>
-      <c r="BC112" s="20"/>
-      <c r="BD112" s="20"/>
+      <c r="BC112" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BD112" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BE112" s="20"/>
       <c r="BF112" s="20"/>
       <c r="BG112" s="20"/>
@@ -16598,7 +16644,7 @@
       <c r="DF112" s="20"/>
     </row>
     <row r="113" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="33"/>
+      <c r="A113" s="38"/>
       <c r="B113" s="2" t="s">
         <v>210</v>
       </c>
@@ -16660,8 +16706,12 @@
       <c r="AZ113" s="20"/>
       <c r="BA113" s="20"/>
       <c r="BB113" s="20"/>
-      <c r="BC113" s="20"/>
-      <c r="BD113" s="20"/>
+      <c r="BC113" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BD113" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BE113" s="20"/>
       <c r="BF113" s="20"/>
       <c r="BG113" s="20"/>
@@ -16704,7 +16754,9 @@
       <c r="CR113" s="20"/>
       <c r="CS113" s="20"/>
       <c r="CT113" s="20"/>
-      <c r="CU113" s="20"/>
+      <c r="CU113" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="CV113" s="20"/>
       <c r="CW113" s="20"/>
       <c r="CX113" s="20"/>
@@ -16718,7 +16770,7 @@
       <c r="DF113" s="20"/>
     </row>
     <row r="114" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="33"/>
+      <c r="A114" s="38"/>
       <c r="B114" s="2" t="s">
         <v>211</v>
       </c>
@@ -16774,8 +16826,12 @@
       <c r="AZ114" s="20"/>
       <c r="BA114" s="20"/>
       <c r="BB114" s="20"/>
-      <c r="BC114" s="20"/>
-      <c r="BD114" s="20"/>
+      <c r="BC114" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BD114" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BE114" s="20"/>
       <c r="BF114" s="20"/>
       <c r="BG114" s="20"/>
@@ -16832,7 +16888,7 @@
       <c r="DF114" s="20"/>
     </row>
     <row r="115" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="30" t="s">
+      <c r="A115" s="34" t="s">
         <v>97</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -16948,7 +17004,7 @@
       <c r="DF115" s="21"/>
     </row>
     <row r="116" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="31"/>
+      <c r="A116" s="35"/>
       <c r="B116" s="3" t="s">
         <v>213</v>
       </c>
@@ -17062,7 +17118,7 @@
       <c r="DF116" s="21"/>
     </row>
     <row r="117" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="32" t="s">
+      <c r="A117" s="37" t="s">
         <v>98</v>
       </c>
       <c r="B117" s="2" t="s">
@@ -17180,7 +17236,7 @@
       <c r="DF117" s="20"/>
     </row>
     <row r="118" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="33"/>
+      <c r="A118" s="38"/>
       <c r="B118" s="2" t="s">
         <v>204</v>
       </c>
@@ -17294,7 +17350,7 @@
       <c r="DF118" s="20"/>
     </row>
     <row r="119" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="33"/>
+      <c r="A119" s="38"/>
       <c r="B119" s="2" t="s">
         <v>141</v>
       </c>
@@ -17408,7 +17464,7 @@
       <c r="DF119" s="20"/>
     </row>
     <row r="120" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="33"/>
+      <c r="A120" s="38"/>
       <c r="B120" s="2" t="s">
         <v>214</v>
       </c>
@@ -17524,7 +17580,7 @@
       <c r="DF120" s="20"/>
     </row>
     <row r="121" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="38" t="s">
+      <c r="A121" s="41" t="s">
         <v>99</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -17642,7 +17698,7 @@
       <c r="DF121" s="21"/>
     </row>
     <row r="122" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="39"/>
+      <c r="A122" s="42"/>
       <c r="B122" s="3" t="s">
         <v>147</v>
       </c>
@@ -17756,7 +17812,7 @@
       <c r="DF122" s="21"/>
     </row>
     <row r="123" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="39"/>
+      <c r="A123" s="42"/>
       <c r="B123" s="3" t="s">
         <v>216</v>
       </c>
@@ -17986,7 +18042,7 @@
       <c r="DF124" s="21"/>
     </row>
     <row r="125" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="35" t="s">
+      <c r="A125" s="48" t="s">
         <v>100</v>
       </c>
       <c r="B125" s="2" t="s">
@@ -18051,9 +18107,15 @@
       <c r="BG125" s="20"/>
       <c r="BH125" s="20"/>
       <c r="BI125" s="20"/>
-      <c r="BJ125" s="20"/>
-      <c r="BK125" s="20"/>
-      <c r="BL125" s="20"/>
+      <c r="BJ125" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BK125" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BL125" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="BM125" s="20"/>
       <c r="BN125" s="20"/>
       <c r="BO125" s="20"/>
@@ -18102,7 +18164,7 @@
       <c r="DF125" s="20"/>
     </row>
     <row r="126" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="36"/>
+      <c r="A126" s="49"/>
       <c r="B126" s="2" t="s">
         <v>217</v>
       </c>
@@ -18167,8 +18229,12 @@
       <c r="BG126" s="20"/>
       <c r="BH126" s="20"/>
       <c r="BI126" s="20"/>
-      <c r="BJ126" s="20"/>
-      <c r="BK126" s="20"/>
+      <c r="BJ126" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="BK126" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BL126" s="20"/>
       <c r="BM126" s="20"/>
       <c r="BN126" s="20"/>
@@ -18218,7 +18284,7 @@
       <c r="DF126" s="20"/>
     </row>
     <row r="127" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="37"/>
+      <c r="A127" s="50"/>
       <c r="B127" s="2" t="s">
         <v>212</v>
       </c>
@@ -18281,8 +18347,12 @@
       <c r="BG127" s="20"/>
       <c r="BH127" s="20"/>
       <c r="BI127" s="20"/>
-      <c r="BJ127" s="20"/>
-      <c r="BK127" s="20"/>
+      <c r="BJ127" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BK127" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BL127" s="20"/>
       <c r="BM127" s="20"/>
       <c r="BN127" s="20"/>
@@ -18332,7 +18402,7 @@
       <c r="DF127" s="20"/>
     </row>
     <row r="128" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="38" t="s">
+      <c r="A128" s="41" t="s">
         <v>102</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -18450,7 +18520,7 @@
       <c r="DF128" s="21"/>
     </row>
     <row r="129" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="39"/>
+      <c r="A129" s="42"/>
       <c r="B129" s="3" t="s">
         <v>142</v>
       </c>
@@ -18566,7 +18636,7 @@
       <c r="DF129" s="21"/>
     </row>
     <row r="130" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="39"/>
+      <c r="A130" s="42"/>
       <c r="B130" s="3" t="s">
         <v>141</v>
       </c>
@@ -18798,7 +18868,7 @@
       <c r="DF131" s="21"/>
     </row>
     <row r="132" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="32" t="s">
+      <c r="A132" s="37" t="s">
         <v>101</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -18918,7 +18988,7 @@
       <c r="DF132" s="20"/>
     </row>
     <row r="133" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="33"/>
+      <c r="A133" s="38"/>
       <c r="B133" s="2" t="s">
         <v>221</v>
       </c>
@@ -19036,7 +19106,7 @@
       <c r="DF133" s="20"/>
     </row>
     <row r="134" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="30" t="s">
+      <c r="A134" s="34" t="s">
         <v>103</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -19104,10 +19174,18 @@
       <c r="BJ134" s="21"/>
       <c r="BK134" s="21"/>
       <c r="BL134" s="21"/>
-      <c r="BM134" s="21"/>
-      <c r="BN134" s="21"/>
-      <c r="BO134" s="21"/>
-      <c r="BP134" s="21"/>
+      <c r="BM134" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="BN134" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="BO134" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="BP134" s="21" t="s">
+        <v>432</v>
+      </c>
       <c r="BQ134" s="21"/>
       <c r="BR134" s="21"/>
       <c r="BS134" s="21"/>
@@ -19135,10 +19213,16 @@
       <c r="CO134" s="21"/>
       <c r="CP134" s="21"/>
       <c r="CQ134" s="21"/>
-      <c r="CR134" s="21"/>
+      <c r="CR134" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CS134" s="21"/>
-      <c r="CT134" s="21"/>
-      <c r="CU134" s="21"/>
+      <c r="CT134" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="CU134" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CV134" s="21"/>
       <c r="CW134" s="21"/>
       <c r="CX134" s="21"/>
@@ -19152,7 +19236,7 @@
       <c r="DF134" s="21"/>
     </row>
     <row r="135" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="31"/>
+      <c r="A135" s="35"/>
       <c r="B135" s="3" t="s">
         <v>223</v>
       </c>
@@ -19218,9 +19302,15 @@
       <c r="BJ135" s="21"/>
       <c r="BK135" s="21"/>
       <c r="BL135" s="21"/>
-      <c r="BM135" s="21"/>
-      <c r="BN135" s="21"/>
-      <c r="BO135" s="21"/>
+      <c r="BM135" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="BN135" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="BO135" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="BP135" s="21"/>
       <c r="BQ135" s="21"/>
       <c r="BR135" s="21"/>
@@ -19266,7 +19356,7 @@
       <c r="DF135" s="21"/>
     </row>
     <row r="136" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="31"/>
+      <c r="A136" s="35"/>
       <c r="B136" s="3" t="s">
         <v>210</v>
       </c>
@@ -19333,8 +19423,12 @@
       <c r="BK136" s="21"/>
       <c r="BL136" s="21"/>
       <c r="BM136" s="21"/>
-      <c r="BN136" s="21"/>
-      <c r="BO136" s="21"/>
+      <c r="BN136" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="BO136" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="BP136" s="21"/>
       <c r="BQ136" s="21"/>
       <c r="BR136" s="21"/>
@@ -19364,9 +19458,15 @@
       <c r="CP136" s="21"/>
       <c r="CQ136" s="21"/>
       <c r="CR136" s="21"/>
-      <c r="CS136" s="21"/>
-      <c r="CT136" s="21"/>
-      <c r="CU136" s="21"/>
+      <c r="CS136" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="CT136" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="CU136" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="CV136" s="21"/>
       <c r="CW136" s="21"/>
       <c r="CX136" s="21"/>
@@ -19380,7 +19480,7 @@
       <c r="DF136" s="21"/>
     </row>
     <row r="137" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="31"/>
+      <c r="A137" s="35"/>
       <c r="B137" s="3" t="s">
         <v>224</v>
       </c>
@@ -19447,8 +19547,12 @@
       <c r="BK137" s="21"/>
       <c r="BL137" s="21"/>
       <c r="BM137" s="21"/>
-      <c r="BN137" s="21"/>
-      <c r="BO137" s="21"/>
+      <c r="BN137" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="BO137" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="BP137" s="21"/>
       <c r="BQ137" s="21"/>
       <c r="BR137" s="21"/>
@@ -19494,7 +19598,7 @@
       <c r="DF137" s="21"/>
     </row>
     <row r="138" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="31"/>
+      <c r="A138" s="35"/>
       <c r="B138" s="3" t="s">
         <v>225</v>
       </c>
@@ -19561,8 +19665,12 @@
       <c r="BK138" s="21"/>
       <c r="BL138" s="21"/>
       <c r="BM138" s="21"/>
-      <c r="BN138" s="21"/>
-      <c r="BO138" s="21"/>
+      <c r="BN138" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="BO138" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="BP138" s="21"/>
       <c r="BQ138" s="21"/>
       <c r="BR138" s="21"/>
@@ -19608,7 +19716,7 @@
       <c r="DF138" s="21"/>
     </row>
     <row r="139" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="32" t="s">
+      <c r="A139" s="37" t="s">
         <v>104</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -19724,7 +19832,7 @@
       <c r="DF139" s="20"/>
     </row>
     <row r="140" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="33"/>
+      <c r="A140" s="38"/>
       <c r="B140" s="2" t="s">
         <v>227</v>
       </c>
@@ -19838,7 +19946,7 @@
       <c r="DF140" s="20"/>
     </row>
     <row r="141" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="33"/>
+      <c r="A141" s="38"/>
       <c r="B141" s="2" t="s">
         <v>228</v>
       </c>
@@ -19952,7 +20060,7 @@
       <c r="DF141" s="20"/>
     </row>
     <row r="142" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="33"/>
+      <c r="A142" s="38"/>
       <c r="B142" s="2" t="s">
         <v>229</v>
       </c>
@@ -20066,141 +20174,141 @@
       <c r="DF142" s="20"/>
     </row>
     <row r="143" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="23"/>
+      <c r="A143" s="44"/>
       <c r="B143" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="25" t="s">
+      <c r="C143" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D143" s="26"/>
-      <c r="E143" s="26"/>
-      <c r="F143" s="27"/>
-      <c r="G143" s="28" t="s">
+      <c r="D143" s="24"/>
+      <c r="E143" s="24"/>
+      <c r="F143" s="25"/>
+      <c r="G143" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H143" s="29"/>
-      <c r="I143" s="29"/>
-      <c r="J143" s="28" t="s">
+      <c r="H143" s="28"/>
+      <c r="I143" s="28"/>
+      <c r="J143" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="K143" s="29"/>
-      <c r="L143" s="29"/>
-      <c r="M143" s="29"/>
-      <c r="N143" s="29"/>
-      <c r="O143" s="29"/>
-      <c r="P143" s="29"/>
-      <c r="Q143" s="29"/>
-      <c r="R143" s="29"/>
-      <c r="S143" s="29"/>
-      <c r="T143" s="29"/>
-      <c r="U143" s="29"/>
-      <c r="V143" s="29"/>
-      <c r="W143" s="29"/>
-      <c r="X143" s="29"/>
-      <c r="Y143" s="28" t="s">
+      <c r="K143" s="28"/>
+      <c r="L143" s="28"/>
+      <c r="M143" s="28"/>
+      <c r="N143" s="28"/>
+      <c r="O143" s="28"/>
+      <c r="P143" s="28"/>
+      <c r="Q143" s="28"/>
+      <c r="R143" s="28"/>
+      <c r="S143" s="28"/>
+      <c r="T143" s="28"/>
+      <c r="U143" s="28"/>
+      <c r="V143" s="28"/>
+      <c r="W143" s="28"/>
+      <c r="X143" s="28"/>
+      <c r="Y143" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="Z143" s="29"/>
-      <c r="AA143" s="29"/>
-      <c r="AB143" s="29"/>
-      <c r="AC143" s="29"/>
-      <c r="AD143" s="29"/>
-      <c r="AE143" s="29"/>
-      <c r="AF143" s="29"/>
-      <c r="AG143" s="29"/>
-      <c r="AH143" s="29"/>
-      <c r="AI143" s="29"/>
-      <c r="AJ143" s="29"/>
-      <c r="AK143" s="29"/>
-      <c r="AL143" s="29"/>
-      <c r="AM143" s="29"/>
-      <c r="AN143" s="29"/>
-      <c r="AO143" s="29"/>
-      <c r="AP143" s="29"/>
-      <c r="AQ143" s="45" t="s">
+      <c r="Z143" s="28"/>
+      <c r="AA143" s="28"/>
+      <c r="AB143" s="28"/>
+      <c r="AC143" s="28"/>
+      <c r="AD143" s="28"/>
+      <c r="AE143" s="28"/>
+      <c r="AF143" s="28"/>
+      <c r="AG143" s="28"/>
+      <c r="AH143" s="28"/>
+      <c r="AI143" s="28"/>
+      <c r="AJ143" s="28"/>
+      <c r="AK143" s="28"/>
+      <c r="AL143" s="28"/>
+      <c r="AM143" s="28"/>
+      <c r="AN143" s="28"/>
+      <c r="AO143" s="28"/>
+      <c r="AP143" s="28"/>
+      <c r="AQ143" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="AR143" s="46"/>
-      <c r="AS143" s="46"/>
-      <c r="AT143" s="46"/>
-      <c r="AU143" s="46"/>
-      <c r="AV143" s="46"/>
-      <c r="AW143" s="46"/>
-      <c r="AX143" s="46"/>
-      <c r="AY143" s="46"/>
-      <c r="AZ143" s="46"/>
-      <c r="BA143" s="47"/>
-      <c r="BB143" s="45" t="s">
+      <c r="AR143" s="30"/>
+      <c r="AS143" s="30"/>
+      <c r="AT143" s="30"/>
+      <c r="AU143" s="30"/>
+      <c r="AV143" s="30"/>
+      <c r="AW143" s="30"/>
+      <c r="AX143" s="30"/>
+      <c r="AY143" s="30"/>
+      <c r="AZ143" s="30"/>
+      <c r="BA143" s="31"/>
+      <c r="BB143" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="BC143" s="46"/>
-      <c r="BD143" s="46"/>
-      <c r="BE143" s="46"/>
-      <c r="BF143" s="46"/>
-      <c r="BG143" s="46"/>
-      <c r="BH143" s="46"/>
-      <c r="BI143" s="46"/>
-      <c r="BJ143" s="46"/>
-      <c r="BK143" s="46"/>
-      <c r="BL143" s="46"/>
-      <c r="BM143" s="46"/>
-      <c r="BN143" s="46"/>
-      <c r="BO143" s="46"/>
-      <c r="BP143" s="47"/>
-      <c r="BQ143" s="48" t="s">
+      <c r="BC143" s="30"/>
+      <c r="BD143" s="30"/>
+      <c r="BE143" s="30"/>
+      <c r="BF143" s="30"/>
+      <c r="BG143" s="30"/>
+      <c r="BH143" s="30"/>
+      <c r="BI143" s="30"/>
+      <c r="BJ143" s="30"/>
+      <c r="BK143" s="30"/>
+      <c r="BL143" s="30"/>
+      <c r="BM143" s="30"/>
+      <c r="BN143" s="30"/>
+      <c r="BO143" s="30"/>
+      <c r="BP143" s="31"/>
+      <c r="BQ143" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="BR143" s="49"/>
-      <c r="BS143" s="49"/>
-      <c r="BT143" s="49"/>
-      <c r="BU143" s="44" t="s">
+      <c r="BR143" s="33"/>
+      <c r="BS143" s="33"/>
+      <c r="BT143" s="33"/>
+      <c r="BU143" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BV143" s="26"/>
-      <c r="BW143" s="26"/>
-      <c r="BX143" s="26"/>
-      <c r="BY143" s="26"/>
-      <c r="BZ143" s="26"/>
-      <c r="CA143" s="26"/>
-      <c r="CB143" s="26"/>
-      <c r="CC143" s="26"/>
-      <c r="CD143" s="26"/>
-      <c r="CE143" s="26"/>
-      <c r="CF143" s="26"/>
-      <c r="CG143" s="26"/>
-      <c r="CH143" s="26"/>
-      <c r="CI143" s="26"/>
-      <c r="CJ143" s="26"/>
-      <c r="CK143" s="26"/>
-      <c r="CL143" s="27"/>
-      <c r="CM143" s="44" t="s">
+      <c r="BV143" s="24"/>
+      <c r="BW143" s="24"/>
+      <c r="BX143" s="24"/>
+      <c r="BY143" s="24"/>
+      <c r="BZ143" s="24"/>
+      <c r="CA143" s="24"/>
+      <c r="CB143" s="24"/>
+      <c r="CC143" s="24"/>
+      <c r="CD143" s="24"/>
+      <c r="CE143" s="24"/>
+      <c r="CF143" s="24"/>
+      <c r="CG143" s="24"/>
+      <c r="CH143" s="24"/>
+      <c r="CI143" s="24"/>
+      <c r="CJ143" s="24"/>
+      <c r="CK143" s="24"/>
+      <c r="CL143" s="25"/>
+      <c r="CM143" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="CN143" s="26"/>
-      <c r="CO143" s="26"/>
-      <c r="CP143" s="26"/>
-      <c r="CQ143" s="26"/>
-      <c r="CR143" s="26"/>
-      <c r="CS143" s="26"/>
-      <c r="CT143" s="26"/>
-      <c r="CU143" s="26"/>
-      <c r="CV143" s="27"/>
-      <c r="CW143" s="44" t="s">
+      <c r="CN143" s="24"/>
+      <c r="CO143" s="24"/>
+      <c r="CP143" s="24"/>
+      <c r="CQ143" s="24"/>
+      <c r="CR143" s="24"/>
+      <c r="CS143" s="24"/>
+      <c r="CT143" s="24"/>
+      <c r="CU143" s="24"/>
+      <c r="CV143" s="25"/>
+      <c r="CW143" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="CX143" s="26"/>
-      <c r="CY143" s="26"/>
-      <c r="CZ143" s="26"/>
-      <c r="DA143" s="26"/>
-      <c r="DB143" s="26"/>
-      <c r="DC143" s="26"/>
-      <c r="DD143" s="26"/>
-      <c r="DE143" s="26"/>
-      <c r="DF143" s="27"/>
+      <c r="CX143" s="24"/>
+      <c r="CY143" s="24"/>
+      <c r="CZ143" s="24"/>
+      <c r="DA143" s="24"/>
+      <c r="DB143" s="24"/>
+      <c r="DC143" s="24"/>
+      <c r="DD143" s="24"/>
+      <c r="DE143" s="24"/>
+      <c r="DF143" s="25"/>
     </row>
-    <row r="144" spans="1:110" ht="120" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A144" s="24"/>
+    <row r="144" spans="1:110" ht="56.25" x14ac:dyDescent="0.15">
+      <c r="A144" s="45"/>
       <c r="B144" s="12" t="s">
         <v>2</v>
       </c>
@@ -20862,7 +20970,7 @@
       </c>
     </row>
     <row r="146" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="30" t="s">
+      <c r="A146" s="34" t="s">
         <v>105</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -20978,7 +21086,7 @@
       <c r="DF146" s="21"/>
     </row>
     <row r="147" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="31"/>
+      <c r="A147" s="35"/>
       <c r="B147" s="3" t="s">
         <v>127</v>
       </c>
@@ -21092,7 +21200,7 @@
       <c r="DF147" s="21"/>
     </row>
     <row r="148" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="32" t="s">
+      <c r="A148" s="37" t="s">
         <v>106</v>
       </c>
       <c r="B148" s="2" t="s">
@@ -21208,7 +21316,7 @@
       <c r="DF148" s="20"/>
     </row>
     <row r="149" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="33"/>
+      <c r="A149" s="38"/>
       <c r="B149" s="2" t="s">
         <v>142</v>
       </c>
@@ -21322,7 +21430,7 @@
       <c r="DF149" s="20"/>
     </row>
     <row r="150" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="33"/>
+      <c r="A150" s="38"/>
       <c r="B150" s="2" t="s">
         <v>226</v>
       </c>
@@ -21436,7 +21544,7 @@
       <c r="DF150" s="20"/>
     </row>
     <row r="151" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="33"/>
+      <c r="A151" s="38"/>
       <c r="B151" s="2" t="s">
         <v>232</v>
       </c>
@@ -21550,7 +21658,7 @@
       <c r="DF151" s="20"/>
     </row>
     <row r="152" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="33"/>
+      <c r="A152" s="38"/>
       <c r="B152" s="2" t="s">
         <v>230</v>
       </c>
@@ -21664,7 +21772,7 @@
       <c r="DF152" s="20"/>
     </row>
     <row r="153" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="30" t="s">
+      <c r="A153" s="34" t="s">
         <v>107</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -21784,7 +21892,7 @@
       <c r="DF153" s="21"/>
     </row>
     <row r="154" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="31"/>
+      <c r="A154" s="35"/>
       <c r="B154" s="3" t="s">
         <v>77</v>
       </c>
@@ -21902,7 +22010,7 @@
       <c r="DF154" s="21"/>
     </row>
     <row r="155" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="31"/>
+      <c r="A155" s="35"/>
       <c r="B155" s="3" t="s">
         <v>220</v>
       </c>
@@ -22020,7 +22128,7 @@
       <c r="DF155" s="21"/>
     </row>
     <row r="156" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="32" t="s">
+      <c r="A156" s="37" t="s">
         <v>108</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -22140,7 +22248,7 @@
       <c r="DF156" s="20"/>
     </row>
     <row r="157" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="33"/>
+      <c r="A157" s="38"/>
       <c r="B157" s="2" t="s">
         <v>139</v>
       </c>
@@ -22258,7 +22366,7 @@
       <c r="DF157" s="20"/>
     </row>
     <row r="158" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="33"/>
+      <c r="A158" s="38"/>
       <c r="B158" s="2" t="s">
         <v>189</v>
       </c>
@@ -22376,7 +22484,7 @@
       <c r="DF158" s="20"/>
     </row>
     <row r="159" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="42"/>
+      <c r="A159" s="39"/>
       <c r="B159" s="2" t="s">
         <v>233</v>
       </c>
@@ -22494,7 +22602,7 @@
       <c r="DF159" s="20"/>
     </row>
     <row r="160" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="30" t="s">
+      <c r="A160" s="34" t="s">
         <v>109</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -22614,7 +22722,7 @@
       <c r="DF160" s="21"/>
     </row>
     <row r="161" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="31"/>
+      <c r="A161" s="35"/>
       <c r="B161" s="3" t="s">
         <v>149</v>
       </c>
@@ -22730,7 +22838,7 @@
       <c r="DF161" s="21"/>
     </row>
     <row r="162" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="31"/>
+      <c r="A162" s="35"/>
       <c r="B162" s="3" t="s">
         <v>194</v>
       </c>
@@ -22846,7 +22954,7 @@
       <c r="DF162" s="21"/>
     </row>
     <row r="163" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="31"/>
+      <c r="A163" s="35"/>
       <c r="B163" s="3" t="s">
         <v>235</v>
       </c>
@@ -22964,7 +23072,7 @@
       <c r="DF163" s="21"/>
     </row>
     <row r="164" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="34"/>
+      <c r="A164" s="40"/>
       <c r="B164" s="3" t="s">
         <v>142</v>
       </c>
@@ -23082,7 +23190,7 @@
       <c r="DF164" s="21"/>
     </row>
     <row r="165" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="32" t="s">
+      <c r="A165" s="37" t="s">
         <v>110</v>
       </c>
       <c r="B165" s="2" t="s">
@@ -23200,7 +23308,7 @@
       <c r="DF165" s="20"/>
     </row>
     <row r="166" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="33"/>
+      <c r="A166" s="38"/>
       <c r="B166" s="2" t="s">
         <v>237</v>
       </c>
@@ -23316,7 +23424,7 @@
       <c r="DF166" s="20"/>
     </row>
     <row r="167" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="33"/>
+      <c r="A167" s="38"/>
       <c r="B167" s="2" t="s">
         <v>139</v>
       </c>
@@ -23432,7 +23540,7 @@
       <c r="DF167" s="20"/>
     </row>
     <row r="168" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="38" t="s">
+      <c r="A168" s="41" t="s">
         <v>111</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -23550,7 +23658,7 @@
       <c r="DF168" s="21"/>
     </row>
     <row r="169" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="39"/>
+      <c r="A169" s="42"/>
       <c r="B169" s="3" t="s">
         <v>239</v>
       </c>
@@ -23666,7 +23774,7 @@
       <c r="DF169" s="21"/>
     </row>
     <row r="170" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="39"/>
+      <c r="A170" s="42"/>
       <c r="B170" s="3" t="s">
         <v>236</v>
       </c>
@@ -23898,7 +24006,7 @@
       <c r="DF171" s="21"/>
     </row>
     <row r="172" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="32" t="s">
+      <c r="A172" s="37" t="s">
         <v>112</v>
       </c>
       <c r="B172" s="2" t="s">
@@ -24020,7 +24128,7 @@
       <c r="DF172" s="20"/>
     </row>
     <row r="173" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="33"/>
+      <c r="A173" s="38"/>
       <c r="B173" s="2" t="s">
         <v>247</v>
       </c>
@@ -24138,7 +24246,7 @@
       <c r="DF173" s="20"/>
     </row>
     <row r="174" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="33"/>
+      <c r="A174" s="38"/>
       <c r="B174" s="2" t="s">
         <v>219</v>
       </c>
@@ -24254,7 +24362,7 @@
       <c r="DF174" s="20"/>
     </row>
     <row r="175" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="30" t="s">
+      <c r="A175" s="34" t="s">
         <v>113</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -24376,7 +24484,7 @@
       <c r="DF175" s="21"/>
     </row>
     <row r="176" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="31"/>
+      <c r="A176" s="35"/>
       <c r="B176" s="3" t="s">
         <v>245</v>
       </c>
@@ -24492,7 +24600,7 @@
       <c r="DF176" s="21"/>
     </row>
     <row r="177" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="31"/>
+      <c r="A177" s="35"/>
       <c r="B177" s="3" t="s">
         <v>141</v>
       </c>
@@ -24608,7 +24716,7 @@
       <c r="DF177" s="21"/>
     </row>
     <row r="178" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A178" s="31"/>
+      <c r="A178" s="35"/>
       <c r="B178" s="3" t="s">
         <v>142</v>
       </c>
@@ -24726,7 +24834,7 @@
       <c r="DF178" s="21"/>
     </row>
     <row r="179" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A179" s="32" t="s">
+      <c r="A179" s="37" t="s">
         <v>114</v>
       </c>
       <c r="B179" s="2" t="s">
@@ -24850,7 +24958,7 @@
       <c r="DF179" s="20"/>
     </row>
     <row r="180" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A180" s="33"/>
+      <c r="A180" s="38"/>
       <c r="B180" s="2" t="s">
         <v>242</v>
       </c>
@@ -24968,7 +25076,7 @@
       <c r="DF180" s="20"/>
     </row>
     <row r="181" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="33"/>
+      <c r="A181" s="38"/>
       <c r="B181" s="2" t="s">
         <v>243</v>
       </c>
@@ -25086,7 +25194,7 @@
       <c r="DF181" s="20"/>
     </row>
     <row r="182" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="33"/>
+      <c r="A182" s="38"/>
       <c r="B182" s="2" t="s">
         <v>244</v>
       </c>
@@ -25204,7 +25312,7 @@
       <c r="DF182" s="20"/>
     </row>
     <row r="183" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A183" s="42"/>
+      <c r="A183" s="39"/>
       <c r="B183" s="2" t="s">
         <v>245</v>
       </c>
@@ -25320,7 +25428,7 @@
       <c r="DF183" s="20"/>
     </row>
     <row r="184" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A184" s="38" t="s">
+      <c r="A184" s="41" t="s">
         <v>115</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -25562,7 +25670,7 @@
       <c r="DF185" s="21"/>
     </row>
     <row r="186" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="32" t="s">
+      <c r="A186" s="37" t="s">
         <v>116</v>
       </c>
       <c r="B186" s="2" t="s">
@@ -25682,7 +25790,7 @@
       <c r="DF186" s="20"/>
     </row>
     <row r="187" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="33"/>
+      <c r="A187" s="38"/>
       <c r="B187" s="2" t="s">
         <v>248</v>
       </c>
@@ -25796,7 +25904,7 @@
       <c r="DF187" s="20"/>
     </row>
     <row r="188" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A188" s="30" t="s">
+      <c r="A188" s="34" t="s">
         <v>117</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -25916,7 +26024,7 @@
       <c r="DF188" s="21"/>
     </row>
     <row r="189" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="31"/>
+      <c r="A189" s="35"/>
       <c r="B189" s="3" t="s">
         <v>162</v>
       </c>
@@ -26030,7 +26138,7 @@
       <c r="DF189" s="21"/>
     </row>
     <row r="190" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="31"/>
+      <c r="A190" s="35"/>
       <c r="B190" s="3" t="s">
         <v>133</v>
       </c>
@@ -26144,7 +26252,7 @@
       <c r="DF190" s="21"/>
     </row>
     <row r="191" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="50" t="s">
+      <c r="A191" s="46" t="s">
         <v>118</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -26264,7 +26372,7 @@
       <c r="DF191" s="20"/>
     </row>
     <row r="192" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="51"/>
+      <c r="A192" s="47"/>
       <c r="B192" s="2" t="s">
         <v>249</v>
       </c>
@@ -26378,7 +26486,7 @@
       <c r="DF192" s="20"/>
     </row>
     <row r="193" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="51"/>
+      <c r="A193" s="47"/>
       <c r="B193" s="2" t="s">
         <v>167</v>
       </c>
@@ -26492,141 +26600,141 @@
       <c r="DF193" s="20"/>
     </row>
     <row r="194" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="23"/>
+      <c r="A194" s="44"/>
       <c r="B194" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C194" s="25" t="s">
+      <c r="C194" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="D194" s="26"/>
-      <c r="E194" s="26"/>
-      <c r="F194" s="27"/>
-      <c r="G194" s="28" t="s">
+      <c r="D194" s="24"/>
+      <c r="E194" s="24"/>
+      <c r="F194" s="25"/>
+      <c r="G194" s="27" t="s">
         <v>274</v>
       </c>
-      <c r="H194" s="29"/>
-      <c r="I194" s="29"/>
-      <c r="J194" s="28" t="s">
+      <c r="H194" s="28"/>
+      <c r="I194" s="28"/>
+      <c r="J194" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="K194" s="29"/>
-      <c r="L194" s="29"/>
-      <c r="M194" s="29"/>
-      <c r="N194" s="29"/>
-      <c r="O194" s="29"/>
-      <c r="P194" s="29"/>
-      <c r="Q194" s="29"/>
-      <c r="R194" s="29"/>
-      <c r="S194" s="29"/>
-      <c r="T194" s="29"/>
-      <c r="U194" s="29"/>
-      <c r="V194" s="29"/>
-      <c r="W194" s="29"/>
-      <c r="X194" s="29"/>
-      <c r="Y194" s="28" t="s">
+      <c r="K194" s="28"/>
+      <c r="L194" s="28"/>
+      <c r="M194" s="28"/>
+      <c r="N194" s="28"/>
+      <c r="O194" s="28"/>
+      <c r="P194" s="28"/>
+      <c r="Q194" s="28"/>
+      <c r="R194" s="28"/>
+      <c r="S194" s="28"/>
+      <c r="T194" s="28"/>
+      <c r="U194" s="28"/>
+      <c r="V194" s="28"/>
+      <c r="W194" s="28"/>
+      <c r="X194" s="28"/>
+      <c r="Y194" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="Z194" s="29"/>
-      <c r="AA194" s="29"/>
-      <c r="AB194" s="29"/>
-      <c r="AC194" s="29"/>
-      <c r="AD194" s="29"/>
-      <c r="AE194" s="29"/>
-      <c r="AF194" s="29"/>
-      <c r="AG194" s="29"/>
-      <c r="AH194" s="29"/>
-      <c r="AI194" s="29"/>
-      <c r="AJ194" s="29"/>
-      <c r="AK194" s="29"/>
-      <c r="AL194" s="29"/>
-      <c r="AM194" s="29"/>
-      <c r="AN194" s="29"/>
-      <c r="AO194" s="29"/>
-      <c r="AP194" s="29"/>
-      <c r="AQ194" s="45" t="s">
+      <c r="Z194" s="28"/>
+      <c r="AA194" s="28"/>
+      <c r="AB194" s="28"/>
+      <c r="AC194" s="28"/>
+      <c r="AD194" s="28"/>
+      <c r="AE194" s="28"/>
+      <c r="AF194" s="28"/>
+      <c r="AG194" s="28"/>
+      <c r="AH194" s="28"/>
+      <c r="AI194" s="28"/>
+      <c r="AJ194" s="28"/>
+      <c r="AK194" s="28"/>
+      <c r="AL194" s="28"/>
+      <c r="AM194" s="28"/>
+      <c r="AN194" s="28"/>
+      <c r="AO194" s="28"/>
+      <c r="AP194" s="28"/>
+      <c r="AQ194" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="AR194" s="46"/>
-      <c r="AS194" s="46"/>
-      <c r="AT194" s="46"/>
-      <c r="AU194" s="46"/>
-      <c r="AV194" s="46"/>
-      <c r="AW194" s="46"/>
-      <c r="AX194" s="46"/>
-      <c r="AY194" s="46"/>
-      <c r="AZ194" s="46"/>
-      <c r="BA194" s="47"/>
-      <c r="BB194" s="45" t="s">
+      <c r="AR194" s="30"/>
+      <c r="AS194" s="30"/>
+      <c r="AT194" s="30"/>
+      <c r="AU194" s="30"/>
+      <c r="AV194" s="30"/>
+      <c r="AW194" s="30"/>
+      <c r="AX194" s="30"/>
+      <c r="AY194" s="30"/>
+      <c r="AZ194" s="30"/>
+      <c r="BA194" s="31"/>
+      <c r="BB194" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="BC194" s="46"/>
-      <c r="BD194" s="46"/>
-      <c r="BE194" s="46"/>
-      <c r="BF194" s="46"/>
-      <c r="BG194" s="46"/>
-      <c r="BH194" s="46"/>
-      <c r="BI194" s="46"/>
-      <c r="BJ194" s="46"/>
-      <c r="BK194" s="46"/>
-      <c r="BL194" s="46"/>
-      <c r="BM194" s="46"/>
-      <c r="BN194" s="46"/>
-      <c r="BO194" s="46"/>
-      <c r="BP194" s="47"/>
-      <c r="BQ194" s="48" t="s">
+      <c r="BC194" s="30"/>
+      <c r="BD194" s="30"/>
+      <c r="BE194" s="30"/>
+      <c r="BF194" s="30"/>
+      <c r="BG194" s="30"/>
+      <c r="BH194" s="30"/>
+      <c r="BI194" s="30"/>
+      <c r="BJ194" s="30"/>
+      <c r="BK194" s="30"/>
+      <c r="BL194" s="30"/>
+      <c r="BM194" s="30"/>
+      <c r="BN194" s="30"/>
+      <c r="BO194" s="30"/>
+      <c r="BP194" s="31"/>
+      <c r="BQ194" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="BR194" s="49"/>
-      <c r="BS194" s="49"/>
-      <c r="BT194" s="49"/>
-      <c r="BU194" s="44" t="s">
+      <c r="BR194" s="33"/>
+      <c r="BS194" s="33"/>
+      <c r="BT194" s="33"/>
+      <c r="BU194" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="BV194" s="26"/>
-      <c r="BW194" s="26"/>
-      <c r="BX194" s="26"/>
-      <c r="BY194" s="26"/>
-      <c r="BZ194" s="26"/>
-      <c r="CA194" s="26"/>
-      <c r="CB194" s="26"/>
-      <c r="CC194" s="26"/>
-      <c r="CD194" s="26"/>
-      <c r="CE194" s="26"/>
-      <c r="CF194" s="26"/>
-      <c r="CG194" s="26"/>
-      <c r="CH194" s="26"/>
-      <c r="CI194" s="26"/>
-      <c r="CJ194" s="26"/>
-      <c r="CK194" s="26"/>
-      <c r="CL194" s="27"/>
-      <c r="CM194" s="44" t="s">
+      <c r="BV194" s="24"/>
+      <c r="BW194" s="24"/>
+      <c r="BX194" s="24"/>
+      <c r="BY194" s="24"/>
+      <c r="BZ194" s="24"/>
+      <c r="CA194" s="24"/>
+      <c r="CB194" s="24"/>
+      <c r="CC194" s="24"/>
+      <c r="CD194" s="24"/>
+      <c r="CE194" s="24"/>
+      <c r="CF194" s="24"/>
+      <c r="CG194" s="24"/>
+      <c r="CH194" s="24"/>
+      <c r="CI194" s="24"/>
+      <c r="CJ194" s="24"/>
+      <c r="CK194" s="24"/>
+      <c r="CL194" s="25"/>
+      <c r="CM194" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="CN194" s="26"/>
-      <c r="CO194" s="26"/>
-      <c r="CP194" s="26"/>
-      <c r="CQ194" s="26"/>
-      <c r="CR194" s="26"/>
-      <c r="CS194" s="26"/>
-      <c r="CT194" s="26"/>
-      <c r="CU194" s="26"/>
-      <c r="CV194" s="27"/>
-      <c r="CW194" s="44" t="s">
+      <c r="CN194" s="24"/>
+      <c r="CO194" s="24"/>
+      <c r="CP194" s="24"/>
+      <c r="CQ194" s="24"/>
+      <c r="CR194" s="24"/>
+      <c r="CS194" s="24"/>
+      <c r="CT194" s="24"/>
+      <c r="CU194" s="24"/>
+      <c r="CV194" s="25"/>
+      <c r="CW194" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="CX194" s="26"/>
-      <c r="CY194" s="26"/>
-      <c r="CZ194" s="26"/>
-      <c r="DA194" s="26"/>
-      <c r="DB194" s="26"/>
-      <c r="DC194" s="26"/>
-      <c r="DD194" s="26"/>
-      <c r="DE194" s="26"/>
-      <c r="DF194" s="27"/>
+      <c r="CX194" s="24"/>
+      <c r="CY194" s="24"/>
+      <c r="CZ194" s="24"/>
+      <c r="DA194" s="24"/>
+      <c r="DB194" s="24"/>
+      <c r="DC194" s="24"/>
+      <c r="DD194" s="24"/>
+      <c r="DE194" s="24"/>
+      <c r="DF194" s="25"/>
     </row>
-    <row r="195" spans="1:110" ht="120" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="24"/>
+    <row r="195" spans="1:110" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A195" s="45"/>
       <c r="B195" s="12" t="s">
         <v>2</v>
       </c>
@@ -27288,7 +27396,7 @@
       </c>
     </row>
     <row r="197" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="32" t="s">
+      <c r="A197" s="37" t="s">
         <v>119</v>
       </c>
       <c r="B197" s="2" t="s">
@@ -27406,7 +27514,7 @@
       <c r="DF197" s="20"/>
     </row>
     <row r="198" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="33"/>
+      <c r="A198" s="38"/>
       <c r="B198" s="2" t="s">
         <v>250</v>
       </c>
@@ -27522,7 +27630,7 @@
       <c r="DF198" s="20"/>
     </row>
     <row r="199" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="30" t="s">
+      <c r="A199" s="34" t="s">
         <v>120</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -27640,7 +27748,7 @@
       <c r="DF199" s="21"/>
     </row>
     <row r="200" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="31"/>
+      <c r="A200" s="35"/>
       <c r="B200" s="3" t="s">
         <v>251</v>
       </c>
@@ -27758,7 +27866,7 @@
       <c r="DF200" s="21"/>
     </row>
     <row r="201" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="32" t="s">
+      <c r="A201" s="37" t="s">
         <v>121</v>
       </c>
       <c r="B201" s="2" t="s">
@@ -27878,7 +27986,7 @@
       <c r="DF201" s="20"/>
     </row>
     <row r="202" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="33"/>
+      <c r="A202" s="38"/>
       <c r="B202" s="2" t="s">
         <v>182</v>
       </c>
@@ -27996,7 +28104,7 @@
       <c r="DF202" s="20"/>
     </row>
     <row r="203" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="33"/>
+      <c r="A203" s="38"/>
       <c r="B203" s="2" t="s">
         <v>181</v>
       </c>
@@ -28114,7 +28222,7 @@
       <c r="DF203" s="20"/>
     </row>
     <row r="204" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="30" t="s">
+      <c r="A204" s="34" t="s">
         <v>122</v>
       </c>
       <c r="B204" s="3" t="s">
@@ -28208,13 +28316,21 @@
       <c r="CJ204" s="21"/>
       <c r="CK204" s="21"/>
       <c r="CL204" s="21"/>
-      <c r="CM204" s="21"/>
-      <c r="CN204" s="21"/>
-      <c r="CO204" s="21"/>
+      <c r="CM204" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="CN204" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="CO204" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CP204" s="21"/>
       <c r="CQ204" s="21"/>
       <c r="CR204" s="21"/>
-      <c r="CS204" s="21"/>
+      <c r="CS204" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CT204" s="21"/>
       <c r="CU204" s="21"/>
       <c r="CV204" s="21"/>
@@ -28230,7 +28346,7 @@
       <c r="DF204" s="21"/>
     </row>
     <row r="205" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="31"/>
+      <c r="A205" s="35"/>
       <c r="B205" s="3" t="s">
         <v>253</v>
       </c>
@@ -28322,13 +28438,21 @@
       <c r="CJ205" s="21"/>
       <c r="CK205" s="21"/>
       <c r="CL205" s="21"/>
-      <c r="CM205" s="21"/>
-      <c r="CN205" s="21"/>
-      <c r="CO205" s="21"/>
+      <c r="CM205" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="CN205" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="CO205" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CP205" s="21"/>
       <c r="CQ205" s="21"/>
       <c r="CR205" s="21"/>
-      <c r="CS205" s="21"/>
+      <c r="CS205" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CT205" s="21"/>
       <c r="CU205" s="21"/>
       <c r="CV205" s="21"/>
@@ -28344,7 +28468,7 @@
       <c r="DF205" s="21"/>
     </row>
     <row r="206" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="31"/>
+      <c r="A206" s="35"/>
       <c r="B206" s="3" t="s">
         <v>254</v>
       </c>
@@ -28436,9 +28560,15 @@
       <c r="CJ206" s="21"/>
       <c r="CK206" s="21"/>
       <c r="CL206" s="21"/>
-      <c r="CM206" s="21"/>
-      <c r="CN206" s="21"/>
-      <c r="CO206" s="21"/>
+      <c r="CM206" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="CN206" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="CO206" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CP206" s="21"/>
       <c r="CQ206" s="21"/>
       <c r="CR206" s="21"/>
@@ -28458,7 +28588,7 @@
       <c r="DF206" s="21"/>
     </row>
     <row r="207" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A207" s="31"/>
+      <c r="A207" s="35"/>
       <c r="B207" s="3" t="s">
         <v>255</v>
       </c>
@@ -28550,9 +28680,15 @@
       <c r="CJ207" s="21"/>
       <c r="CK207" s="21"/>
       <c r="CL207" s="21"/>
-      <c r="CM207" s="21"/>
-      <c r="CN207" s="21"/>
-      <c r="CO207" s="21"/>
+      <c r="CM207" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="CN207" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="CO207" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CP207" s="21"/>
       <c r="CQ207" s="21"/>
       <c r="CR207" s="21"/>
@@ -28572,7 +28708,7 @@
       <c r="DF207" s="21"/>
     </row>
     <row r="208" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A208" s="32" t="s">
+      <c r="A208" s="37" t="s">
         <v>123</v>
       </c>
       <c r="B208" s="2" t="s">
@@ -28669,11 +28805,19 @@
       <c r="CM208" s="20"/>
       <c r="CN208" s="20"/>
       <c r="CO208" s="20"/>
-      <c r="CP208" s="20"/>
-      <c r="CQ208" s="20"/>
-      <c r="CR208" s="20"/>
+      <c r="CP208" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="CQ208" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="CR208" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="CS208" s="20"/>
-      <c r="CT208" s="20"/>
+      <c r="CT208" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CU208" s="20"/>
       <c r="CV208" s="20"/>
       <c r="CW208" s="20"/>
@@ -28688,7 +28832,7 @@
       <c r="DF208" s="20"/>
     </row>
     <row r="209" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="33"/>
+      <c r="A209" s="38"/>
       <c r="B209" s="2" t="s">
         <v>257</v>
       </c>
@@ -28783,11 +28927,17 @@
       <c r="CM209" s="20"/>
       <c r="CN209" s="20"/>
       <c r="CO209" s="20"/>
-      <c r="CP209" s="20"/>
-      <c r="CQ209" s="20"/>
+      <c r="CP209" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="CQ209" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CR209" s="20"/>
       <c r="CS209" s="20"/>
-      <c r="CT209" s="20"/>
+      <c r="CT209" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="CU209" s="20"/>
       <c r="CV209" s="20"/>
       <c r="CW209" s="20"/>
@@ -28802,7 +28952,7 @@
       <c r="DF209" s="20"/>
     </row>
     <row r="210" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="33"/>
+      <c r="A210" s="38"/>
       <c r="B210" s="2" t="s">
         <v>258</v>
       </c>
@@ -28897,7 +29047,9 @@
       <c r="CM210" s="20"/>
       <c r="CN210" s="20"/>
       <c r="CO210" s="20"/>
-      <c r="CP210" s="20"/>
+      <c r="CP210" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CQ210" s="20"/>
       <c r="CR210" s="20"/>
       <c r="CS210" s="20"/>
@@ -28916,7 +29068,7 @@
       <c r="DF210" s="20"/>
     </row>
     <row r="211" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="30" t="s">
+      <c r="A211" s="34" t="s">
         <v>124</v>
       </c>
       <c r="B211" s="3" t="s">
@@ -29013,11 +29165,19 @@
       <c r="CM211" s="21"/>
       <c r="CN211" s="21"/>
       <c r="CO211" s="21"/>
-      <c r="CP211" s="21"/>
-      <c r="CQ211" s="21"/>
-      <c r="CR211" s="21"/>
+      <c r="CP211" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="CQ211" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="CR211" s="21" t="s">
+        <v>432</v>
+      </c>
       <c r="CS211" s="21"/>
-      <c r="CT211" s="21"/>
+      <c r="CT211" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CU211" s="21"/>
       <c r="CV211" s="21"/>
       <c r="CW211" s="21"/>
@@ -29032,7 +29192,7 @@
       <c r="DF211" s="21"/>
     </row>
     <row r="212" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="31"/>
+      <c r="A212" s="35"/>
       <c r="B212" s="3" t="s">
         <v>256</v>
       </c>
@@ -29127,7 +29287,9 @@
       <c r="CM212" s="21"/>
       <c r="CN212" s="21"/>
       <c r="CO212" s="21"/>
-      <c r="CP212" s="21"/>
+      <c r="CP212" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CQ212" s="21"/>
       <c r="CR212" s="21"/>
       <c r="CS212" s="21"/>
@@ -29146,7 +29308,7 @@
       <c r="DF212" s="21"/>
     </row>
     <row r="213" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="31"/>
+      <c r="A213" s="35"/>
       <c r="B213" s="3" t="s">
         <v>142</v>
       </c>
@@ -29241,11 +29403,17 @@
       <c r="CM213" s="21"/>
       <c r="CN213" s="21"/>
       <c r="CO213" s="21"/>
-      <c r="CP213" s="21"/>
-      <c r="CQ213" s="21"/>
+      <c r="CP213" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="CQ213" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CR213" s="21"/>
       <c r="CS213" s="21"/>
-      <c r="CT213" s="21"/>
+      <c r="CT213" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="CU213" s="21"/>
       <c r="CV213" s="21"/>
       <c r="CW213" s="21"/>
@@ -29260,7 +29428,7 @@
       <c r="DF213" s="21"/>
     </row>
     <row r="214" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="31"/>
+      <c r="A214" s="35"/>
       <c r="B214" s="3" t="s">
         <v>141</v>
       </c>
@@ -29374,7 +29542,7 @@
       <c r="DF214" s="21"/>
     </row>
     <row r="215" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="31"/>
+      <c r="A215" s="35"/>
       <c r="B215" s="3" t="s">
         <v>222</v>
       </c>
@@ -29488,7 +29656,7 @@
       <c r="DF215" s="21"/>
     </row>
     <row r="216" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="32" t="s">
+      <c r="A216" s="37" t="s">
         <v>125</v>
       </c>
       <c r="B216" s="2" t="s">
@@ -29604,7 +29772,7 @@
       <c r="DF216" s="20"/>
     </row>
     <row r="217" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A217" s="33"/>
+      <c r="A217" s="38"/>
       <c r="B217" s="2" t="s">
         <v>260</v>
       </c>
@@ -29718,7 +29886,7 @@
       <c r="DF217" s="20"/>
     </row>
     <row r="218" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A218" s="30" t="s">
+      <c r="A218" s="34" t="s">
         <v>126</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -29834,7 +30002,7 @@
       <c r="DF218" s="21"/>
     </row>
     <row r="219" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" s="31"/>
+      <c r="A219" s="35"/>
       <c r="B219" s="3" t="s">
         <v>272</v>
       </c>
@@ -29948,7 +30116,7 @@
       <c r="DF219" s="21"/>
     </row>
     <row r="220" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A220" s="31"/>
+      <c r="A220" s="35"/>
       <c r="B220" s="3" t="s">
         <v>273</v>
       </c>
@@ -30062,7 +30230,7 @@
       <c r="DF220" s="21"/>
     </row>
     <row r="221" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A221" s="32" t="s">
+      <c r="A221" s="37" t="s">
         <v>127</v>
       </c>
       <c r="B221" s="2" t="s">
@@ -30178,7 +30346,7 @@
       <c r="DF221" s="20"/>
     </row>
     <row r="222" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A222" s="33"/>
+      <c r="A222" s="38"/>
       <c r="B222" s="2" t="s">
         <v>271</v>
       </c>
@@ -30292,7 +30460,7 @@
       <c r="DF222" s="20"/>
     </row>
     <row r="223" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A223" s="30" t="s">
+      <c r="A223" s="34" t="s">
         <v>128</v>
       </c>
       <c r="B223" s="3" t="s">
@@ -30410,7 +30578,7 @@
       <c r="DF223" s="21"/>
     </row>
     <row r="224" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A224" s="31"/>
+      <c r="A224" s="35"/>
       <c r="B224" s="3" t="s">
         <v>269</v>
       </c>
@@ -30530,7 +30698,7 @@
       <c r="DF224" s="21"/>
     </row>
     <row r="225" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A225" s="31"/>
+      <c r="A225" s="35"/>
       <c r="B225" s="3" t="s">
         <v>270</v>
       </c>
@@ -30648,7 +30816,7 @@
       <c r="DF225" s="21"/>
     </row>
     <row r="226" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A226" s="31"/>
+      <c r="A226" s="35"/>
       <c r="B226" s="3" t="s">
         <v>266</v>
       </c>
@@ -30766,7 +30934,7 @@
       <c r="DF226" s="21"/>
     </row>
     <row r="227" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A227" s="32" t="s">
+      <c r="A227" s="37" t="s">
         <v>129</v>
       </c>
       <c r="B227" s="2" t="s">
@@ -30882,7 +31050,7 @@
       <c r="DF227" s="20"/>
     </row>
     <row r="228" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A228" s="33"/>
+      <c r="A228" s="38"/>
       <c r="B228" s="2" t="s">
         <v>267</v>
       </c>
@@ -30996,7 +31164,7 @@
       <c r="DF228" s="20"/>
     </row>
     <row r="229" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A229" s="33"/>
+      <c r="A229" s="38"/>
       <c r="B229" s="2" t="s">
         <v>268</v>
       </c>
@@ -31110,7 +31278,7 @@
       <c r="DF229" s="20"/>
     </row>
     <row r="230" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A230" s="30" t="s">
+      <c r="A230" s="34" t="s">
         <v>130</v>
       </c>
       <c r="B230" s="3" t="s">
@@ -31226,7 +31394,7 @@
       <c r="DF230" s="21"/>
     </row>
     <row r="231" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A231" s="31"/>
+      <c r="A231" s="35"/>
       <c r="B231" s="3" t="s">
         <v>262</v>
       </c>
@@ -31340,7 +31508,7 @@
       <c r="DF231" s="21"/>
     </row>
     <row r="232" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="31"/>
+      <c r="A232" s="35"/>
       <c r="B232" s="3" t="s">
         <v>263</v>
       </c>
@@ -31454,7 +31622,7 @@
       <c r="DF232" s="21"/>
     </row>
     <row r="233" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A233" s="32" t="s">
+      <c r="A233" s="37" t="s">
         <v>131</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -31576,7 +31744,7 @@
       <c r="DF233" s="20"/>
     </row>
     <row r="234" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A234" s="33"/>
+      <c r="A234" s="38"/>
       <c r="B234" s="2" t="s">
         <v>139</v>
       </c>
@@ -31692,7 +31860,7 @@
       <c r="DF234" s="20"/>
     </row>
     <row r="235" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A235" s="30" t="s">
+      <c r="A235" s="34" t="s">
         <v>132</v>
       </c>
       <c r="B235" s="3" t="s">
@@ -31814,7 +31982,7 @@
       <c r="DF235" s="21"/>
     </row>
     <row r="236" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A236" s="31"/>
+      <c r="A236" s="35"/>
       <c r="B236" s="3" t="s">
         <v>141</v>
       </c>
@@ -31932,7 +32100,7 @@
       <c r="DF236" s="21"/>
     </row>
     <row r="237" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A237" s="31"/>
+      <c r="A237" s="35"/>
       <c r="B237" s="3" t="s">
         <v>264</v>
       </c>
@@ -32048,7 +32216,7 @@
       <c r="DF237" s="21"/>
     </row>
     <row r="238" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A238" s="52"/>
+      <c r="A238" s="36"/>
       <c r="B238" s="3" t="s">
         <v>142</v>
       </c>
@@ -32167,45 +32335,50 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="CW1:DF1"/>
-    <mergeCell ref="CW143:DF143"/>
-    <mergeCell ref="CW194:DF194"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="J73:X73"/>
-    <mergeCell ref="Y73:AP73"/>
-    <mergeCell ref="AQ73:BA73"/>
-    <mergeCell ref="BB73:BP73"/>
-    <mergeCell ref="BQ73:BT73"/>
-    <mergeCell ref="BU73:CL73"/>
-    <mergeCell ref="CM73:CV73"/>
-    <mergeCell ref="CW73:DF73"/>
-    <mergeCell ref="CM194:CV194"/>
-    <mergeCell ref="AQ1:BA1"/>
-    <mergeCell ref="BB1:BP1"/>
-    <mergeCell ref="BQ1:BT1"/>
-    <mergeCell ref="BU1:CL1"/>
-    <mergeCell ref="CM1:CV1"/>
-    <mergeCell ref="BU194:CL194"/>
-    <mergeCell ref="A235:A238"/>
-    <mergeCell ref="A221:A222"/>
-    <mergeCell ref="A223:A226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="A230:A232"/>
-    <mergeCell ref="A233:A234"/>
-    <mergeCell ref="A208:A210"/>
-    <mergeCell ref="A211:A215"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="A218:A220"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A199:A200"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A204:A207"/>
-    <mergeCell ref="Y194:AP194"/>
-    <mergeCell ref="AQ194:BA194"/>
-    <mergeCell ref="BB194:BP194"/>
-    <mergeCell ref="BQ194:BT194"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:X1"/>
+    <mergeCell ref="Y1:AP1"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A139:A142"/>
+    <mergeCell ref="C143:F143"/>
+    <mergeCell ref="G143:I143"/>
+    <mergeCell ref="J143:X143"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A134:A138"/>
     <mergeCell ref="A156:A159"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A165:A167"/>
@@ -32230,50 +32403,45 @@
     <mergeCell ref="A179:A183"/>
     <mergeCell ref="A184:A185"/>
     <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A139:A142"/>
-    <mergeCell ref="C143:F143"/>
-    <mergeCell ref="G143:I143"/>
-    <mergeCell ref="J143:X143"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A134:A138"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:X1"/>
-    <mergeCell ref="Y1:AP1"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A199:A200"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A204:A207"/>
+    <mergeCell ref="Y194:AP194"/>
+    <mergeCell ref="AQ194:BA194"/>
+    <mergeCell ref="BB194:BP194"/>
+    <mergeCell ref="BQ194:BT194"/>
+    <mergeCell ref="A235:A238"/>
+    <mergeCell ref="A221:A222"/>
+    <mergeCell ref="A223:A226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="A230:A232"/>
+    <mergeCell ref="A233:A234"/>
+    <mergeCell ref="A208:A210"/>
+    <mergeCell ref="A211:A215"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="A218:A220"/>
+    <mergeCell ref="CW1:DF1"/>
+    <mergeCell ref="CW143:DF143"/>
+    <mergeCell ref="CW194:DF194"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="J73:X73"/>
+    <mergeCell ref="Y73:AP73"/>
+    <mergeCell ref="AQ73:BA73"/>
+    <mergeCell ref="BB73:BP73"/>
+    <mergeCell ref="BQ73:BT73"/>
+    <mergeCell ref="BU73:CL73"/>
+    <mergeCell ref="CM73:CV73"/>
+    <mergeCell ref="CW73:DF73"/>
+    <mergeCell ref="CM194:CV194"/>
+    <mergeCell ref="AQ1:BA1"/>
+    <mergeCell ref="BB1:BP1"/>
+    <mergeCell ref="BQ1:BT1"/>
+    <mergeCell ref="BU1:CL1"/>
+    <mergeCell ref="CM1:CV1"/>
+    <mergeCell ref="BU194:CL194"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Team 3  - Del 6 CRUD Matrix.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Team 3  - Del 6 CRUD Matrix.xlsx
+++ b/Documentation/Team 3  - Del 6 CRUD Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Team-3-Orion\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pride\OneDrive\Documents\GitHub\Team-3-Orion\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7054B26-6B95-418D-B4A5-58C32F262665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{B7054B26-6B95-418D-B4A5-58C32F262665}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{0467BB1D-B464-4B93-98F2-B04DB05C5D55}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1611" uniqueCount="436">
   <si>
     <r>
       <rPr>
@@ -1829,6 +1829,9 @@
   </si>
   <si>
     <t>C/R</t>
+  </si>
+  <si>
+    <t>R/U</t>
   </si>
 </sst>
 </file>
@@ -2086,7 +2089,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2095,14 +2104,56 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -2119,61 +2170,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2517,10 +2520,10 @@
   <dimension ref="A1:DF238"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="BA115" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="CC217" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="BF2" sqref="BF2:BH2"/>
+      <selection pane="bottomRight" activeCell="CW222" sqref="CW222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="6" x14ac:dyDescent="0.2"/>
@@ -2580,141 +2583,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
+      <c r="A1" s="23"/>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="27" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="27" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="27" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="29" t="s">
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="29" t="s">
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
+      <c r="AY1" s="46"/>
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="47"/>
+      <c r="BB1" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
-      <c r="BN1" s="30"/>
-      <c r="BO1" s="30"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="32" t="s">
+      <c r="BC1" s="46"/>
+      <c r="BD1" s="46"/>
+      <c r="BE1" s="46"/>
+      <c r="BF1" s="46"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="47"/>
+      <c r="BQ1" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="23" t="s">
+      <c r="BR1" s="49"/>
+      <c r="BS1" s="49"/>
+      <c r="BT1" s="49"/>
+      <c r="BU1" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV1" s="24"/>
-      <c r="BW1" s="24"/>
-      <c r="BX1" s="24"/>
-      <c r="BY1" s="24"/>
-      <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-      <c r="CD1" s="24"/>
-      <c r="CE1" s="24"/>
-      <c r="CF1" s="24"/>
-      <c r="CG1" s="24"/>
-      <c r="CH1" s="24"/>
-      <c r="CI1" s="24"/>
-      <c r="CJ1" s="24"/>
-      <c r="CK1" s="24"/>
-      <c r="CL1" s="25"/>
-      <c r="CM1" s="23" t="s">
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="26"/>
+      <c r="CD1" s="26"/>
+      <c r="CE1" s="26"/>
+      <c r="CF1" s="26"/>
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="26"/>
+      <c r="CJ1" s="26"/>
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="27"/>
+      <c r="CM1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN1" s="24"/>
-      <c r="CO1" s="24"/>
-      <c r="CP1" s="24"/>
-      <c r="CQ1" s="24"/>
-      <c r="CR1" s="24"/>
-      <c r="CS1" s="24"/>
-      <c r="CT1" s="24"/>
-      <c r="CU1" s="24"/>
-      <c r="CV1" s="25"/>
-      <c r="CW1" s="23" t="s">
+      <c r="CN1" s="26"/>
+      <c r="CO1" s="26"/>
+      <c r="CP1" s="26"/>
+      <c r="CQ1" s="26"/>
+      <c r="CR1" s="26"/>
+      <c r="CS1" s="26"/>
+      <c r="CT1" s="26"/>
+      <c r="CU1" s="26"/>
+      <c r="CV1" s="27"/>
+      <c r="CW1" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX1" s="24"/>
-      <c r="CY1" s="24"/>
-      <c r="CZ1" s="24"/>
-      <c r="DA1" s="24"/>
-      <c r="DB1" s="24"/>
-      <c r="DC1" s="24"/>
-      <c r="DD1" s="24"/>
-      <c r="DE1" s="24"/>
-      <c r="DF1" s="25"/>
+      <c r="CX1" s="26"/>
+      <c r="CY1" s="26"/>
+      <c r="CZ1" s="26"/>
+      <c r="DA1" s="26"/>
+      <c r="DB1" s="26"/>
+      <c r="DC1" s="26"/>
+      <c r="DD1" s="26"/>
+      <c r="DE1" s="26"/>
+      <c r="DF1" s="27"/>
     </row>
     <row r="2" spans="1:110" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="45"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -3376,7 +3379,7 @@
       </c>
     </row>
     <row r="4" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3496,7 +3499,7 @@
       <c r="DF4" s="20"/>
     </row>
     <row r="5" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="49"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="2" t="s">
         <v>134</v>
       </c>
@@ -3614,7 +3617,7 @@
       <c r="DF5" s="20"/>
     </row>
     <row r="6" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="49"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="2" t="s">
         <v>135</v>
       </c>
@@ -3728,7 +3731,7 @@
       <c r="DF6" s="20"/>
     </row>
     <row r="7" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="50"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="2" t="s">
         <v>136</v>
       </c>
@@ -3842,7 +3845,7 @@
       <c r="DF7" s="20"/>
     </row>
     <row r="8" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3962,7 +3965,7 @@
       <c r="DF8" s="21"/>
     </row>
     <row r="9" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="35"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="3" t="s">
         <v>138</v>
       </c>
@@ -4076,7 +4079,7 @@
       <c r="DF9" s="21"/>
     </row>
     <row r="10" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="35"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="3" t="s">
         <v>139</v>
       </c>
@@ -4190,7 +4193,7 @@
       <c r="DF10" s="21"/>
     </row>
     <row r="11" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4312,7 +4315,7 @@
       <c r="DF11" s="20"/>
     </row>
     <row r="12" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="38"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="2" t="s">
         <v>137</v>
       </c>
@@ -4428,7 +4431,7 @@
       <c r="DF12" s="20"/>
     </row>
     <row r="13" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="38"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="2" t="s">
         <v>141</v>
       </c>
@@ -4544,7 +4547,7 @@
       <c r="DF13" s="20"/>
     </row>
     <row r="14" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="2" t="s">
         <v>142</v>
       </c>
@@ -4662,7 +4665,7 @@
       <c r="DF14" s="20"/>
     </row>
     <row r="15" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="38" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4778,7 +4781,7 @@
       <c r="DF15" s="21"/>
     </row>
     <row r="16" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="42"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="3" t="s">
         <v>144</v>
       </c>
@@ -4892,7 +4895,7 @@
       <c r="DF16" s="21"/>
     </row>
     <row r="17" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="42"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="3" t="s">
         <v>133</v>
       </c>
@@ -5006,7 +5009,7 @@
       <c r="DF17" s="21"/>
     </row>
     <row r="18" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="32" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -5128,7 +5131,7 @@
       <c r="DF18" s="20"/>
     </row>
     <row r="19" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="38"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="2" t="s">
         <v>146</v>
       </c>
@@ -5248,7 +5251,7 @@
       <c r="DF19" s="20"/>
     </row>
     <row r="20" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="2" t="s">
         <v>147</v>
       </c>
@@ -5362,7 +5365,7 @@
       <c r="DF20" s="20"/>
     </row>
     <row r="21" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="30" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -5478,7 +5481,7 @@
       <c r="DF21" s="21"/>
     </row>
     <row r="22" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="35"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="3" t="s">
         <v>139</v>
       </c>
@@ -5592,7 +5595,7 @@
       <c r="DF22" s="21"/>
     </row>
     <row r="23" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="35"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="3" t="s">
         <v>149</v>
       </c>
@@ -5706,7 +5709,7 @@
       <c r="DF23" s="21"/>
     </row>
     <row r="24" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="32" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5830,7 +5833,7 @@
       <c r="DF24" s="20"/>
     </row>
     <row r="25" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="38"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="2" t="s">
         <v>151</v>
       </c>
@@ -5950,7 +5953,7 @@
       <c r="DF25" s="20"/>
     </row>
     <row r="26" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="38"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="2" t="s">
         <v>152</v>
       </c>
@@ -6070,7 +6073,7 @@
       <c r="DF26" s="20"/>
     </row>
     <row r="27" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="38"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="2" t="s">
         <v>153</v>
       </c>
@@ -6188,7 +6191,7 @@
       <c r="DF27" s="20"/>
     </row>
     <row r="28" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="38"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="2" t="s">
         <v>154</v>
       </c>
@@ -6306,7 +6309,7 @@
       <c r="DF28" s="20"/>
     </row>
     <row r="29" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="38"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="2" t="s">
         <v>155</v>
       </c>
@@ -6424,7 +6427,7 @@
       <c r="DF29" s="20"/>
     </row>
     <row r="30" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="38"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="2" t="s">
         <v>156</v>
       </c>
@@ -6542,7 +6545,7 @@
       <c r="DF30" s="20"/>
     </row>
     <row r="31" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="38"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="2" t="s">
         <v>150</v>
       </c>
@@ -6660,7 +6663,7 @@
       <c r="DF31" s="20"/>
     </row>
     <row r="32" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="38"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="2" t="s">
         <v>138</v>
       </c>
@@ -6774,7 +6777,7 @@
       <c r="DF32" s="20"/>
     </row>
     <row r="33" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -6890,7 +6893,7 @@
       <c r="DF33" s="21"/>
     </row>
     <row r="34" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="35"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="3" t="s">
         <v>157</v>
       </c>
@@ -7004,7 +7007,7 @@
       <c r="DF34" s="21"/>
     </row>
     <row r="35" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="40"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="3" t="s">
         <v>158</v>
       </c>
@@ -7118,7 +7121,7 @@
       <c r="DF35" s="21"/>
     </row>
     <row r="36" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="32" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -7238,7 +7241,7 @@
       <c r="DF36" s="18"/>
     </row>
     <row r="37" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="38"/>
+      <c r="A37" s="33"/>
       <c r="B37" s="2" t="s">
         <v>160</v>
       </c>
@@ -7356,7 +7359,7 @@
       <c r="DF37" s="18"/>
     </row>
     <row r="38" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -7472,7 +7475,7 @@
       <c r="DF38" s="15"/>
     </row>
     <row r="39" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="35"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="3" t="s">
         <v>162</v>
       </c>
@@ -7586,7 +7589,7 @@
       <c r="DF39" s="15"/>
     </row>
     <row r="40" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="35"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="3" t="s">
         <v>163</v>
       </c>
@@ -7700,7 +7703,7 @@
       <c r="DF40" s="15"/>
     </row>
     <row r="41" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="35"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="3" t="s">
         <v>159</v>
       </c>
@@ -7814,7 +7817,7 @@
       <c r="DF41" s="15"/>
     </row>
     <row r="42" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="32" t="s">
         <v>79</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -7930,7 +7933,7 @@
       <c r="DF42" s="20"/>
     </row>
     <row r="43" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="38"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="2" t="s">
         <v>164</v>
       </c>
@@ -8044,7 +8047,7 @@
       <c r="DF43" s="20"/>
     </row>
     <row r="44" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="38"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="2" t="s">
         <v>165</v>
       </c>
@@ -8158,7 +8161,7 @@
       <c r="DF44" s="20"/>
     </row>
     <row r="45" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="39"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="2" t="s">
         <v>166</v>
       </c>
@@ -8272,7 +8275,7 @@
       <c r="DF45" s="20"/>
     </row>
     <row r="46" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="30" t="s">
         <v>80</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -8388,7 +8391,7 @@
       <c r="DF46" s="21"/>
     </row>
     <row r="47" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="35"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="3" t="s">
         <v>168</v>
       </c>
@@ -8502,7 +8505,7 @@
       <c r="DF47" s="21"/>
     </row>
     <row r="48" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="35"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="3" t="s">
         <v>169</v>
       </c>
@@ -8616,7 +8619,7 @@
       <c r="DF48" s="21"/>
     </row>
     <row r="49" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="35"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="3" t="s">
         <v>170</v>
       </c>
@@ -8730,7 +8733,7 @@
       <c r="DF49" s="21"/>
     </row>
     <row r="50" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="35"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="3" t="s">
         <v>171</v>
       </c>
@@ -8844,7 +8847,7 @@
       <c r="DF50" s="21"/>
     </row>
     <row r="51" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="35"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="3" t="s">
         <v>172</v>
       </c>
@@ -8958,7 +8961,7 @@
       <c r="DF51" s="21"/>
     </row>
     <row r="52" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="40"/>
+      <c r="A52" s="34"/>
       <c r="B52" s="3" t="s">
         <v>138</v>
       </c>
@@ -9072,7 +9075,7 @@
       <c r="DF52" s="21"/>
     </row>
     <row r="53" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="32" t="s">
         <v>81</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -9188,7 +9191,7 @@
       <c r="DF53" s="20"/>
     </row>
     <row r="54" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="38"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="2" t="s">
         <v>173</v>
       </c>
@@ -9302,7 +9305,7 @@
       <c r="DF54" s="20"/>
     </row>
     <row r="55" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="30" t="s">
         <v>82</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -9418,7 +9421,7 @@
       <c r="DF55" s="21"/>
     </row>
     <row r="56" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="35"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="3" t="s">
         <v>175</v>
       </c>
@@ -9532,7 +9535,7 @@
       <c r="DF56" s="21"/>
     </row>
     <row r="57" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="35"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="3" t="s">
         <v>176</v>
       </c>
@@ -9646,7 +9649,7 @@
       <c r="DF57" s="21"/>
     </row>
     <row r="58" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="35"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="3" t="s">
         <v>141</v>
       </c>
@@ -9760,7 +9763,7 @@
       <c r="DF58" s="21"/>
     </row>
     <row r="59" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="32" t="s">
         <v>83</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -9876,7 +9879,7 @@
       <c r="DF59" s="20"/>
     </row>
     <row r="60" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="38"/>
+      <c r="A60" s="33"/>
       <c r="B60" s="2" t="s">
         <v>178</v>
       </c>
@@ -9990,7 +9993,7 @@
       <c r="DF60" s="20"/>
     </row>
     <row r="61" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="38"/>
+      <c r="A61" s="33"/>
       <c r="B61" s="2" t="s">
         <v>179</v>
       </c>
@@ -10104,7 +10107,7 @@
       <c r="DF61" s="20"/>
     </row>
     <row r="62" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -10220,7 +10223,7 @@
       <c r="DF62" s="21"/>
     </row>
     <row r="63" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="35"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="3" t="s">
         <v>178</v>
       </c>
@@ -10334,7 +10337,7 @@
       <c r="DF63" s="21"/>
     </row>
     <row r="64" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="35"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="3" t="s">
         <v>177</v>
       </c>
@@ -10448,7 +10451,7 @@
       <c r="DF64" s="21"/>
     </row>
     <row r="65" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="35"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="3" t="s">
         <v>182</v>
       </c>
@@ -10562,7 +10565,7 @@
       <c r="DF65" s="21"/>
     </row>
     <row r="66" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="40"/>
+      <c r="A66" s="34"/>
       <c r="B66" s="3" t="s">
         <v>181</v>
       </c>
@@ -10676,7 +10679,7 @@
       <c r="DF66" s="21"/>
     </row>
     <row r="67" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="32" t="s">
         <v>85</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -10792,7 +10795,7 @@
       <c r="DF67" s="20"/>
     </row>
     <row r="68" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="38"/>
+      <c r="A68" s="33"/>
       <c r="B68" s="2" t="s">
         <v>183</v>
       </c>
@@ -10906,7 +10909,7 @@
       <c r="DF68" s="20"/>
     </row>
     <row r="69" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="30" t="s">
         <v>86</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -11022,7 +11025,7 @@
       <c r="DF69" s="21"/>
     </row>
     <row r="70" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="35"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="3" t="s">
         <v>174</v>
       </c>
@@ -11136,7 +11139,7 @@
       <c r="DF70" s="21"/>
     </row>
     <row r="71" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="35"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="3" t="s">
         <v>184</v>
       </c>
@@ -11250,7 +11253,7 @@
       <c r="DF71" s="21"/>
     </row>
     <row r="72" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="35"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="3" t="s">
         <v>185</v>
       </c>
@@ -11370,138 +11373,138 @@
       <c r="DF72" s="21"/>
     </row>
     <row r="73" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="35"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="27" t="s">
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="27" t="s">
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="28"/>
-      <c r="N73" s="28"/>
-      <c r="O73" s="28"/>
-      <c r="P73" s="28"/>
-      <c r="Q73" s="28"/>
-      <c r="R73" s="28"/>
-      <c r="S73" s="28"/>
-      <c r="T73" s="28"/>
-      <c r="U73" s="28"/>
-      <c r="V73" s="28"/>
-      <c r="W73" s="28"/>
-      <c r="X73" s="28"/>
-      <c r="Y73" s="27" t="s">
+      <c r="K73" s="29"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
+      <c r="O73" s="29"/>
+      <c r="P73" s="29"/>
+      <c r="Q73" s="29"/>
+      <c r="R73" s="29"/>
+      <c r="S73" s="29"/>
+      <c r="T73" s="29"/>
+      <c r="U73" s="29"/>
+      <c r="V73" s="29"/>
+      <c r="W73" s="29"/>
+      <c r="X73" s="29"/>
+      <c r="Y73" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z73" s="28"/>
-      <c r="AA73" s="28"/>
-      <c r="AB73" s="28"/>
-      <c r="AC73" s="28"/>
-      <c r="AD73" s="28"/>
-      <c r="AE73" s="28"/>
-      <c r="AF73" s="28"/>
-      <c r="AG73" s="28"/>
-      <c r="AH73" s="28"/>
-      <c r="AI73" s="28"/>
-      <c r="AJ73" s="28"/>
-      <c r="AK73" s="28"/>
-      <c r="AL73" s="28"/>
-      <c r="AM73" s="28"/>
-      <c r="AN73" s="28"/>
-      <c r="AO73" s="28"/>
-      <c r="AP73" s="28"/>
-      <c r="AQ73" s="29" t="s">
+      <c r="Z73" s="29"/>
+      <c r="AA73" s="29"/>
+      <c r="AB73" s="29"/>
+      <c r="AC73" s="29"/>
+      <c r="AD73" s="29"/>
+      <c r="AE73" s="29"/>
+      <c r="AF73" s="29"/>
+      <c r="AG73" s="29"/>
+      <c r="AH73" s="29"/>
+      <c r="AI73" s="29"/>
+      <c r="AJ73" s="29"/>
+      <c r="AK73" s="29"/>
+      <c r="AL73" s="29"/>
+      <c r="AM73" s="29"/>
+      <c r="AN73" s="29"/>
+      <c r="AO73" s="29"/>
+      <c r="AP73" s="29"/>
+      <c r="AQ73" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR73" s="30"/>
-      <c r="AS73" s="30"/>
-      <c r="AT73" s="30"/>
-      <c r="AU73" s="30"/>
-      <c r="AV73" s="30"/>
-      <c r="AW73" s="30"/>
-      <c r="AX73" s="30"/>
-      <c r="AY73" s="30"/>
-      <c r="AZ73" s="30"/>
-      <c r="BA73" s="31"/>
-      <c r="BB73" s="29" t="s">
+      <c r="AR73" s="46"/>
+      <c r="AS73" s="46"/>
+      <c r="AT73" s="46"/>
+      <c r="AU73" s="46"/>
+      <c r="AV73" s="46"/>
+      <c r="AW73" s="46"/>
+      <c r="AX73" s="46"/>
+      <c r="AY73" s="46"/>
+      <c r="AZ73" s="46"/>
+      <c r="BA73" s="47"/>
+      <c r="BB73" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC73" s="30"/>
-      <c r="BD73" s="30"/>
-      <c r="BE73" s="30"/>
-      <c r="BF73" s="30"/>
-      <c r="BG73" s="30"/>
-      <c r="BH73" s="30"/>
-      <c r="BI73" s="30"/>
-      <c r="BJ73" s="30"/>
-      <c r="BK73" s="30"/>
-      <c r="BL73" s="30"/>
-      <c r="BM73" s="30"/>
-      <c r="BN73" s="30"/>
-      <c r="BO73" s="30"/>
-      <c r="BP73" s="31"/>
-      <c r="BQ73" s="32" t="s">
+      <c r="BC73" s="46"/>
+      <c r="BD73" s="46"/>
+      <c r="BE73" s="46"/>
+      <c r="BF73" s="46"/>
+      <c r="BG73" s="46"/>
+      <c r="BH73" s="46"/>
+      <c r="BI73" s="46"/>
+      <c r="BJ73" s="46"/>
+      <c r="BK73" s="46"/>
+      <c r="BL73" s="46"/>
+      <c r="BM73" s="46"/>
+      <c r="BN73" s="46"/>
+      <c r="BO73" s="46"/>
+      <c r="BP73" s="47"/>
+      <c r="BQ73" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR73" s="33"/>
-      <c r="BS73" s="33"/>
-      <c r="BT73" s="33"/>
-      <c r="BU73" s="23" t="s">
+      <c r="BR73" s="49"/>
+      <c r="BS73" s="49"/>
+      <c r="BT73" s="49"/>
+      <c r="BU73" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV73" s="24"/>
-      <c r="BW73" s="24"/>
-      <c r="BX73" s="24"/>
-      <c r="BY73" s="24"/>
-      <c r="BZ73" s="24"/>
-      <c r="CA73" s="24"/>
-      <c r="CB73" s="24"/>
-      <c r="CC73" s="24"/>
-      <c r="CD73" s="24"/>
-      <c r="CE73" s="24"/>
-      <c r="CF73" s="24"/>
-      <c r="CG73" s="24"/>
-      <c r="CH73" s="24"/>
-      <c r="CI73" s="24"/>
-      <c r="CJ73" s="24"/>
-      <c r="CK73" s="24"/>
-      <c r="CL73" s="25"/>
-      <c r="CM73" s="23" t="s">
+      <c r="BV73" s="26"/>
+      <c r="BW73" s="26"/>
+      <c r="BX73" s="26"/>
+      <c r="BY73" s="26"/>
+      <c r="BZ73" s="26"/>
+      <c r="CA73" s="26"/>
+      <c r="CB73" s="26"/>
+      <c r="CC73" s="26"/>
+      <c r="CD73" s="26"/>
+      <c r="CE73" s="26"/>
+      <c r="CF73" s="26"/>
+      <c r="CG73" s="26"/>
+      <c r="CH73" s="26"/>
+      <c r="CI73" s="26"/>
+      <c r="CJ73" s="26"/>
+      <c r="CK73" s="26"/>
+      <c r="CL73" s="27"/>
+      <c r="CM73" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN73" s="24"/>
-      <c r="CO73" s="24"/>
-      <c r="CP73" s="24"/>
-      <c r="CQ73" s="24"/>
-      <c r="CR73" s="24"/>
-      <c r="CS73" s="24"/>
-      <c r="CT73" s="24"/>
-      <c r="CU73" s="24"/>
-      <c r="CV73" s="25"/>
-      <c r="CW73" s="23" t="s">
+      <c r="CN73" s="26"/>
+      <c r="CO73" s="26"/>
+      <c r="CP73" s="26"/>
+      <c r="CQ73" s="26"/>
+      <c r="CR73" s="26"/>
+      <c r="CS73" s="26"/>
+      <c r="CT73" s="26"/>
+      <c r="CU73" s="26"/>
+      <c r="CV73" s="27"/>
+      <c r="CW73" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX73" s="24"/>
-      <c r="CY73" s="24"/>
-      <c r="CZ73" s="24"/>
-      <c r="DA73" s="24"/>
-      <c r="DB73" s="24"/>
-      <c r="DC73" s="24"/>
-      <c r="DD73" s="24"/>
-      <c r="DE73" s="24"/>
-      <c r="DF73" s="25"/>
+      <c r="CX73" s="26"/>
+      <c r="CY73" s="26"/>
+      <c r="CZ73" s="26"/>
+      <c r="DA73" s="26"/>
+      <c r="DB73" s="26"/>
+      <c r="DC73" s="26"/>
+      <c r="DD73" s="26"/>
+      <c r="DE73" s="26"/>
+      <c r="DF73" s="27"/>
     </row>
     <row r="74" spans="1:110" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="22"/>
@@ -12166,7 +12169,7 @@
       </c>
     </row>
     <row r="76" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="51" t="s">
+      <c r="A76" s="40" t="s">
         <v>87</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -12286,7 +12289,7 @@
       <c r="DF76" s="21"/>
     </row>
     <row r="77" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="52"/>
+      <c r="A77" s="41"/>
       <c r="B77" s="3" t="s">
         <v>187</v>
       </c>
@@ -12400,7 +12403,7 @@
       <c r="DF77" s="21"/>
     </row>
     <row r="78" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="32" t="s">
         <v>88</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -12516,7 +12519,7 @@
       <c r="DF78" s="20"/>
     </row>
     <row r="79" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="38"/>
+      <c r="A79" s="33"/>
       <c r="B79" s="2" t="s">
         <v>188</v>
       </c>
@@ -12630,7 +12633,7 @@
       <c r="DF79" s="20"/>
     </row>
     <row r="80" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="38" t="s">
         <v>89</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -12718,8 +12721,12 @@
       <c r="BN80" s="21"/>
       <c r="BO80" s="21"/>
       <c r="BP80" s="21"/>
-      <c r="BQ80" s="21"/>
-      <c r="BR80" s="21"/>
+      <c r="BQ80" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR80" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="BS80" s="15"/>
       <c r="BT80" s="15"/>
       <c r="BU80" s="21"/>
@@ -12764,7 +12771,7 @@
       <c r="DF80" s="21"/>
     </row>
     <row r="81" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="42"/>
+      <c r="A81" s="39"/>
       <c r="B81" s="3" t="s">
         <v>190</v>
       </c>
@@ -12844,8 +12851,12 @@
       <c r="BN81" s="21"/>
       <c r="BO81" s="21"/>
       <c r="BP81" s="21"/>
-      <c r="BQ81" s="21"/>
-      <c r="BR81" s="21"/>
+      <c r="BQ81" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR81" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="BS81" s="15"/>
       <c r="BT81" s="15"/>
       <c r="BU81" s="21"/>
@@ -12890,7 +12901,7 @@
       <c r="DF81" s="21"/>
     </row>
     <row r="82" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="42"/>
+      <c r="A82" s="39"/>
       <c r="B82" s="3" t="s">
         <v>191</v>
       </c>
@@ -13008,7 +13019,7 @@
       <c r="DF82" s="21"/>
     </row>
     <row r="83" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="42"/>
+      <c r="A83" s="39"/>
       <c r="B83" s="3" t="s">
         <v>192</v>
       </c>
@@ -13128,7 +13139,7 @@
       <c r="DF83" s="21"/>
     </row>
     <row r="84" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="42"/>
+      <c r="A84" s="39"/>
       <c r="B84" s="3" t="s">
         <v>139</v>
       </c>
@@ -13242,7 +13253,7 @@
       <c r="DF84" s="21"/>
     </row>
     <row r="85" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="42"/>
+      <c r="A85" s="39"/>
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -13476,7 +13487,7 @@
       <c r="DF86" s="21"/>
     </row>
     <row r="87" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="37" t="s">
+      <c r="A87" s="32" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -13558,8 +13569,12 @@
       <c r="BN87" s="20"/>
       <c r="BO87" s="20"/>
       <c r="BP87" s="20"/>
-      <c r="BQ87" s="20"/>
-      <c r="BR87" s="20"/>
+      <c r="BQ87" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR87" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BS87" s="20"/>
       <c r="BT87" s="20"/>
       <c r="BU87" s="20"/>
@@ -13604,7 +13619,7 @@
       <c r="DF87" s="20"/>
     </row>
     <row r="88" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="38"/>
+      <c r="A88" s="33"/>
       <c r="B88" s="2" t="s">
         <v>189</v>
       </c>
@@ -13718,7 +13733,7 @@
       <c r="DF88" s="20"/>
     </row>
     <row r="89" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="38"/>
+      <c r="A89" s="33"/>
       <c r="B89" s="2" t="s">
         <v>141</v>
       </c>
@@ -13788,8 +13803,12 @@
       <c r="BN89" s="20"/>
       <c r="BO89" s="20"/>
       <c r="BP89" s="20"/>
-      <c r="BQ89" s="20"/>
-      <c r="BR89" s="20"/>
+      <c r="BQ89" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR89" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BS89" s="20"/>
       <c r="BT89" s="20"/>
       <c r="BU89" s="20"/>
@@ -13832,7 +13851,7 @@
       <c r="DF89" s="20"/>
     </row>
     <row r="90" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="38"/>
+      <c r="A90" s="33"/>
       <c r="B90" s="2" t="s">
         <v>142</v>
       </c>
@@ -13912,8 +13931,12 @@
       <c r="BN90" s="20"/>
       <c r="BO90" s="20"/>
       <c r="BP90" s="20"/>
-      <c r="BQ90" s="20"/>
-      <c r="BR90" s="20"/>
+      <c r="BQ90" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR90" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BS90" s="20"/>
       <c r="BT90" s="20"/>
       <c r="BU90" s="20"/>
@@ -13958,7 +13981,7 @@
       <c r="DF90" s="20"/>
     </row>
     <row r="91" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="34" t="s">
+      <c r="A91" s="30" t="s">
         <v>91</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -14076,7 +14099,7 @@
       <c r="DF91" s="21"/>
     </row>
     <row r="92" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="35"/>
+      <c r="A92" s="31"/>
       <c r="B92" s="3" t="s">
         <v>196</v>
       </c>
@@ -14192,7 +14215,7 @@
       <c r="DF92" s="21"/>
     </row>
     <row r="93" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="35"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="3" t="s">
         <v>197</v>
       </c>
@@ -14308,7 +14331,7 @@
       <c r="DF93" s="21"/>
     </row>
     <row r="94" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="35"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="3" t="s">
         <v>198</v>
       </c>
@@ -14422,7 +14445,7 @@
       <c r="DF94" s="21"/>
     </row>
     <row r="95" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="35"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="3" t="s">
         <v>199</v>
       </c>
@@ -14538,7 +14561,7 @@
       <c r="DF95" s="21"/>
     </row>
     <row r="96" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="40"/>
+      <c r="A96" s="34"/>
       <c r="B96" s="3" t="s">
         <v>189</v>
       </c>
@@ -14652,7 +14675,7 @@
       <c r="DF96" s="21"/>
     </row>
     <row r="97" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="37" t="s">
+      <c r="A97" s="32" t="s">
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -14774,7 +14797,7 @@
       <c r="DF97" s="20"/>
     </row>
     <row r="98" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="38"/>
+      <c r="A98" s="33"/>
       <c r="B98" s="2" t="s">
         <v>200</v>
       </c>
@@ -14894,7 +14917,7 @@
       <c r="DF98" s="20"/>
     </row>
     <row r="99" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="34" t="s">
+      <c r="A99" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -15030,7 +15053,7 @@
       <c r="DF99" s="21"/>
     </row>
     <row r="100" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="40"/>
+      <c r="A100" s="34"/>
       <c r="B100" s="3" t="s">
         <v>201</v>
       </c>
@@ -15164,7 +15187,7 @@
       <c r="DF100" s="21"/>
     </row>
     <row r="101" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="37" t="s">
+      <c r="A101" s="32" t="s">
         <v>94</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -15282,7 +15305,7 @@
       <c r="DF101" s="20"/>
     </row>
     <row r="102" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="38"/>
+      <c r="A102" s="33"/>
       <c r="B102" s="2" t="s">
         <v>202</v>
       </c>
@@ -15398,7 +15421,7 @@
       <c r="DF102" s="20"/>
     </row>
     <row r="103" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="38"/>
+      <c r="A103" s="33"/>
       <c r="B103" s="2" t="s">
         <v>203</v>
       </c>
@@ -15514,7 +15537,7 @@
       <c r="DF103" s="20"/>
     </row>
     <row r="104" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="34" t="s">
+      <c r="A104" s="30" t="s">
         <v>95</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -15640,7 +15663,7 @@
       <c r="DF104" s="21"/>
     </row>
     <row r="105" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="35"/>
+      <c r="A105" s="31"/>
       <c r="B105" s="3" t="s">
         <v>205</v>
       </c>
@@ -15764,7 +15787,7 @@
       <c r="DF105" s="21"/>
     </row>
     <row r="106" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="35"/>
+      <c r="A106" s="31"/>
       <c r="B106" s="3" t="s">
         <v>206</v>
       </c>
@@ -15882,7 +15905,7 @@
       <c r="DF106" s="21"/>
     </row>
     <row r="107" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="35"/>
+      <c r="A107" s="31"/>
       <c r="B107" s="3" t="s">
         <v>431</v>
       </c>
@@ -15996,7 +16019,7 @@
       <c r="DF107" s="21"/>
     </row>
     <row r="108" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="40"/>
+      <c r="A108" s="34"/>
       <c r="B108" s="3" t="s">
         <v>77</v>
       </c>
@@ -16110,7 +16133,7 @@
       <c r="DF108" s="21"/>
     </row>
     <row r="109" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="37" t="s">
+      <c r="A109" s="32" t="s">
         <v>96</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -16201,7 +16224,9 @@
       <c r="BQ109" s="20"/>
       <c r="BR109" s="20"/>
       <c r="BS109" s="20"/>
-      <c r="BT109" s="20"/>
+      <c r="BT109" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU109" s="20"/>
       <c r="BV109" s="20"/>
       <c r="BW109" s="20"/>
@@ -16250,7 +16275,7 @@
       <c r="DF109" s="20"/>
     </row>
     <row r="110" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="38"/>
+      <c r="A110" s="33"/>
       <c r="B110" s="2" t="s">
         <v>207</v>
       </c>
@@ -16345,7 +16370,9 @@
       <c r="BQ110" s="20"/>
       <c r="BR110" s="20"/>
       <c r="BS110" s="20"/>
-      <c r="BT110" s="20"/>
+      <c r="BT110" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU110" s="20"/>
       <c r="BV110" s="20"/>
       <c r="BW110" s="20"/>
@@ -16392,7 +16419,7 @@
       <c r="DF110" s="20"/>
     </row>
     <row r="111" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="38"/>
+      <c r="A111" s="33"/>
       <c r="B111" s="2" t="s">
         <v>208</v>
       </c>
@@ -16471,7 +16498,9 @@
       <c r="BQ111" s="20"/>
       <c r="BR111" s="20"/>
       <c r="BS111" s="20"/>
-      <c r="BT111" s="20"/>
+      <c r="BT111" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU111" s="20"/>
       <c r="BV111" s="20"/>
       <c r="BW111" s="20"/>
@@ -16514,7 +16543,7 @@
       <c r="DF111" s="20"/>
     </row>
     <row r="112" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="38"/>
+      <c r="A112" s="33"/>
       <c r="B112" s="2" t="s">
         <v>209</v>
       </c>
@@ -16603,7 +16632,9 @@
       <c r="BQ112" s="20"/>
       <c r="BR112" s="20"/>
       <c r="BS112" s="20"/>
-      <c r="BT112" s="20"/>
+      <c r="BT112" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU112" s="20"/>
       <c r="BV112" s="20"/>
       <c r="BW112" s="20"/>
@@ -16644,7 +16675,7 @@
       <c r="DF112" s="20"/>
     </row>
     <row r="113" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="38"/>
+      <c r="A113" s="33"/>
       <c r="B113" s="2" t="s">
         <v>210</v>
       </c>
@@ -16727,7 +16758,9 @@
       <c r="BQ113" s="20"/>
       <c r="BR113" s="20"/>
       <c r="BS113" s="20"/>
-      <c r="BT113" s="20"/>
+      <c r="BT113" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU113" s="20"/>
       <c r="BV113" s="20"/>
       <c r="BW113" s="20"/>
@@ -16770,7 +16803,7 @@
       <c r="DF113" s="20"/>
     </row>
     <row r="114" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="38"/>
+      <c r="A114" s="33"/>
       <c r="B114" s="2" t="s">
         <v>211</v>
       </c>
@@ -16847,7 +16880,9 @@
       <c r="BQ114" s="20"/>
       <c r="BR114" s="20"/>
       <c r="BS114" s="20"/>
-      <c r="BT114" s="20"/>
+      <c r="BT114" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU114" s="20"/>
       <c r="BV114" s="20"/>
       <c r="BW114" s="20"/>
@@ -16888,7 +16923,7 @@
       <c r="DF114" s="20"/>
     </row>
     <row r="115" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="34" t="s">
+      <c r="A115" s="30" t="s">
         <v>97</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -16963,7 +16998,9 @@
       <c r="BQ115" s="15"/>
       <c r="BR115" s="15"/>
       <c r="BS115" s="15"/>
-      <c r="BT115" s="15"/>
+      <c r="BT115" s="15" t="s">
+        <v>425</v>
+      </c>
       <c r="BU115" s="21"/>
       <c r="BV115" s="21"/>
       <c r="BW115" s="21"/>
@@ -17004,7 +17041,7 @@
       <c r="DF115" s="21"/>
     </row>
     <row r="116" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="35"/>
+      <c r="A116" s="31"/>
       <c r="B116" s="3" t="s">
         <v>213</v>
       </c>
@@ -17077,7 +17114,9 @@
       <c r="BQ116" s="15"/>
       <c r="BR116" s="15"/>
       <c r="BS116" s="15"/>
-      <c r="BT116" s="15"/>
+      <c r="BT116" s="15" t="s">
+        <v>425</v>
+      </c>
       <c r="BU116" s="21"/>
       <c r="BV116" s="21"/>
       <c r="BW116" s="21"/>
@@ -17118,7 +17157,7 @@
       <c r="DF116" s="21"/>
     </row>
     <row r="117" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="37" t="s">
+      <c r="A117" s="32" t="s">
         <v>98</v>
       </c>
       <c r="B117" s="2" t="s">
@@ -17195,7 +17234,9 @@
       <c r="BQ117" s="20"/>
       <c r="BR117" s="20"/>
       <c r="BS117" s="20"/>
-      <c r="BT117" s="20"/>
+      <c r="BT117" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU117" s="20"/>
       <c r="BV117" s="17"/>
       <c r="BW117" s="17"/>
@@ -17236,7 +17277,7 @@
       <c r="DF117" s="20"/>
     </row>
     <row r="118" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="38"/>
+      <c r="A118" s="33"/>
       <c r="B118" s="2" t="s">
         <v>204</v>
       </c>
@@ -17350,7 +17391,7 @@
       <c r="DF118" s="20"/>
     </row>
     <row r="119" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="38"/>
+      <c r="A119" s="33"/>
       <c r="B119" s="2" t="s">
         <v>141</v>
       </c>
@@ -17464,7 +17505,7 @@
       <c r="DF119" s="20"/>
     </row>
     <row r="120" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="38"/>
+      <c r="A120" s="33"/>
       <c r="B120" s="2" t="s">
         <v>214</v>
       </c>
@@ -17580,7 +17621,7 @@
       <c r="DF120" s="20"/>
     </row>
     <row r="121" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="41" t="s">
+      <c r="A121" s="38" t="s">
         <v>99</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -17698,7 +17739,7 @@
       <c r="DF121" s="21"/>
     </row>
     <row r="122" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="42"/>
+      <c r="A122" s="39"/>
       <c r="B122" s="3" t="s">
         <v>147</v>
       </c>
@@ -17812,7 +17853,7 @@
       <c r="DF122" s="21"/>
     </row>
     <row r="123" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="42"/>
+      <c r="A123" s="39"/>
       <c r="B123" s="3" t="s">
         <v>216</v>
       </c>
@@ -18042,7 +18083,7 @@
       <c r="DF124" s="21"/>
     </row>
     <row r="125" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="48" t="s">
+      <c r="A125" s="35" t="s">
         <v>100</v>
       </c>
       <c r="B125" s="2" t="s">
@@ -18123,7 +18164,9 @@
       <c r="BQ125" s="20"/>
       <c r="BR125" s="20"/>
       <c r="BS125" s="20"/>
-      <c r="BT125" s="20"/>
+      <c r="BT125" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU125" s="20"/>
       <c r="BV125" s="20"/>
       <c r="BW125" s="20"/>
@@ -18164,7 +18207,7 @@
       <c r="DF125" s="20"/>
     </row>
     <row r="126" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="49"/>
+      <c r="A126" s="36"/>
       <c r="B126" s="2" t="s">
         <v>217</v>
       </c>
@@ -18243,7 +18286,9 @@
       <c r="BQ126" s="20"/>
       <c r="BR126" s="20"/>
       <c r="BS126" s="20"/>
-      <c r="BT126" s="20"/>
+      <c r="BT126" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BU126" s="20"/>
       <c r="BV126" s="20"/>
       <c r="BW126" s="20"/>
@@ -18284,7 +18329,7 @@
       <c r="DF126" s="20"/>
     </row>
     <row r="127" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="50"/>
+      <c r="A127" s="37"/>
       <c r="B127" s="2" t="s">
         <v>212</v>
       </c>
@@ -18402,7 +18447,7 @@
       <c r="DF127" s="20"/>
     </row>
     <row r="128" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="41" t="s">
+      <c r="A128" s="38" t="s">
         <v>102</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -18520,7 +18565,7 @@
       <c r="DF128" s="21"/>
     </row>
     <row r="129" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="42"/>
+      <c r="A129" s="39"/>
       <c r="B129" s="3" t="s">
         <v>142</v>
       </c>
@@ -18636,7 +18681,7 @@
       <c r="DF129" s="21"/>
     </row>
     <row r="130" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="42"/>
+      <c r="A130" s="39"/>
       <c r="B130" s="3" t="s">
         <v>141</v>
       </c>
@@ -18868,7 +18913,7 @@
       <c r="DF131" s="21"/>
     </row>
     <row r="132" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="32" t="s">
         <v>101</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -18988,7 +19033,7 @@
       <c r="DF132" s="20"/>
     </row>
     <row r="133" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="38"/>
+      <c r="A133" s="33"/>
       <c r="B133" s="2" t="s">
         <v>221</v>
       </c>
@@ -19106,7 +19151,7 @@
       <c r="DF133" s="20"/>
     </row>
     <row r="134" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="34" t="s">
+      <c r="A134" s="30" t="s">
         <v>103</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -19224,7 +19269,9 @@
         <v>425</v>
       </c>
       <c r="CV134" s="21"/>
-      <c r="CW134" s="21"/>
+      <c r="CW134" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CX134" s="21"/>
       <c r="CY134" s="21"/>
       <c r="CZ134" s="21"/>
@@ -19236,7 +19283,7 @@
       <c r="DF134" s="21"/>
     </row>
     <row r="135" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="35"/>
+      <c r="A135" s="31"/>
       <c r="B135" s="3" t="s">
         <v>223</v>
       </c>
@@ -19344,7 +19391,9 @@
       <c r="CT135" s="21"/>
       <c r="CU135" s="21"/>
       <c r="CV135" s="21"/>
-      <c r="CW135" s="21"/>
+      <c r="CW135" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CX135" s="21"/>
       <c r="CY135" s="21"/>
       <c r="CZ135" s="21"/>
@@ -19356,7 +19405,7 @@
       <c r="DF135" s="21"/>
     </row>
     <row r="136" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="35"/>
+      <c r="A136" s="31"/>
       <c r="B136" s="3" t="s">
         <v>210</v>
       </c>
@@ -19468,7 +19517,9 @@
         <v>430</v>
       </c>
       <c r="CV136" s="21"/>
-      <c r="CW136" s="21"/>
+      <c r="CW136" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="CX136" s="21"/>
       <c r="CY136" s="21"/>
       <c r="CZ136" s="21"/>
@@ -19480,7 +19531,7 @@
       <c r="DF136" s="21"/>
     </row>
     <row r="137" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="35"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="3" t="s">
         <v>224</v>
       </c>
@@ -19586,7 +19637,9 @@
       <c r="CT137" s="21"/>
       <c r="CU137" s="21"/>
       <c r="CV137" s="21"/>
-      <c r="CW137" s="21"/>
+      <c r="CW137" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="CX137" s="21"/>
       <c r="CY137" s="21"/>
       <c r="CZ137" s="21"/>
@@ -19598,7 +19651,7 @@
       <c r="DF137" s="21"/>
     </row>
     <row r="138" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="35"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="3" t="s">
         <v>225</v>
       </c>
@@ -19716,7 +19769,7 @@
       <c r="DF138" s="21"/>
     </row>
     <row r="139" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="37" t="s">
+      <c r="A139" s="32" t="s">
         <v>104</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -19820,7 +19873,9 @@
       <c r="CT139" s="20"/>
       <c r="CU139" s="20"/>
       <c r="CV139" s="20"/>
-      <c r="CW139" s="20"/>
+      <c r="CW139" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CX139" s="20"/>
       <c r="CY139" s="20"/>
       <c r="CZ139" s="20"/>
@@ -19832,7 +19887,7 @@
       <c r="DF139" s="20"/>
     </row>
     <row r="140" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="38"/>
+      <c r="A140" s="33"/>
       <c r="B140" s="2" t="s">
         <v>227</v>
       </c>
@@ -19934,7 +19989,9 @@
       <c r="CT140" s="20"/>
       <c r="CU140" s="20"/>
       <c r="CV140" s="20"/>
-      <c r="CW140" s="20"/>
+      <c r="CW140" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CX140" s="20"/>
       <c r="CY140" s="20"/>
       <c r="CZ140" s="20"/>
@@ -19946,7 +20003,7 @@
       <c r="DF140" s="20"/>
     </row>
     <row r="141" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="38"/>
+      <c r="A141" s="33"/>
       <c r="B141" s="2" t="s">
         <v>228</v>
       </c>
@@ -20048,7 +20105,9 @@
       <c r="CT141" s="20"/>
       <c r="CU141" s="20"/>
       <c r="CV141" s="20"/>
-      <c r="CW141" s="20"/>
+      <c r="CW141" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CX141" s="20"/>
       <c r="CY141" s="20"/>
       <c r="CZ141" s="20"/>
@@ -20060,7 +20119,7 @@
       <c r="DF141" s="20"/>
     </row>
     <row r="142" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="38"/>
+      <c r="A142" s="33"/>
       <c r="B142" s="2" t="s">
         <v>229</v>
       </c>
@@ -20162,7 +20221,9 @@
       <c r="CT142" s="20"/>
       <c r="CU142" s="20"/>
       <c r="CV142" s="20"/>
-      <c r="CW142" s="20"/>
+      <c r="CW142" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CX142" s="20"/>
       <c r="CY142" s="20"/>
       <c r="CZ142" s="20"/>
@@ -20174,141 +20235,141 @@
       <c r="DF142" s="20"/>
     </row>
     <row r="143" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="44"/>
+      <c r="A143" s="23"/>
       <c r="B143" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="26" t="s">
+      <c r="C143" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D143" s="24"/>
-      <c r="E143" s="24"/>
-      <c r="F143" s="25"/>
-      <c r="G143" s="27" t="s">
+      <c r="D143" s="26"/>
+      <c r="E143" s="26"/>
+      <c r="F143" s="27"/>
+      <c r="G143" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H143" s="28"/>
-      <c r="I143" s="28"/>
-      <c r="J143" s="27" t="s">
+      <c r="H143" s="29"/>
+      <c r="I143" s="29"/>
+      <c r="J143" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K143" s="28"/>
-      <c r="L143" s="28"/>
-      <c r="M143" s="28"/>
-      <c r="N143" s="28"/>
-      <c r="O143" s="28"/>
-      <c r="P143" s="28"/>
-      <c r="Q143" s="28"/>
-      <c r="R143" s="28"/>
-      <c r="S143" s="28"/>
-      <c r="T143" s="28"/>
-      <c r="U143" s="28"/>
-      <c r="V143" s="28"/>
-      <c r="W143" s="28"/>
-      <c r="X143" s="28"/>
-      <c r="Y143" s="27" t="s">
+      <c r="K143" s="29"/>
+      <c r="L143" s="29"/>
+      <c r="M143" s="29"/>
+      <c r="N143" s="29"/>
+      <c r="O143" s="29"/>
+      <c r="P143" s="29"/>
+      <c r="Q143" s="29"/>
+      <c r="R143" s="29"/>
+      <c r="S143" s="29"/>
+      <c r="T143" s="29"/>
+      <c r="U143" s="29"/>
+      <c r="V143" s="29"/>
+      <c r="W143" s="29"/>
+      <c r="X143" s="29"/>
+      <c r="Y143" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z143" s="28"/>
-      <c r="AA143" s="28"/>
-      <c r="AB143" s="28"/>
-      <c r="AC143" s="28"/>
-      <c r="AD143" s="28"/>
-      <c r="AE143" s="28"/>
-      <c r="AF143" s="28"/>
-      <c r="AG143" s="28"/>
-      <c r="AH143" s="28"/>
-      <c r="AI143" s="28"/>
-      <c r="AJ143" s="28"/>
-      <c r="AK143" s="28"/>
-      <c r="AL143" s="28"/>
-      <c r="AM143" s="28"/>
-      <c r="AN143" s="28"/>
-      <c r="AO143" s="28"/>
-      <c r="AP143" s="28"/>
-      <c r="AQ143" s="29" t="s">
+      <c r="Z143" s="29"/>
+      <c r="AA143" s="29"/>
+      <c r="AB143" s="29"/>
+      <c r="AC143" s="29"/>
+      <c r="AD143" s="29"/>
+      <c r="AE143" s="29"/>
+      <c r="AF143" s="29"/>
+      <c r="AG143" s="29"/>
+      <c r="AH143" s="29"/>
+      <c r="AI143" s="29"/>
+      <c r="AJ143" s="29"/>
+      <c r="AK143" s="29"/>
+      <c r="AL143" s="29"/>
+      <c r="AM143" s="29"/>
+      <c r="AN143" s="29"/>
+      <c r="AO143" s="29"/>
+      <c r="AP143" s="29"/>
+      <c r="AQ143" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR143" s="30"/>
-      <c r="AS143" s="30"/>
-      <c r="AT143" s="30"/>
-      <c r="AU143" s="30"/>
-      <c r="AV143" s="30"/>
-      <c r="AW143" s="30"/>
-      <c r="AX143" s="30"/>
-      <c r="AY143" s="30"/>
-      <c r="AZ143" s="30"/>
-      <c r="BA143" s="31"/>
-      <c r="BB143" s="29" t="s">
+      <c r="AR143" s="46"/>
+      <c r="AS143" s="46"/>
+      <c r="AT143" s="46"/>
+      <c r="AU143" s="46"/>
+      <c r="AV143" s="46"/>
+      <c r="AW143" s="46"/>
+      <c r="AX143" s="46"/>
+      <c r="AY143" s="46"/>
+      <c r="AZ143" s="46"/>
+      <c r="BA143" s="47"/>
+      <c r="BB143" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC143" s="30"/>
-      <c r="BD143" s="30"/>
-      <c r="BE143" s="30"/>
-      <c r="BF143" s="30"/>
-      <c r="BG143" s="30"/>
-      <c r="BH143" s="30"/>
-      <c r="BI143" s="30"/>
-      <c r="BJ143" s="30"/>
-      <c r="BK143" s="30"/>
-      <c r="BL143" s="30"/>
-      <c r="BM143" s="30"/>
-      <c r="BN143" s="30"/>
-      <c r="BO143" s="30"/>
-      <c r="BP143" s="31"/>
-      <c r="BQ143" s="32" t="s">
+      <c r="BC143" s="46"/>
+      <c r="BD143" s="46"/>
+      <c r="BE143" s="46"/>
+      <c r="BF143" s="46"/>
+      <c r="BG143" s="46"/>
+      <c r="BH143" s="46"/>
+      <c r="BI143" s="46"/>
+      <c r="BJ143" s="46"/>
+      <c r="BK143" s="46"/>
+      <c r="BL143" s="46"/>
+      <c r="BM143" s="46"/>
+      <c r="BN143" s="46"/>
+      <c r="BO143" s="46"/>
+      <c r="BP143" s="47"/>
+      <c r="BQ143" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR143" s="33"/>
-      <c r="BS143" s="33"/>
-      <c r="BT143" s="33"/>
-      <c r="BU143" s="23" t="s">
+      <c r="BR143" s="49"/>
+      <c r="BS143" s="49"/>
+      <c r="BT143" s="49"/>
+      <c r="BU143" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV143" s="24"/>
-      <c r="BW143" s="24"/>
-      <c r="BX143" s="24"/>
-      <c r="BY143" s="24"/>
-      <c r="BZ143" s="24"/>
-      <c r="CA143" s="24"/>
-      <c r="CB143" s="24"/>
-      <c r="CC143" s="24"/>
-      <c r="CD143" s="24"/>
-      <c r="CE143" s="24"/>
-      <c r="CF143" s="24"/>
-      <c r="CG143" s="24"/>
-      <c r="CH143" s="24"/>
-      <c r="CI143" s="24"/>
-      <c r="CJ143" s="24"/>
-      <c r="CK143" s="24"/>
-      <c r="CL143" s="25"/>
-      <c r="CM143" s="23" t="s">
+      <c r="BV143" s="26"/>
+      <c r="BW143" s="26"/>
+      <c r="BX143" s="26"/>
+      <c r="BY143" s="26"/>
+      <c r="BZ143" s="26"/>
+      <c r="CA143" s="26"/>
+      <c r="CB143" s="26"/>
+      <c r="CC143" s="26"/>
+      <c r="CD143" s="26"/>
+      <c r="CE143" s="26"/>
+      <c r="CF143" s="26"/>
+      <c r="CG143" s="26"/>
+      <c r="CH143" s="26"/>
+      <c r="CI143" s="26"/>
+      <c r="CJ143" s="26"/>
+      <c r="CK143" s="26"/>
+      <c r="CL143" s="27"/>
+      <c r="CM143" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN143" s="24"/>
-      <c r="CO143" s="24"/>
-      <c r="CP143" s="24"/>
-      <c r="CQ143" s="24"/>
-      <c r="CR143" s="24"/>
-      <c r="CS143" s="24"/>
-      <c r="CT143" s="24"/>
-      <c r="CU143" s="24"/>
-      <c r="CV143" s="25"/>
-      <c r="CW143" s="23" t="s">
+      <c r="CN143" s="26"/>
+      <c r="CO143" s="26"/>
+      <c r="CP143" s="26"/>
+      <c r="CQ143" s="26"/>
+      <c r="CR143" s="26"/>
+      <c r="CS143" s="26"/>
+      <c r="CT143" s="26"/>
+      <c r="CU143" s="26"/>
+      <c r="CV143" s="27"/>
+      <c r="CW143" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX143" s="24"/>
-      <c r="CY143" s="24"/>
-      <c r="CZ143" s="24"/>
-      <c r="DA143" s="24"/>
-      <c r="DB143" s="24"/>
-      <c r="DC143" s="24"/>
-      <c r="DD143" s="24"/>
-      <c r="DE143" s="24"/>
-      <c r="DF143" s="25"/>
+      <c r="CX143" s="26"/>
+      <c r="CY143" s="26"/>
+      <c r="CZ143" s="26"/>
+      <c r="DA143" s="26"/>
+      <c r="DB143" s="26"/>
+      <c r="DC143" s="26"/>
+      <c r="DD143" s="26"/>
+      <c r="DE143" s="26"/>
+      <c r="DF143" s="27"/>
     </row>
     <row r="144" spans="1:110" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A144" s="45"/>
+      <c r="A144" s="24"/>
       <c r="B144" s="12" t="s">
         <v>2</v>
       </c>
@@ -20970,7 +21031,7 @@
       </c>
     </row>
     <row r="146" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="34" t="s">
+      <c r="A146" s="30" t="s">
         <v>105</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -21086,7 +21147,7 @@
       <c r="DF146" s="21"/>
     </row>
     <row r="147" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="35"/>
+      <c r="A147" s="31"/>
       <c r="B147" s="3" t="s">
         <v>127</v>
       </c>
@@ -21200,7 +21261,7 @@
       <c r="DF147" s="21"/>
     </row>
     <row r="148" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="37" t="s">
+      <c r="A148" s="32" t="s">
         <v>106</v>
       </c>
       <c r="B148" s="2" t="s">
@@ -21304,7 +21365,9 @@
       <c r="CT148" s="20"/>
       <c r="CU148" s="20"/>
       <c r="CV148" s="20"/>
-      <c r="CW148" s="20"/>
+      <c r="CW148" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CX148" s="20"/>
       <c r="CY148" s="20"/>
       <c r="CZ148" s="20"/>
@@ -21316,7 +21379,7 @@
       <c r="DF148" s="20"/>
     </row>
     <row r="149" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="38"/>
+      <c r="A149" s="33"/>
       <c r="B149" s="2" t="s">
         <v>142</v>
       </c>
@@ -21418,7 +21481,9 @@
       <c r="CT149" s="20"/>
       <c r="CU149" s="20"/>
       <c r="CV149" s="20"/>
-      <c r="CW149" s="20"/>
+      <c r="CW149" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="CX149" s="20"/>
       <c r="CY149" s="20"/>
       <c r="CZ149" s="20"/>
@@ -21430,7 +21495,7 @@
       <c r="DF149" s="20"/>
     </row>
     <row r="150" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="38"/>
+      <c r="A150" s="33"/>
       <c r="B150" s="2" t="s">
         <v>226</v>
       </c>
@@ -21544,7 +21609,7 @@
       <c r="DF150" s="20"/>
     </row>
     <row r="151" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="38"/>
+      <c r="A151" s="33"/>
       <c r="B151" s="2" t="s">
         <v>232</v>
       </c>
@@ -21658,7 +21723,7 @@
       <c r="DF151" s="20"/>
     </row>
     <row r="152" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="38"/>
+      <c r="A152" s="33"/>
       <c r="B152" s="2" t="s">
         <v>230</v>
       </c>
@@ -21772,7 +21837,7 @@
       <c r="DF152" s="20"/>
     </row>
     <row r="153" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="34" t="s">
+      <c r="A153" s="30" t="s">
         <v>107</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -21892,7 +21957,7 @@
       <c r="DF153" s="21"/>
     </row>
     <row r="154" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="35"/>
+      <c r="A154" s="31"/>
       <c r="B154" s="3" t="s">
         <v>77</v>
       </c>
@@ -22010,7 +22075,7 @@
       <c r="DF154" s="21"/>
     </row>
     <row r="155" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="35"/>
+      <c r="A155" s="31"/>
       <c r="B155" s="3" t="s">
         <v>220</v>
       </c>
@@ -22128,7 +22193,7 @@
       <c r="DF155" s="21"/>
     </row>
     <row r="156" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="37" t="s">
+      <c r="A156" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -22248,7 +22313,7 @@
       <c r="DF156" s="20"/>
     </row>
     <row r="157" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="38"/>
+      <c r="A157" s="33"/>
       <c r="B157" s="2" t="s">
         <v>139</v>
       </c>
@@ -22366,7 +22431,7 @@
       <c r="DF157" s="20"/>
     </row>
     <row r="158" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="38"/>
+      <c r="A158" s="33"/>
       <c r="B158" s="2" t="s">
         <v>189</v>
       </c>
@@ -22484,7 +22549,7 @@
       <c r="DF158" s="20"/>
     </row>
     <row r="159" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="39"/>
+      <c r="A159" s="42"/>
       <c r="B159" s="2" t="s">
         <v>233</v>
       </c>
@@ -22602,7 +22667,7 @@
       <c r="DF159" s="20"/>
     </row>
     <row r="160" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="34" t="s">
+      <c r="A160" s="30" t="s">
         <v>109</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -22722,7 +22787,7 @@
       <c r="DF160" s="21"/>
     </row>
     <row r="161" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="35"/>
+      <c r="A161" s="31"/>
       <c r="B161" s="3" t="s">
         <v>149</v>
       </c>
@@ -22838,7 +22903,7 @@
       <c r="DF161" s="21"/>
     </row>
     <row r="162" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="35"/>
+      <c r="A162" s="31"/>
       <c r="B162" s="3" t="s">
         <v>194</v>
       </c>
@@ -22954,7 +23019,7 @@
       <c r="DF162" s="21"/>
     </row>
     <row r="163" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="35"/>
+      <c r="A163" s="31"/>
       <c r="B163" s="3" t="s">
         <v>235</v>
       </c>
@@ -23072,7 +23137,7 @@
       <c r="DF163" s="21"/>
     </row>
     <row r="164" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="40"/>
+      <c r="A164" s="34"/>
       <c r="B164" s="3" t="s">
         <v>142</v>
       </c>
@@ -23190,7 +23255,7 @@
       <c r="DF164" s="21"/>
     </row>
     <row r="165" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="37" t="s">
+      <c r="A165" s="32" t="s">
         <v>110</v>
       </c>
       <c r="B165" s="2" t="s">
@@ -23308,7 +23373,7 @@
       <c r="DF165" s="20"/>
     </row>
     <row r="166" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="38"/>
+      <c r="A166" s="33"/>
       <c r="B166" s="2" t="s">
         <v>237</v>
       </c>
@@ -23424,7 +23489,7 @@
       <c r="DF166" s="20"/>
     </row>
     <row r="167" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="38"/>
+      <c r="A167" s="33"/>
       <c r="B167" s="2" t="s">
         <v>139</v>
       </c>
@@ -23540,7 +23605,7 @@
       <c r="DF167" s="20"/>
     </row>
     <row r="168" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="41" t="s">
+      <c r="A168" s="38" t="s">
         <v>111</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -23658,7 +23723,7 @@
       <c r="DF168" s="21"/>
     </row>
     <row r="169" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="42"/>
+      <c r="A169" s="39"/>
       <c r="B169" s="3" t="s">
         <v>239</v>
       </c>
@@ -23774,7 +23839,7 @@
       <c r="DF169" s="21"/>
     </row>
     <row r="170" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="42"/>
+      <c r="A170" s="39"/>
       <c r="B170" s="3" t="s">
         <v>236</v>
       </c>
@@ -24006,7 +24071,7 @@
       <c r="DF171" s="21"/>
     </row>
     <row r="172" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="37" t="s">
+      <c r="A172" s="32" t="s">
         <v>112</v>
       </c>
       <c r="B172" s="2" t="s">
@@ -24084,8 +24149,12 @@
       <c r="BN172" s="20"/>
       <c r="BO172" s="20"/>
       <c r="BP172" s="20"/>
-      <c r="BQ172" s="20"/>
-      <c r="BR172" s="20"/>
+      <c r="BQ172" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR172" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BS172" s="20"/>
       <c r="BT172" s="20"/>
       <c r="BU172" s="20"/>
@@ -24128,7 +24197,7 @@
       <c r="DF172" s="20"/>
     </row>
     <row r="173" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="38"/>
+      <c r="A173" s="33"/>
       <c r="B173" s="2" t="s">
         <v>247</v>
       </c>
@@ -24202,8 +24271,12 @@
       <c r="BN173" s="20"/>
       <c r="BO173" s="20"/>
       <c r="BP173" s="20"/>
-      <c r="BQ173" s="20"/>
-      <c r="BR173" s="20"/>
+      <c r="BQ173" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR173" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BS173" s="20"/>
       <c r="BT173" s="20"/>
       <c r="BU173" s="20"/>
@@ -24246,7 +24319,7 @@
       <c r="DF173" s="20"/>
     </row>
     <row r="174" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="38"/>
+      <c r="A174" s="33"/>
       <c r="B174" s="2" t="s">
         <v>219</v>
       </c>
@@ -24362,7 +24435,7 @@
       <c r="DF174" s="20"/>
     </row>
     <row r="175" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="34" t="s">
+      <c r="A175" s="30" t="s">
         <v>113</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -24440,8 +24513,12 @@
       <c r="BN175" s="21"/>
       <c r="BO175" s="21"/>
       <c r="BP175" s="21"/>
-      <c r="BQ175" s="15"/>
-      <c r="BR175" s="15"/>
+      <c r="BQ175" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR175" s="15" t="s">
+        <v>425</v>
+      </c>
       <c r="BS175" s="15"/>
       <c r="BT175" s="15"/>
       <c r="BU175" s="21"/>
@@ -24484,7 +24561,7 @@
       <c r="DF175" s="21"/>
     </row>
     <row r="176" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="35"/>
+      <c r="A176" s="31"/>
       <c r="B176" s="3" t="s">
         <v>245</v>
       </c>
@@ -24600,7 +24677,7 @@
       <c r="DF176" s="21"/>
     </row>
     <row r="177" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="35"/>
+      <c r="A177" s="31"/>
       <c r="B177" s="3" t="s">
         <v>141</v>
       </c>
@@ -24672,8 +24749,12 @@
       <c r="BN177" s="21"/>
       <c r="BO177" s="21"/>
       <c r="BP177" s="21"/>
-      <c r="BQ177" s="15"/>
-      <c r="BR177" s="15"/>
+      <c r="BQ177" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR177" s="15" t="s">
+        <v>425</v>
+      </c>
       <c r="BS177" s="15"/>
       <c r="BT177" s="15"/>
       <c r="BU177" s="21"/>
@@ -24716,7 +24797,7 @@
       <c r="DF177" s="21"/>
     </row>
     <row r="178" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A178" s="35"/>
+      <c r="A178" s="31"/>
       <c r="B178" s="3" t="s">
         <v>142</v>
       </c>
@@ -24790,8 +24871,12 @@
       <c r="BN178" s="21"/>
       <c r="BO178" s="21"/>
       <c r="BP178" s="21"/>
-      <c r="BQ178" s="15"/>
-      <c r="BR178" s="21"/>
+      <c r="BQ178" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="BR178" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="BS178" s="15"/>
       <c r="BT178" s="15"/>
       <c r="BU178" s="21"/>
@@ -24834,7 +24919,7 @@
       <c r="DF178" s="21"/>
     </row>
     <row r="179" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A179" s="37" t="s">
+      <c r="A179" s="32" t="s">
         <v>114</v>
       </c>
       <c r="B179" s="2" t="s">
@@ -24958,7 +25043,7 @@
       <c r="DF179" s="20"/>
     </row>
     <row r="180" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A180" s="38"/>
+      <c r="A180" s="33"/>
       <c r="B180" s="2" t="s">
         <v>242</v>
       </c>
@@ -25076,7 +25161,7 @@
       <c r="DF180" s="20"/>
     </row>
     <row r="181" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="38"/>
+      <c r="A181" s="33"/>
       <c r="B181" s="2" t="s">
         <v>243</v>
       </c>
@@ -25194,7 +25279,7 @@
       <c r="DF181" s="20"/>
     </row>
     <row r="182" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="38"/>
+      <c r="A182" s="33"/>
       <c r="B182" s="2" t="s">
         <v>244</v>
       </c>
@@ -25312,7 +25397,7 @@
       <c r="DF182" s="20"/>
     </row>
     <row r="183" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A183" s="39"/>
+      <c r="A183" s="42"/>
       <c r="B183" s="2" t="s">
         <v>245</v>
       </c>
@@ -25428,7 +25513,7 @@
       <c r="DF183" s="20"/>
     </row>
     <row r="184" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A184" s="41" t="s">
+      <c r="A184" s="38" t="s">
         <v>115</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -25670,7 +25755,7 @@
       <c r="DF185" s="21"/>
     </row>
     <row r="186" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="37" t="s">
+      <c r="A186" s="32" t="s">
         <v>116</v>
       </c>
       <c r="B186" s="2" t="s">
@@ -25728,9 +25813,15 @@
       <c r="AV186" s="20"/>
       <c r="AW186" s="20"/>
       <c r="AX186" s="20"/>
-      <c r="AY186" s="20"/>
-      <c r="AZ186" s="20"/>
-      <c r="BA186" s="20"/>
+      <c r="AY186" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="AZ186" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="BA186" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="BB186" s="20"/>
       <c r="BC186" s="20"/>
       <c r="BD186" s="20"/>
@@ -25790,7 +25881,7 @@
       <c r="DF186" s="20"/>
     </row>
     <row r="187" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="38"/>
+      <c r="A187" s="33"/>
       <c r="B187" s="2" t="s">
         <v>248</v>
       </c>
@@ -25842,9 +25933,15 @@
       <c r="AV187" s="20"/>
       <c r="AW187" s="20"/>
       <c r="AX187" s="20"/>
-      <c r="AY187" s="20"/>
-      <c r="AZ187" s="20"/>
-      <c r="BA187" s="20"/>
+      <c r="AY187" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="AZ187" s="20" t="s">
+        <v>430</v>
+      </c>
+      <c r="BA187" s="20" t="s">
+        <v>432</v>
+      </c>
       <c r="BB187" s="20"/>
       <c r="BC187" s="20"/>
       <c r="BD187" s="20"/>
@@ -25904,7 +26001,7 @@
       <c r="DF187" s="20"/>
     </row>
     <row r="188" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A188" s="34" t="s">
+      <c r="A188" s="30" t="s">
         <v>117</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -25962,8 +26059,12 @@
       <c r="AV188" s="21"/>
       <c r="AW188" s="21"/>
       <c r="AX188" s="21"/>
-      <c r="AY188" s="21"/>
-      <c r="AZ188" s="21"/>
+      <c r="AY188" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="AZ188" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="BA188" s="21"/>
       <c r="BB188" s="21"/>
       <c r="BC188" s="21"/>
@@ -26024,7 +26125,7 @@
       <c r="DF188" s="21"/>
     </row>
     <row r="189" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="35"/>
+      <c r="A189" s="31"/>
       <c r="B189" s="3" t="s">
         <v>162</v>
       </c>
@@ -26076,7 +26177,9 @@
       <c r="AV189" s="21"/>
       <c r="AW189" s="21"/>
       <c r="AX189" s="21"/>
-      <c r="AY189" s="21"/>
+      <c r="AY189" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="AZ189" s="21"/>
       <c r="BA189" s="21"/>
       <c r="BB189" s="21"/>
@@ -26138,7 +26241,7 @@
       <c r="DF189" s="21"/>
     </row>
     <row r="190" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="35"/>
+      <c r="A190" s="31"/>
       <c r="B190" s="3" t="s">
         <v>133</v>
       </c>
@@ -26190,8 +26293,12 @@
       <c r="AV190" s="21"/>
       <c r="AW190" s="21"/>
       <c r="AX190" s="21"/>
-      <c r="AY190" s="21"/>
-      <c r="AZ190" s="21"/>
+      <c r="AY190" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="AZ190" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="BA190" s="21"/>
       <c r="BB190" s="21"/>
       <c r="BC190" s="21"/>
@@ -26252,7 +26359,7 @@
       <c r="DF190" s="21"/>
     </row>
     <row r="191" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="46" t="s">
+      <c r="A191" s="50" t="s">
         <v>118</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -26310,8 +26417,12 @@
       <c r="AV191" s="20"/>
       <c r="AW191" s="20"/>
       <c r="AX191" s="20"/>
-      <c r="AY191" s="20"/>
-      <c r="AZ191" s="20"/>
+      <c r="AY191" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="AZ191" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BA191" s="20"/>
       <c r="BB191" s="20"/>
       <c r="BC191" s="20"/>
@@ -26372,7 +26483,7 @@
       <c r="DF191" s="20"/>
     </row>
     <row r="192" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="47"/>
+      <c r="A192" s="51"/>
       <c r="B192" s="2" t="s">
         <v>249</v>
       </c>
@@ -26424,7 +26535,9 @@
       <c r="AV192" s="20"/>
       <c r="AW192" s="20"/>
       <c r="AX192" s="20"/>
-      <c r="AY192" s="20"/>
+      <c r="AY192" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AZ192" s="20"/>
       <c r="BA192" s="20"/>
       <c r="BB192" s="20"/>
@@ -26486,7 +26599,7 @@
       <c r="DF192" s="20"/>
     </row>
     <row r="193" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="47"/>
+      <c r="A193" s="51"/>
       <c r="B193" s="2" t="s">
         <v>167</v>
       </c>
@@ -26538,7 +26651,9 @@
       <c r="AV193" s="20"/>
       <c r="AW193" s="20"/>
       <c r="AX193" s="20"/>
-      <c r="AY193" s="20"/>
+      <c r="AY193" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AZ193" s="20"/>
       <c r="BA193" s="20"/>
       <c r="BB193" s="20"/>
@@ -26600,141 +26715,141 @@
       <c r="DF193" s="20"/>
     </row>
     <row r="194" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="44"/>
+      <c r="A194" s="23"/>
       <c r="B194" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C194" s="26" t="s">
+      <c r="C194" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D194" s="24"/>
-      <c r="E194" s="24"/>
-      <c r="F194" s="25"/>
-      <c r="G194" s="27" t="s">
+      <c r="D194" s="26"/>
+      <c r="E194" s="26"/>
+      <c r="F194" s="27"/>
+      <c r="G194" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H194" s="28"/>
-      <c r="I194" s="28"/>
-      <c r="J194" s="27" t="s">
+      <c r="H194" s="29"/>
+      <c r="I194" s="29"/>
+      <c r="J194" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K194" s="28"/>
-      <c r="L194" s="28"/>
-      <c r="M194" s="28"/>
-      <c r="N194" s="28"/>
-      <c r="O194" s="28"/>
-      <c r="P194" s="28"/>
-      <c r="Q194" s="28"/>
-      <c r="R194" s="28"/>
-      <c r="S194" s="28"/>
-      <c r="T194" s="28"/>
-      <c r="U194" s="28"/>
-      <c r="V194" s="28"/>
-      <c r="W194" s="28"/>
-      <c r="X194" s="28"/>
-      <c r="Y194" s="27" t="s">
+      <c r="K194" s="29"/>
+      <c r="L194" s="29"/>
+      <c r="M194" s="29"/>
+      <c r="N194" s="29"/>
+      <c r="O194" s="29"/>
+      <c r="P194" s="29"/>
+      <c r="Q194" s="29"/>
+      <c r="R194" s="29"/>
+      <c r="S194" s="29"/>
+      <c r="T194" s="29"/>
+      <c r="U194" s="29"/>
+      <c r="V194" s="29"/>
+      <c r="W194" s="29"/>
+      <c r="X194" s="29"/>
+      <c r="Y194" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z194" s="28"/>
-      <c r="AA194" s="28"/>
-      <c r="AB194" s="28"/>
-      <c r="AC194" s="28"/>
-      <c r="AD194" s="28"/>
-      <c r="AE194" s="28"/>
-      <c r="AF194" s="28"/>
-      <c r="AG194" s="28"/>
-      <c r="AH194" s="28"/>
-      <c r="AI194" s="28"/>
-      <c r="AJ194" s="28"/>
-      <c r="AK194" s="28"/>
-      <c r="AL194" s="28"/>
-      <c r="AM194" s="28"/>
-      <c r="AN194" s="28"/>
-      <c r="AO194" s="28"/>
-      <c r="AP194" s="28"/>
-      <c r="AQ194" s="29" t="s">
+      <c r="Z194" s="29"/>
+      <c r="AA194" s="29"/>
+      <c r="AB194" s="29"/>
+      <c r="AC194" s="29"/>
+      <c r="AD194" s="29"/>
+      <c r="AE194" s="29"/>
+      <c r="AF194" s="29"/>
+      <c r="AG194" s="29"/>
+      <c r="AH194" s="29"/>
+      <c r="AI194" s="29"/>
+      <c r="AJ194" s="29"/>
+      <c r="AK194" s="29"/>
+      <c r="AL194" s="29"/>
+      <c r="AM194" s="29"/>
+      <c r="AN194" s="29"/>
+      <c r="AO194" s="29"/>
+      <c r="AP194" s="29"/>
+      <c r="AQ194" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR194" s="30"/>
-      <c r="AS194" s="30"/>
-      <c r="AT194" s="30"/>
-      <c r="AU194" s="30"/>
-      <c r="AV194" s="30"/>
-      <c r="AW194" s="30"/>
-      <c r="AX194" s="30"/>
-      <c r="AY194" s="30"/>
-      <c r="AZ194" s="30"/>
-      <c r="BA194" s="31"/>
-      <c r="BB194" s="29" t="s">
+      <c r="AR194" s="46"/>
+      <c r="AS194" s="46"/>
+      <c r="AT194" s="46"/>
+      <c r="AU194" s="46"/>
+      <c r="AV194" s="46"/>
+      <c r="AW194" s="46"/>
+      <c r="AX194" s="46"/>
+      <c r="AY194" s="46"/>
+      <c r="AZ194" s="46"/>
+      <c r="BA194" s="47"/>
+      <c r="BB194" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC194" s="30"/>
-      <c r="BD194" s="30"/>
-      <c r="BE194" s="30"/>
-      <c r="BF194" s="30"/>
-      <c r="BG194" s="30"/>
-      <c r="BH194" s="30"/>
-      <c r="BI194" s="30"/>
-      <c r="BJ194" s="30"/>
-      <c r="BK194" s="30"/>
-      <c r="BL194" s="30"/>
-      <c r="BM194" s="30"/>
-      <c r="BN194" s="30"/>
-      <c r="BO194" s="30"/>
-      <c r="BP194" s="31"/>
-      <c r="BQ194" s="32" t="s">
+      <c r="BC194" s="46"/>
+      <c r="BD194" s="46"/>
+      <c r="BE194" s="46"/>
+      <c r="BF194" s="46"/>
+      <c r="BG194" s="46"/>
+      <c r="BH194" s="46"/>
+      <c r="BI194" s="46"/>
+      <c r="BJ194" s="46"/>
+      <c r="BK194" s="46"/>
+      <c r="BL194" s="46"/>
+      <c r="BM194" s="46"/>
+      <c r="BN194" s="46"/>
+      <c r="BO194" s="46"/>
+      <c r="BP194" s="47"/>
+      <c r="BQ194" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR194" s="33"/>
-      <c r="BS194" s="33"/>
-      <c r="BT194" s="33"/>
-      <c r="BU194" s="23" t="s">
+      <c r="BR194" s="49"/>
+      <c r="BS194" s="49"/>
+      <c r="BT194" s="49"/>
+      <c r="BU194" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV194" s="24"/>
-      <c r="BW194" s="24"/>
-      <c r="BX194" s="24"/>
-      <c r="BY194" s="24"/>
-      <c r="BZ194" s="24"/>
-      <c r="CA194" s="24"/>
-      <c r="CB194" s="24"/>
-      <c r="CC194" s="24"/>
-      <c r="CD194" s="24"/>
-      <c r="CE194" s="24"/>
-      <c r="CF194" s="24"/>
-      <c r="CG194" s="24"/>
-      <c r="CH194" s="24"/>
-      <c r="CI194" s="24"/>
-      <c r="CJ194" s="24"/>
-      <c r="CK194" s="24"/>
-      <c r="CL194" s="25"/>
-      <c r="CM194" s="23" t="s">
+      <c r="BV194" s="26"/>
+      <c r="BW194" s="26"/>
+      <c r="BX194" s="26"/>
+      <c r="BY194" s="26"/>
+      <c r="BZ194" s="26"/>
+      <c r="CA194" s="26"/>
+      <c r="CB194" s="26"/>
+      <c r="CC194" s="26"/>
+      <c r="CD194" s="26"/>
+      <c r="CE194" s="26"/>
+      <c r="CF194" s="26"/>
+      <c r="CG194" s="26"/>
+      <c r="CH194" s="26"/>
+      <c r="CI194" s="26"/>
+      <c r="CJ194" s="26"/>
+      <c r="CK194" s="26"/>
+      <c r="CL194" s="27"/>
+      <c r="CM194" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN194" s="24"/>
-      <c r="CO194" s="24"/>
-      <c r="CP194" s="24"/>
-      <c r="CQ194" s="24"/>
-      <c r="CR194" s="24"/>
-      <c r="CS194" s="24"/>
-      <c r="CT194" s="24"/>
-      <c r="CU194" s="24"/>
-      <c r="CV194" s="25"/>
-      <c r="CW194" s="23" t="s">
+      <c r="CN194" s="26"/>
+      <c r="CO194" s="26"/>
+      <c r="CP194" s="26"/>
+      <c r="CQ194" s="26"/>
+      <c r="CR194" s="26"/>
+      <c r="CS194" s="26"/>
+      <c r="CT194" s="26"/>
+      <c r="CU194" s="26"/>
+      <c r="CV194" s="27"/>
+      <c r="CW194" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX194" s="24"/>
-      <c r="CY194" s="24"/>
-      <c r="CZ194" s="24"/>
-      <c r="DA194" s="24"/>
-      <c r="DB194" s="24"/>
-      <c r="DC194" s="24"/>
-      <c r="DD194" s="24"/>
-      <c r="DE194" s="24"/>
-      <c r="DF194" s="25"/>
+      <c r="CX194" s="26"/>
+      <c r="CY194" s="26"/>
+      <c r="CZ194" s="26"/>
+      <c r="DA194" s="26"/>
+      <c r="DB194" s="26"/>
+      <c r="DC194" s="26"/>
+      <c r="DD194" s="26"/>
+      <c r="DE194" s="26"/>
+      <c r="DF194" s="27"/>
     </row>
     <row r="195" spans="1:110" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="45"/>
+      <c r="A195" s="24"/>
       <c r="B195" s="12" t="s">
         <v>2</v>
       </c>
@@ -27396,7 +27511,7 @@
       </c>
     </row>
     <row r="197" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="37" t="s">
+      <c r="A197" s="32" t="s">
         <v>119</v>
       </c>
       <c r="B197" s="2" t="s">
@@ -27452,8 +27567,12 @@
       <c r="AV197" s="20"/>
       <c r="AW197" s="20"/>
       <c r="AX197" s="20"/>
-      <c r="AY197" s="20"/>
-      <c r="AZ197" s="20"/>
+      <c r="AY197" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="AZ197" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="BA197" s="20"/>
       <c r="BB197" s="20"/>
       <c r="BC197" s="20"/>
@@ -27514,7 +27633,7 @@
       <c r="DF197" s="20"/>
     </row>
     <row r="198" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="38"/>
+      <c r="A198" s="33"/>
       <c r="B198" s="2" t="s">
         <v>250</v>
       </c>
@@ -27568,8 +27687,12 @@
       <c r="AV198" s="20"/>
       <c r="AW198" s="20"/>
       <c r="AX198" s="20"/>
-      <c r="AY198" s="20"/>
-      <c r="AZ198" s="20"/>
+      <c r="AY198" s="20" t="s">
+        <v>425</v>
+      </c>
+      <c r="AZ198" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="BA198" s="20"/>
       <c r="BB198" s="20"/>
       <c r="BC198" s="20"/>
@@ -27630,7 +27753,7 @@
       <c r="DF198" s="20"/>
     </row>
     <row r="199" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="34" t="s">
+      <c r="A199" s="30" t="s">
         <v>120</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -27748,7 +27871,7 @@
       <c r="DF199" s="21"/>
     </row>
     <row r="200" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="35"/>
+      <c r="A200" s="31"/>
       <c r="B200" s="3" t="s">
         <v>251</v>
       </c>
@@ -27866,7 +27989,7 @@
       <c r="DF200" s="21"/>
     </row>
     <row r="201" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="37" t="s">
+      <c r="A201" s="32" t="s">
         <v>121</v>
       </c>
       <c r="B201" s="2" t="s">
@@ -27986,7 +28109,7 @@
       <c r="DF201" s="20"/>
     </row>
     <row r="202" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="38"/>
+      <c r="A202" s="33"/>
       <c r="B202" s="2" t="s">
         <v>182</v>
       </c>
@@ -28104,7 +28227,7 @@
       <c r="DF202" s="20"/>
     </row>
     <row r="203" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="38"/>
+      <c r="A203" s="33"/>
       <c r="B203" s="2" t="s">
         <v>181</v>
       </c>
@@ -28222,7 +28345,7 @@
       <c r="DF203" s="20"/>
     </row>
     <row r="204" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="34" t="s">
+      <c r="A204" s="30" t="s">
         <v>122</v>
       </c>
       <c r="B204" s="3" t="s">
@@ -28346,7 +28469,7 @@
       <c r="DF204" s="21"/>
     </row>
     <row r="205" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="35"/>
+      <c r="A205" s="31"/>
       <c r="B205" s="3" t="s">
         <v>253</v>
       </c>
@@ -28468,7 +28591,7 @@
       <c r="DF205" s="21"/>
     </row>
     <row r="206" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="35"/>
+      <c r="A206" s="31"/>
       <c r="B206" s="3" t="s">
         <v>254</v>
       </c>
@@ -28588,7 +28711,7 @@
       <c r="DF206" s="21"/>
     </row>
     <row r="207" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A207" s="35"/>
+      <c r="A207" s="31"/>
       <c r="B207" s="3" t="s">
         <v>255</v>
       </c>
@@ -28708,7 +28831,7 @@
       <c r="DF207" s="21"/>
     </row>
     <row r="208" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A208" s="37" t="s">
+      <c r="A208" s="32" t="s">
         <v>123</v>
       </c>
       <c r="B208" s="2" t="s">
@@ -28832,7 +28955,7 @@
       <c r="DF208" s="20"/>
     </row>
     <row r="209" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="38"/>
+      <c r="A209" s="33"/>
       <c r="B209" s="2" t="s">
         <v>257</v>
       </c>
@@ -28952,7 +29075,7 @@
       <c r="DF209" s="20"/>
     </row>
     <row r="210" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="38"/>
+      <c r="A210" s="33"/>
       <c r="B210" s="2" t="s">
         <v>258</v>
       </c>
@@ -29068,7 +29191,7 @@
       <c r="DF210" s="20"/>
     </row>
     <row r="211" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="34" t="s">
+      <c r="A211" s="30" t="s">
         <v>124</v>
       </c>
       <c r="B211" s="3" t="s">
@@ -29192,7 +29315,7 @@
       <c r="DF211" s="21"/>
     </row>
     <row r="212" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="35"/>
+      <c r="A212" s="31"/>
       <c r="B212" s="3" t="s">
         <v>256</v>
       </c>
@@ -29308,7 +29431,7 @@
       <c r="DF212" s="21"/>
     </row>
     <row r="213" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="35"/>
+      <c r="A213" s="31"/>
       <c r="B213" s="3" t="s">
         <v>142</v>
       </c>
@@ -29428,7 +29551,7 @@
       <c r="DF213" s="21"/>
     </row>
     <row r="214" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="35"/>
+      <c r="A214" s="31"/>
       <c r="B214" s="3" t="s">
         <v>141</v>
       </c>
@@ -29542,7 +29665,7 @@
       <c r="DF214" s="21"/>
     </row>
     <row r="215" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="35"/>
+      <c r="A215" s="31"/>
       <c r="B215" s="3" t="s">
         <v>222</v>
       </c>
@@ -29656,7 +29779,7 @@
       <c r="DF215" s="21"/>
     </row>
     <row r="216" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="37" t="s">
+      <c r="A216" s="32" t="s">
         <v>125</v>
       </c>
       <c r="B216" s="2" t="s">
@@ -29772,7 +29895,7 @@
       <c r="DF216" s="20"/>
     </row>
     <row r="217" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A217" s="38"/>
+      <c r="A217" s="33"/>
       <c r="B217" s="2" t="s">
         <v>260</v>
       </c>
@@ -29886,7 +30009,7 @@
       <c r="DF217" s="20"/>
     </row>
     <row r="218" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A218" s="34" t="s">
+      <c r="A218" s="30" t="s">
         <v>126</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -30002,7 +30125,7 @@
       <c r="DF218" s="21"/>
     </row>
     <row r="219" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" s="35"/>
+      <c r="A219" s="31"/>
       <c r="B219" s="3" t="s">
         <v>272</v>
       </c>
@@ -30116,7 +30239,7 @@
       <c r="DF219" s="21"/>
     </row>
     <row r="220" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A220" s="35"/>
+      <c r="A220" s="31"/>
       <c r="B220" s="3" t="s">
         <v>273</v>
       </c>
@@ -30230,7 +30353,7 @@
       <c r="DF220" s="21"/>
     </row>
     <row r="221" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A221" s="37" t="s">
+      <c r="A221" s="32" t="s">
         <v>127</v>
       </c>
       <c r="B221" s="2" t="s">
@@ -30334,7 +30457,9 @@
       <c r="CT221" s="20"/>
       <c r="CU221" s="20"/>
       <c r="CV221" s="20"/>
-      <c r="CW221" s="20"/>
+      <c r="CW221" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="CX221" s="20"/>
       <c r="CY221" s="20"/>
       <c r="CZ221" s="20"/>
@@ -30346,7 +30471,7 @@
       <c r="DF221" s="20"/>
     </row>
     <row r="222" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A222" s="38"/>
+      <c r="A222" s="33"/>
       <c r="B222" s="2" t="s">
         <v>271</v>
       </c>
@@ -30448,7 +30573,9 @@
       <c r="CT222" s="20"/>
       <c r="CU222" s="20"/>
       <c r="CV222" s="20"/>
-      <c r="CW222" s="20"/>
+      <c r="CW222" s="20" t="s">
+        <v>435</v>
+      </c>
       <c r="CX222" s="20"/>
       <c r="CY222" s="20"/>
       <c r="CZ222" s="20"/>
@@ -30460,7 +30587,7 @@
       <c r="DF222" s="20"/>
     </row>
     <row r="223" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A223" s="34" t="s">
+      <c r="A223" s="30" t="s">
         <v>128</v>
       </c>
       <c r="B223" s="3" t="s">
@@ -30578,7 +30705,7 @@
       <c r="DF223" s="21"/>
     </row>
     <row r="224" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A224" s="35"/>
+      <c r="A224" s="31"/>
       <c r="B224" s="3" t="s">
         <v>269</v>
       </c>
@@ -30698,7 +30825,7 @@
       <c r="DF224" s="21"/>
     </row>
     <row r="225" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A225" s="35"/>
+      <c r="A225" s="31"/>
       <c r="B225" s="3" t="s">
         <v>270</v>
       </c>
@@ -30816,7 +30943,7 @@
       <c r="DF225" s="21"/>
     </row>
     <row r="226" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A226" s="35"/>
+      <c r="A226" s="31"/>
       <c r="B226" s="3" t="s">
         <v>266</v>
       </c>
@@ -30934,7 +31061,7 @@
       <c r="DF226" s="21"/>
     </row>
     <row r="227" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A227" s="37" t="s">
+      <c r="A227" s="32" t="s">
         <v>129</v>
       </c>
       <c r="B227" s="2" t="s">
@@ -31050,7 +31177,7 @@
       <c r="DF227" s="20"/>
     </row>
     <row r="228" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A228" s="38"/>
+      <c r="A228" s="33"/>
       <c r="B228" s="2" t="s">
         <v>267</v>
       </c>
@@ -31164,7 +31291,7 @@
       <c r="DF228" s="20"/>
     </row>
     <row r="229" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A229" s="38"/>
+      <c r="A229" s="33"/>
       <c r="B229" s="2" t="s">
         <v>268</v>
       </c>
@@ -31278,7 +31405,7 @@
       <c r="DF229" s="20"/>
     </row>
     <row r="230" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A230" s="34" t="s">
+      <c r="A230" s="30" t="s">
         <v>130</v>
       </c>
       <c r="B230" s="3" t="s">
@@ -31394,7 +31521,7 @@
       <c r="DF230" s="21"/>
     </row>
     <row r="231" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A231" s="35"/>
+      <c r="A231" s="31"/>
       <c r="B231" s="3" t="s">
         <v>262</v>
       </c>
@@ -31508,7 +31635,7 @@
       <c r="DF231" s="21"/>
     </row>
     <row r="232" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="35"/>
+      <c r="A232" s="31"/>
       <c r="B232" s="3" t="s">
         <v>263</v>
       </c>
@@ -31622,7 +31749,7 @@
       <c r="DF232" s="21"/>
     </row>
     <row r="233" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A233" s="37" t="s">
+      <c r="A233" s="32" t="s">
         <v>131</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -31744,7 +31871,7 @@
       <c r="DF233" s="20"/>
     </row>
     <row r="234" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A234" s="38"/>
+      <c r="A234" s="33"/>
       <c r="B234" s="2" t="s">
         <v>139</v>
       </c>
@@ -31860,7 +31987,7 @@
       <c r="DF234" s="20"/>
     </row>
     <row r="235" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A235" s="34" t="s">
+      <c r="A235" s="30" t="s">
         <v>132</v>
       </c>
       <c r="B235" s="3" t="s">
@@ -31982,7 +32109,7 @@
       <c r="DF235" s="21"/>
     </row>
     <row r="236" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A236" s="35"/>
+      <c r="A236" s="31"/>
       <c r="B236" s="3" t="s">
         <v>141</v>
       </c>
@@ -32100,7 +32227,7 @@
       <c r="DF236" s="21"/>
     </row>
     <row r="237" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A237" s="35"/>
+      <c r="A237" s="31"/>
       <c r="B237" s="3" t="s">
         <v>264</v>
       </c>
@@ -32216,7 +32343,7 @@
       <c r="DF237" s="21"/>
     </row>
     <row r="238" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A238" s="36"/>
+      <c r="A238" s="52"/>
       <c r="B238" s="3" t="s">
         <v>142</v>
       </c>
@@ -32335,50 +32462,45 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:X1"/>
-    <mergeCell ref="Y1:AP1"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A139:A142"/>
-    <mergeCell ref="C143:F143"/>
-    <mergeCell ref="G143:I143"/>
-    <mergeCell ref="J143:X143"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="CW1:DF1"/>
+    <mergeCell ref="CW143:DF143"/>
+    <mergeCell ref="CW194:DF194"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="J73:X73"/>
+    <mergeCell ref="Y73:AP73"/>
+    <mergeCell ref="AQ73:BA73"/>
+    <mergeCell ref="BB73:BP73"/>
+    <mergeCell ref="BQ73:BT73"/>
+    <mergeCell ref="BU73:CL73"/>
+    <mergeCell ref="CM73:CV73"/>
+    <mergeCell ref="CW73:DF73"/>
+    <mergeCell ref="CM194:CV194"/>
+    <mergeCell ref="AQ1:BA1"/>
+    <mergeCell ref="BB1:BP1"/>
+    <mergeCell ref="BQ1:BT1"/>
+    <mergeCell ref="BU1:CL1"/>
+    <mergeCell ref="CM1:CV1"/>
+    <mergeCell ref="BU194:CL194"/>
+    <mergeCell ref="A235:A238"/>
+    <mergeCell ref="A221:A222"/>
+    <mergeCell ref="A223:A226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="A230:A232"/>
+    <mergeCell ref="A233:A234"/>
+    <mergeCell ref="A208:A210"/>
+    <mergeCell ref="A211:A215"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="A218:A220"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A199:A200"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A204:A207"/>
+    <mergeCell ref="Y194:AP194"/>
+    <mergeCell ref="AQ194:BA194"/>
+    <mergeCell ref="BB194:BP194"/>
+    <mergeCell ref="BQ194:BT194"/>
     <mergeCell ref="A156:A159"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A165:A167"/>
@@ -32403,45 +32525,50 @@
     <mergeCell ref="A179:A183"/>
     <mergeCell ref="A184:A185"/>
     <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A199:A200"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A204:A207"/>
-    <mergeCell ref="Y194:AP194"/>
-    <mergeCell ref="AQ194:BA194"/>
-    <mergeCell ref="BB194:BP194"/>
-    <mergeCell ref="BQ194:BT194"/>
-    <mergeCell ref="A235:A238"/>
-    <mergeCell ref="A221:A222"/>
-    <mergeCell ref="A223:A226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="A230:A232"/>
-    <mergeCell ref="A233:A234"/>
-    <mergeCell ref="A208:A210"/>
-    <mergeCell ref="A211:A215"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="A218:A220"/>
-    <mergeCell ref="CW1:DF1"/>
-    <mergeCell ref="CW143:DF143"/>
-    <mergeCell ref="CW194:DF194"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="J73:X73"/>
-    <mergeCell ref="Y73:AP73"/>
-    <mergeCell ref="AQ73:BA73"/>
-    <mergeCell ref="BB73:BP73"/>
-    <mergeCell ref="BQ73:BT73"/>
-    <mergeCell ref="BU73:CL73"/>
-    <mergeCell ref="CM73:CV73"/>
-    <mergeCell ref="CW73:DF73"/>
-    <mergeCell ref="CM194:CV194"/>
-    <mergeCell ref="AQ1:BA1"/>
-    <mergeCell ref="BB1:BP1"/>
-    <mergeCell ref="BQ1:BT1"/>
-    <mergeCell ref="BU1:CL1"/>
-    <mergeCell ref="CM1:CV1"/>
-    <mergeCell ref="BU194:CL194"/>
+    <mergeCell ref="A139:A142"/>
+    <mergeCell ref="C143:F143"/>
+    <mergeCell ref="G143:I143"/>
+    <mergeCell ref="J143:X143"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:X1"/>
+    <mergeCell ref="Y1:AP1"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
4.1 - 4.8 CRUD Matrix
</commit_message>
<xml_diff>
--- a/Documentation/Team 3  - Del 6 CRUD Matrix.xlsx
+++ b/Documentation/Team 3  - Del 6 CRUD Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Team-3-Orion\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chase\INF370\Team-3-Orion\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7499C7-9A87-4D09-BF5A-5D80B4E89812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50F010B-25E6-4FDE-8C04-A8EF69B1E605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="438">
   <si>
     <r>
       <rPr>
@@ -2095,7 +2095,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2104,14 +2110,56 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -2128,61 +2176,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2525,11 +2525,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DF238"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="CX49" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="AP190" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DE79" sqref="DE79"/>
+      <selection pane="bottomRight" activeCell="AX193" sqref="AX193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="6" x14ac:dyDescent="0.2"/>
@@ -2563,7 +2563,9 @@
     <col min="43" max="43" width="2.5" style="19" customWidth="1"/>
     <col min="44" max="45" width="2.1640625" style="19" customWidth="1"/>
     <col min="46" max="46" width="1.5" style="19" customWidth="1"/>
-    <col min="47" max="52" width="2.1640625" style="19" customWidth="1"/>
+    <col min="47" max="48" width="2.1640625" style="19" customWidth="1"/>
+    <col min="49" max="49" width="3" style="19" customWidth="1"/>
+    <col min="50" max="52" width="2.1640625" style="19" customWidth="1"/>
     <col min="53" max="53" width="2.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="54" max="55" width="2.1640625" style="19" customWidth="1"/>
     <col min="56" max="56" width="2.33203125" style="19" bestFit="1" customWidth="1"/>
@@ -2589,141 +2591,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
+      <c r="A1" s="23"/>
       <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="27" t="s">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="27" t="s">
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K1" s="28"/>
-      <c r="L1" s="28"/>
-      <c r="M1" s="28"/>
-      <c r="N1" s="28"/>
-      <c r="O1" s="28"/>
-      <c r="P1" s="28"/>
-      <c r="Q1" s="28"/>
-      <c r="R1" s="28"/>
-      <c r="S1" s="28"/>
-      <c r="T1" s="28"/>
-      <c r="U1" s="28"/>
-      <c r="V1" s="28"/>
-      <c r="W1" s="28"/>
-      <c r="X1" s="28"/>
-      <c r="Y1" s="27" t="s">
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z1" s="28"/>
-      <c r="AA1" s="28"/>
-      <c r="AB1" s="28"/>
-      <c r="AC1" s="28"/>
-      <c r="AD1" s="28"/>
-      <c r="AE1" s="28"/>
-      <c r="AF1" s="28"/>
-      <c r="AG1" s="28"/>
-      <c r="AH1" s="28"/>
-      <c r="AI1" s="28"/>
-      <c r="AJ1" s="28"/>
-      <c r="AK1" s="28"/>
-      <c r="AL1" s="28"/>
-      <c r="AM1" s="28"/>
-      <c r="AN1" s="28"/>
-      <c r="AO1" s="28"/>
-      <c r="AP1" s="28"/>
-      <c r="AQ1" s="29" t="s">
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR1" s="30"/>
-      <c r="AS1" s="30"/>
-      <c r="AT1" s="30"/>
-      <c r="AU1" s="30"/>
-      <c r="AV1" s="30"/>
-      <c r="AW1" s="30"/>
-      <c r="AX1" s="30"/>
-      <c r="AY1" s="30"/>
-      <c r="AZ1" s="30"/>
-      <c r="BA1" s="31"/>
-      <c r="BB1" s="29" t="s">
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
+      <c r="AY1" s="46"/>
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="47"/>
+      <c r="BB1" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30"/>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30"/>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
-      <c r="BN1" s="30"/>
-      <c r="BO1" s="30"/>
-      <c r="BP1" s="31"/>
-      <c r="BQ1" s="32" t="s">
+      <c r="BC1" s="46"/>
+      <c r="BD1" s="46"/>
+      <c r="BE1" s="46"/>
+      <c r="BF1" s="46"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="47"/>
+      <c r="BQ1" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR1" s="33"/>
-      <c r="BS1" s="33"/>
-      <c r="BT1" s="33"/>
-      <c r="BU1" s="23" t="s">
+      <c r="BR1" s="49"/>
+      <c r="BS1" s="49"/>
+      <c r="BT1" s="49"/>
+      <c r="BU1" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV1" s="24"/>
-      <c r="BW1" s="24"/>
-      <c r="BX1" s="24"/>
-      <c r="BY1" s="24"/>
-      <c r="BZ1" s="24"/>
-      <c r="CA1" s="24"/>
-      <c r="CB1" s="24"/>
-      <c r="CC1" s="24"/>
-      <c r="CD1" s="24"/>
-      <c r="CE1" s="24"/>
-      <c r="CF1" s="24"/>
-      <c r="CG1" s="24"/>
-      <c r="CH1" s="24"/>
-      <c r="CI1" s="24"/>
-      <c r="CJ1" s="24"/>
-      <c r="CK1" s="24"/>
-      <c r="CL1" s="25"/>
-      <c r="CM1" s="23" t="s">
+      <c r="BV1" s="26"/>
+      <c r="BW1" s="26"/>
+      <c r="BX1" s="26"/>
+      <c r="BY1" s="26"/>
+      <c r="BZ1" s="26"/>
+      <c r="CA1" s="26"/>
+      <c r="CB1" s="26"/>
+      <c r="CC1" s="26"/>
+      <c r="CD1" s="26"/>
+      <c r="CE1" s="26"/>
+      <c r="CF1" s="26"/>
+      <c r="CG1" s="26"/>
+      <c r="CH1" s="26"/>
+      <c r="CI1" s="26"/>
+      <c r="CJ1" s="26"/>
+      <c r="CK1" s="26"/>
+      <c r="CL1" s="27"/>
+      <c r="CM1" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN1" s="24"/>
-      <c r="CO1" s="24"/>
-      <c r="CP1" s="24"/>
-      <c r="CQ1" s="24"/>
-      <c r="CR1" s="24"/>
-      <c r="CS1" s="24"/>
-      <c r="CT1" s="24"/>
-      <c r="CU1" s="24"/>
-      <c r="CV1" s="25"/>
-      <c r="CW1" s="23" t="s">
+      <c r="CN1" s="26"/>
+      <c r="CO1" s="26"/>
+      <c r="CP1" s="26"/>
+      <c r="CQ1" s="26"/>
+      <c r="CR1" s="26"/>
+      <c r="CS1" s="26"/>
+      <c r="CT1" s="26"/>
+      <c r="CU1" s="26"/>
+      <c r="CV1" s="27"/>
+      <c r="CW1" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX1" s="24"/>
-      <c r="CY1" s="24"/>
-      <c r="CZ1" s="24"/>
-      <c r="DA1" s="24"/>
-      <c r="DB1" s="24"/>
-      <c r="DC1" s="24"/>
-      <c r="DD1" s="24"/>
-      <c r="DE1" s="24"/>
-      <c r="DF1" s="25"/>
+      <c r="CX1" s="26"/>
+      <c r="CY1" s="26"/>
+      <c r="CZ1" s="26"/>
+      <c r="DA1" s="26"/>
+      <c r="DB1" s="26"/>
+      <c r="DC1" s="26"/>
+      <c r="DD1" s="26"/>
+      <c r="DE1" s="26"/>
+      <c r="DF1" s="27"/>
     </row>
     <row r="2" spans="1:110" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A2" s="45"/>
+      <c r="A2" s="24"/>
       <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
@@ -3385,7 +3387,7 @@
       </c>
     </row>
     <row r="4" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="35" t="s">
         <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3505,7 +3507,7 @@
       <c r="DF4" s="20"/>
     </row>
     <row r="5" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="49"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="2" t="s">
         <v>134</v>
       </c>
@@ -3623,7 +3625,7 @@
       <c r="DF5" s="20"/>
     </row>
     <row r="6" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="49"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="2" t="s">
         <v>135</v>
       </c>
@@ -3737,7 +3739,7 @@
       <c r="DF6" s="20"/>
     </row>
     <row r="7" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="50"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="2" t="s">
         <v>136</v>
       </c>
@@ -3851,7 +3853,7 @@
       <c r="DF7" s="20"/>
     </row>
     <row r="8" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="30" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="3" t="s">
@@ -3971,7 +3973,7 @@
       <c r="DF8" s="21"/>
     </row>
     <row r="9" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="35"/>
+      <c r="A9" s="31"/>
       <c r="B9" s="3" t="s">
         <v>138</v>
       </c>
@@ -4085,7 +4087,7 @@
       <c r="DF9" s="21"/>
     </row>
     <row r="10" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="35"/>
+      <c r="A10" s="31"/>
       <c r="B10" s="3" t="s">
         <v>139</v>
       </c>
@@ -4199,7 +4201,7 @@
       <c r="DF10" s="21"/>
     </row>
     <row r="11" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="32" t="s">
         <v>71</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -4321,7 +4323,7 @@
       <c r="DF11" s="20"/>
     </row>
     <row r="12" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="38"/>
+      <c r="A12" s="33"/>
       <c r="B12" s="2" t="s">
         <v>137</v>
       </c>
@@ -4437,7 +4439,7 @@
       <c r="DF12" s="20"/>
     </row>
     <row r="13" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="38"/>
+      <c r="A13" s="33"/>
       <c r="B13" s="2" t="s">
         <v>141</v>
       </c>
@@ -4553,7 +4555,7 @@
       <c r="DF13" s="20"/>
     </row>
     <row r="14" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="38"/>
+      <c r="A14" s="33"/>
       <c r="B14" s="2" t="s">
         <v>142</v>
       </c>
@@ -4671,7 +4673,7 @@
       <c r="DF14" s="20"/>
     </row>
     <row r="15" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="38" t="s">
         <v>72</v>
       </c>
       <c r="B15" s="3" t="s">
@@ -4721,8 +4723,12 @@
       <c r="AR15" s="21"/>
       <c r="AS15" s="21"/>
       <c r="AT15" s="21"/>
-      <c r="AU15" s="21"/>
-      <c r="AV15" s="21"/>
+      <c r="AU15" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="AV15" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AW15" s="21"/>
       <c r="AX15" s="21"/>
       <c r="AY15" s="21"/>
@@ -4787,7 +4793,7 @@
       <c r="DF15" s="21"/>
     </row>
     <row r="16" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="42"/>
+      <c r="A16" s="39"/>
       <c r="B16" s="3" t="s">
         <v>144</v>
       </c>
@@ -4835,8 +4841,12 @@
       <c r="AR16" s="21"/>
       <c r="AS16" s="21"/>
       <c r="AT16" s="21"/>
-      <c r="AU16" s="21"/>
-      <c r="AV16" s="21"/>
+      <c r="AU16" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="AV16" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AW16" s="21"/>
       <c r="AX16" s="21"/>
       <c r="AY16" s="21"/>
@@ -4901,7 +4911,7 @@
       <c r="DF16" s="21"/>
     </row>
     <row r="17" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="42"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="3" t="s">
         <v>133</v>
       </c>
@@ -4949,8 +4959,12 @@
       <c r="AR17" s="21"/>
       <c r="AS17" s="21"/>
       <c r="AT17" s="21"/>
-      <c r="AU17" s="21"/>
-      <c r="AV17" s="21"/>
+      <c r="AU17" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="AV17" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AW17" s="21"/>
       <c r="AX17" s="21"/>
       <c r="AY17" s="21"/>
@@ -5015,7 +5029,7 @@
       <c r="DF17" s="21"/>
     </row>
     <row r="18" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="32" t="s">
         <v>73</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -5137,7 +5151,7 @@
       <c r="DF18" s="20"/>
     </row>
     <row r="19" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="38"/>
+      <c r="A19" s="33"/>
       <c r="B19" s="2" t="s">
         <v>146</v>
       </c>
@@ -5257,7 +5271,7 @@
       <c r="DF19" s="20"/>
     </row>
     <row r="20" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="38"/>
+      <c r="A20" s="33"/>
       <c r="B20" s="2" t="s">
         <v>147</v>
       </c>
@@ -5371,7 +5385,7 @@
       <c r="DF20" s="20"/>
     </row>
     <row r="21" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="34" t="s">
+      <c r="A21" s="30" t="s">
         <v>74</v>
       </c>
       <c r="B21" s="3" t="s">
@@ -5487,7 +5501,7 @@
       <c r="DF21" s="21"/>
     </row>
     <row r="22" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="35"/>
+      <c r="A22" s="31"/>
       <c r="B22" s="3" t="s">
         <v>139</v>
       </c>
@@ -5601,7 +5615,7 @@
       <c r="DF22" s="21"/>
     </row>
     <row r="23" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="35"/>
+      <c r="A23" s="31"/>
       <c r="B23" s="3" t="s">
         <v>149</v>
       </c>
@@ -5715,7 +5729,7 @@
       <c r="DF23" s="21"/>
     </row>
     <row r="24" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="32" t="s">
         <v>75</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -5839,7 +5853,7 @@
       <c r="DF24" s="20"/>
     </row>
     <row r="25" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="38"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="2" t="s">
         <v>151</v>
       </c>
@@ -5959,7 +5973,7 @@
       <c r="DF25" s="20"/>
     </row>
     <row r="26" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="38"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="2" t="s">
         <v>152</v>
       </c>
@@ -6079,7 +6093,7 @@
       <c r="DF26" s="20"/>
     </row>
     <row r="27" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="38"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="2" t="s">
         <v>153</v>
       </c>
@@ -6197,7 +6211,7 @@
       <c r="DF27" s="20"/>
     </row>
     <row r="28" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="38"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="2" t="s">
         <v>154</v>
       </c>
@@ -6315,7 +6329,7 @@
       <c r="DF28" s="20"/>
     </row>
     <row r="29" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="38"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="2" t="s">
         <v>155</v>
       </c>
@@ -6433,7 +6447,7 @@
       <c r="DF29" s="20"/>
     </row>
     <row r="30" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="38"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="2" t="s">
         <v>156</v>
       </c>
@@ -6551,7 +6565,7 @@
       <c r="DF30" s="20"/>
     </row>
     <row r="31" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="38"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="2" t="s">
         <v>150</v>
       </c>
@@ -6669,7 +6683,7 @@
       <c r="DF31" s="20"/>
     </row>
     <row r="32" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="38"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="2" t="s">
         <v>138</v>
       </c>
@@ -6783,7 +6797,7 @@
       <c r="DF32" s="20"/>
     </row>
     <row r="33" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="34" t="s">
+      <c r="A33" s="30" t="s">
         <v>76</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -6899,7 +6913,7 @@
       <c r="DF33" s="21"/>
     </row>
     <row r="34" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="35"/>
+      <c r="A34" s="31"/>
       <c r="B34" s="3" t="s">
         <v>157</v>
       </c>
@@ -7013,7 +7027,7 @@
       <c r="DF34" s="21"/>
     </row>
     <row r="35" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="40"/>
+      <c r="A35" s="34"/>
       <c r="B35" s="3" t="s">
         <v>158</v>
       </c>
@@ -7127,7 +7141,7 @@
       <c r="DF35" s="21"/>
     </row>
     <row r="36" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="37" t="s">
+      <c r="A36" s="32" t="s">
         <v>77</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -7247,7 +7261,7 @@
       <c r="DF36" s="18"/>
     </row>
     <row r="37" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="38"/>
+      <c r="A37" s="33"/>
       <c r="B37" s="2" t="s">
         <v>160</v>
       </c>
@@ -7365,7 +7379,7 @@
       <c r="DF37" s="18"/>
     </row>
     <row r="38" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="30" t="s">
         <v>78</v>
       </c>
       <c r="B38" s="3" t="s">
@@ -7485,7 +7499,7 @@
       </c>
     </row>
     <row r="39" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="35"/>
+      <c r="A39" s="31"/>
       <c r="B39" s="3" t="s">
         <v>162</v>
       </c>
@@ -7603,7 +7617,7 @@
       </c>
     </row>
     <row r="40" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="35"/>
+      <c r="A40" s="31"/>
       <c r="B40" s="3" t="s">
         <v>163</v>
       </c>
@@ -7721,7 +7735,7 @@
       </c>
     </row>
     <row r="41" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="35"/>
+      <c r="A41" s="31"/>
       <c r="B41" s="3" t="s">
         <v>159</v>
       </c>
@@ -7839,7 +7853,7 @@
       </c>
     </row>
     <row r="42" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="37" t="s">
+      <c r="A42" s="32" t="s">
         <v>79</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -7955,7 +7969,7 @@
       <c r="DF42" s="20"/>
     </row>
     <row r="43" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="38"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="2" t="s">
         <v>164</v>
       </c>
@@ -8069,7 +8083,7 @@
       <c r="DF43" s="20"/>
     </row>
     <row r="44" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="38"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="2" t="s">
         <v>165</v>
       </c>
@@ -8183,7 +8197,7 @@
       <c r="DF44" s="20"/>
     </row>
     <row r="45" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="39"/>
+      <c r="A45" s="42"/>
       <c r="B45" s="2" t="s">
         <v>166</v>
       </c>
@@ -8297,7 +8311,7 @@
       <c r="DF45" s="20"/>
     </row>
     <row r="46" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="30" t="s">
         <v>80</v>
       </c>
       <c r="B46" s="3" t="s">
@@ -8417,7 +8431,7 @@
       </c>
     </row>
     <row r="47" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="35"/>
+      <c r="A47" s="31"/>
       <c r="B47" s="3" t="s">
         <v>168</v>
       </c>
@@ -8531,7 +8545,7 @@
       <c r="DF47" s="21"/>
     </row>
     <row r="48" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="35"/>
+      <c r="A48" s="31"/>
       <c r="B48" s="3" t="s">
         <v>169</v>
       </c>
@@ -8645,7 +8659,7 @@
       <c r="DF48" s="21"/>
     </row>
     <row r="49" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="35"/>
+      <c r="A49" s="31"/>
       <c r="B49" s="3" t="s">
         <v>170</v>
       </c>
@@ -8759,7 +8773,7 @@
       <c r="DF49" s="21"/>
     </row>
     <row r="50" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="35"/>
+      <c r="A50" s="31"/>
       <c r="B50" s="3" t="s">
         <v>171</v>
       </c>
@@ -8873,7 +8887,7 @@
       <c r="DF50" s="21"/>
     </row>
     <row r="51" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="35"/>
+      <c r="A51" s="31"/>
       <c r="B51" s="3" t="s">
         <v>172</v>
       </c>
@@ -8987,7 +9001,7 @@
       <c r="DF51" s="21"/>
     </row>
     <row r="52" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A52" s="40"/>
+      <c r="A52" s="34"/>
       <c r="B52" s="3" t="s">
         <v>138</v>
       </c>
@@ -9101,7 +9115,7 @@
       <c r="DF52" s="21"/>
     </row>
     <row r="53" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A53" s="37" t="s">
+      <c r="A53" s="32" t="s">
         <v>81</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -9217,7 +9231,7 @@
       <c r="DF53" s="20"/>
     </row>
     <row r="54" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A54" s="38"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="2" t="s">
         <v>173</v>
       </c>
@@ -9331,7 +9345,7 @@
       <c r="DF54" s="20"/>
     </row>
     <row r="55" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A55" s="34" t="s">
+      <c r="A55" s="30" t="s">
         <v>82</v>
       </c>
       <c r="B55" s="3" t="s">
@@ -9459,7 +9473,7 @@
       </c>
     </row>
     <row r="56" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="35"/>
+      <c r="A56" s="31"/>
       <c r="B56" s="3" t="s">
         <v>175</v>
       </c>
@@ -9585,7 +9599,7 @@
       </c>
     </row>
     <row r="57" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A57" s="35"/>
+      <c r="A57" s="31"/>
       <c r="B57" s="3" t="s">
         <v>176</v>
       </c>
@@ -9711,7 +9725,7 @@
       </c>
     </row>
     <row r="58" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="35"/>
+      <c r="A58" s="31"/>
       <c r="B58" s="3" t="s">
         <v>141</v>
       </c>
@@ -9837,7 +9851,7 @@
       </c>
     </row>
     <row r="59" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="37" t="s">
+      <c r="A59" s="32" t="s">
         <v>83</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -9953,7 +9967,7 @@
       <c r="DF59" s="20"/>
     </row>
     <row r="60" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="38"/>
+      <c r="A60" s="33"/>
       <c r="B60" s="2" t="s">
         <v>178</v>
       </c>
@@ -10067,7 +10081,7 @@
       <c r="DF60" s="20"/>
     </row>
     <row r="61" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="38"/>
+      <c r="A61" s="33"/>
       <c r="B61" s="2" t="s">
         <v>179</v>
       </c>
@@ -10181,7 +10195,7 @@
       <c r="DF61" s="20"/>
     </row>
     <row r="62" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A62" s="34" t="s">
+      <c r="A62" s="30" t="s">
         <v>84</v>
       </c>
       <c r="B62" s="3" t="s">
@@ -10297,7 +10311,7 @@
       <c r="DF62" s="21"/>
     </row>
     <row r="63" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="35"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="3" t="s">
         <v>178</v>
       </c>
@@ -10411,7 +10425,7 @@
       <c r="DF63" s="21"/>
     </row>
     <row r="64" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="35"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="3" t="s">
         <v>177</v>
       </c>
@@ -10525,7 +10539,7 @@
       <c r="DF64" s="21"/>
     </row>
     <row r="65" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="35"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="3" t="s">
         <v>182</v>
       </c>
@@ -10639,7 +10653,7 @@
       <c r="DF65" s="21"/>
     </row>
     <row r="66" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="40"/>
+      <c r="A66" s="34"/>
       <c r="B66" s="3" t="s">
         <v>181</v>
       </c>
@@ -10753,7 +10767,7 @@
       <c r="DF66" s="21"/>
     </row>
     <row r="67" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A67" s="37" t="s">
+      <c r="A67" s="32" t="s">
         <v>85</v>
       </c>
       <c r="B67" s="2" t="s">
@@ -10873,7 +10887,7 @@
       </c>
     </row>
     <row r="68" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="38"/>
+      <c r="A68" s="33"/>
       <c r="B68" s="2" t="s">
         <v>183</v>
       </c>
@@ -10991,7 +11005,7 @@
       </c>
     </row>
     <row r="69" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="34" t="s">
+      <c r="A69" s="30" t="s">
         <v>86</v>
       </c>
       <c r="B69" s="3" t="s">
@@ -11111,7 +11125,7 @@
       </c>
     </row>
     <row r="70" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="35"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="3" t="s">
         <v>174</v>
       </c>
@@ -11229,7 +11243,7 @@
       </c>
     </row>
     <row r="71" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="35"/>
+      <c r="A71" s="31"/>
       <c r="B71" s="3" t="s">
         <v>184</v>
       </c>
@@ -11347,7 +11361,7 @@
       </c>
     </row>
     <row r="72" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="35"/>
+      <c r="A72" s="31"/>
       <c r="B72" s="3" t="s">
         <v>185</v>
       </c>
@@ -11471,138 +11485,138 @@
       </c>
     </row>
     <row r="73" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="35"/>
+      <c r="A73" s="31"/>
       <c r="B73" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="26" t="s">
+      <c r="C73" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="25"/>
-      <c r="G73" s="27" t="s">
+      <c r="D73" s="26"/>
+      <c r="E73" s="26"/>
+      <c r="F73" s="27"/>
+      <c r="G73" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H73" s="28"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="27" t="s">
+      <c r="H73" s="29"/>
+      <c r="I73" s="29"/>
+      <c r="J73" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K73" s="28"/>
-      <c r="L73" s="28"/>
-      <c r="M73" s="28"/>
-      <c r="N73" s="28"/>
-      <c r="O73" s="28"/>
-      <c r="P73" s="28"/>
-      <c r="Q73" s="28"/>
-      <c r="R73" s="28"/>
-      <c r="S73" s="28"/>
-      <c r="T73" s="28"/>
-      <c r="U73" s="28"/>
-      <c r="V73" s="28"/>
-      <c r="W73" s="28"/>
-      <c r="X73" s="28"/>
-      <c r="Y73" s="27" t="s">
+      <c r="K73" s="29"/>
+      <c r="L73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="29"/>
+      <c r="O73" s="29"/>
+      <c r="P73" s="29"/>
+      <c r="Q73" s="29"/>
+      <c r="R73" s="29"/>
+      <c r="S73" s="29"/>
+      <c r="T73" s="29"/>
+      <c r="U73" s="29"/>
+      <c r="V73" s="29"/>
+      <c r="W73" s="29"/>
+      <c r="X73" s="29"/>
+      <c r="Y73" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z73" s="28"/>
-      <c r="AA73" s="28"/>
-      <c r="AB73" s="28"/>
-      <c r="AC73" s="28"/>
-      <c r="AD73" s="28"/>
-      <c r="AE73" s="28"/>
-      <c r="AF73" s="28"/>
-      <c r="AG73" s="28"/>
-      <c r="AH73" s="28"/>
-      <c r="AI73" s="28"/>
-      <c r="AJ73" s="28"/>
-      <c r="AK73" s="28"/>
-      <c r="AL73" s="28"/>
-      <c r="AM73" s="28"/>
-      <c r="AN73" s="28"/>
-      <c r="AO73" s="28"/>
-      <c r="AP73" s="28"/>
-      <c r="AQ73" s="29" t="s">
+      <c r="Z73" s="29"/>
+      <c r="AA73" s="29"/>
+      <c r="AB73" s="29"/>
+      <c r="AC73" s="29"/>
+      <c r="AD73" s="29"/>
+      <c r="AE73" s="29"/>
+      <c r="AF73" s="29"/>
+      <c r="AG73" s="29"/>
+      <c r="AH73" s="29"/>
+      <c r="AI73" s="29"/>
+      <c r="AJ73" s="29"/>
+      <c r="AK73" s="29"/>
+      <c r="AL73" s="29"/>
+      <c r="AM73" s="29"/>
+      <c r="AN73" s="29"/>
+      <c r="AO73" s="29"/>
+      <c r="AP73" s="29"/>
+      <c r="AQ73" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR73" s="30"/>
-      <c r="AS73" s="30"/>
-      <c r="AT73" s="30"/>
-      <c r="AU73" s="30"/>
-      <c r="AV73" s="30"/>
-      <c r="AW73" s="30"/>
-      <c r="AX73" s="30"/>
-      <c r="AY73" s="30"/>
-      <c r="AZ73" s="30"/>
-      <c r="BA73" s="31"/>
-      <c r="BB73" s="29" t="s">
+      <c r="AR73" s="46"/>
+      <c r="AS73" s="46"/>
+      <c r="AT73" s="46"/>
+      <c r="AU73" s="46"/>
+      <c r="AV73" s="46"/>
+      <c r="AW73" s="46"/>
+      <c r="AX73" s="46"/>
+      <c r="AY73" s="46"/>
+      <c r="AZ73" s="46"/>
+      <c r="BA73" s="47"/>
+      <c r="BB73" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC73" s="30"/>
-      <c r="BD73" s="30"/>
-      <c r="BE73" s="30"/>
-      <c r="BF73" s="30"/>
-      <c r="BG73" s="30"/>
-      <c r="BH73" s="30"/>
-      <c r="BI73" s="30"/>
-      <c r="BJ73" s="30"/>
-      <c r="BK73" s="30"/>
-      <c r="BL73" s="30"/>
-      <c r="BM73" s="30"/>
-      <c r="BN73" s="30"/>
-      <c r="BO73" s="30"/>
-      <c r="BP73" s="31"/>
-      <c r="BQ73" s="32" t="s">
+      <c r="BC73" s="46"/>
+      <c r="BD73" s="46"/>
+      <c r="BE73" s="46"/>
+      <c r="BF73" s="46"/>
+      <c r="BG73" s="46"/>
+      <c r="BH73" s="46"/>
+      <c r="BI73" s="46"/>
+      <c r="BJ73" s="46"/>
+      <c r="BK73" s="46"/>
+      <c r="BL73" s="46"/>
+      <c r="BM73" s="46"/>
+      <c r="BN73" s="46"/>
+      <c r="BO73" s="46"/>
+      <c r="BP73" s="47"/>
+      <c r="BQ73" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR73" s="33"/>
-      <c r="BS73" s="33"/>
-      <c r="BT73" s="33"/>
-      <c r="BU73" s="23" t="s">
+      <c r="BR73" s="49"/>
+      <c r="BS73" s="49"/>
+      <c r="BT73" s="49"/>
+      <c r="BU73" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV73" s="24"/>
-      <c r="BW73" s="24"/>
-      <c r="BX73" s="24"/>
-      <c r="BY73" s="24"/>
-      <c r="BZ73" s="24"/>
-      <c r="CA73" s="24"/>
-      <c r="CB73" s="24"/>
-      <c r="CC73" s="24"/>
-      <c r="CD73" s="24"/>
-      <c r="CE73" s="24"/>
-      <c r="CF73" s="24"/>
-      <c r="CG73" s="24"/>
-      <c r="CH73" s="24"/>
-      <c r="CI73" s="24"/>
-      <c r="CJ73" s="24"/>
-      <c r="CK73" s="24"/>
-      <c r="CL73" s="25"/>
-      <c r="CM73" s="23" t="s">
+      <c r="BV73" s="26"/>
+      <c r="BW73" s="26"/>
+      <c r="BX73" s="26"/>
+      <c r="BY73" s="26"/>
+      <c r="BZ73" s="26"/>
+      <c r="CA73" s="26"/>
+      <c r="CB73" s="26"/>
+      <c r="CC73" s="26"/>
+      <c r="CD73" s="26"/>
+      <c r="CE73" s="26"/>
+      <c r="CF73" s="26"/>
+      <c r="CG73" s="26"/>
+      <c r="CH73" s="26"/>
+      <c r="CI73" s="26"/>
+      <c r="CJ73" s="26"/>
+      <c r="CK73" s="26"/>
+      <c r="CL73" s="27"/>
+      <c r="CM73" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN73" s="24"/>
-      <c r="CO73" s="24"/>
-      <c r="CP73" s="24"/>
-      <c r="CQ73" s="24"/>
-      <c r="CR73" s="24"/>
-      <c r="CS73" s="24"/>
-      <c r="CT73" s="24"/>
-      <c r="CU73" s="24"/>
-      <c r="CV73" s="25"/>
-      <c r="CW73" s="23" t="s">
+      <c r="CN73" s="26"/>
+      <c r="CO73" s="26"/>
+      <c r="CP73" s="26"/>
+      <c r="CQ73" s="26"/>
+      <c r="CR73" s="26"/>
+      <c r="CS73" s="26"/>
+      <c r="CT73" s="26"/>
+      <c r="CU73" s="26"/>
+      <c r="CV73" s="27"/>
+      <c r="CW73" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX73" s="24"/>
-      <c r="CY73" s="24"/>
-      <c r="CZ73" s="24"/>
-      <c r="DA73" s="24"/>
-      <c r="DB73" s="24"/>
-      <c r="DC73" s="24"/>
-      <c r="DD73" s="24"/>
-      <c r="DE73" s="24"/>
-      <c r="DF73" s="25"/>
+      <c r="CX73" s="26"/>
+      <c r="CY73" s="26"/>
+      <c r="CZ73" s="26"/>
+      <c r="DA73" s="26"/>
+      <c r="DB73" s="26"/>
+      <c r="DC73" s="26"/>
+      <c r="DD73" s="26"/>
+      <c r="DE73" s="26"/>
+      <c r="DF73" s="27"/>
     </row>
     <row r="74" spans="1:110" ht="57" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A74" s="22"/>
@@ -12267,7 +12281,7 @@
       </c>
     </row>
     <row r="76" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A76" s="51" t="s">
+      <c r="A76" s="40" t="s">
         <v>87</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -12391,7 +12405,7 @@
       </c>
     </row>
     <row r="77" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A77" s="52"/>
+      <c r="A77" s="41"/>
       <c r="B77" s="3" t="s">
         <v>187</v>
       </c>
@@ -12509,7 +12523,7 @@
       </c>
     </row>
     <row r="78" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A78" s="37" t="s">
+      <c r="A78" s="32" t="s">
         <v>88</v>
       </c>
       <c r="B78" s="2" t="s">
@@ -12627,7 +12641,7 @@
       <c r="DF78" s="20"/>
     </row>
     <row r="79" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A79" s="38"/>
+      <c r="A79" s="33"/>
       <c r="B79" s="2" t="s">
         <v>188</v>
       </c>
@@ -12743,7 +12757,7 @@
       <c r="DF79" s="20"/>
     </row>
     <row r="80" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A80" s="41" t="s">
+      <c r="A80" s="38" t="s">
         <v>89</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -12881,7 +12895,7 @@
       <c r="DF80" s="21"/>
     </row>
     <row r="81" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A81" s="42"/>
+      <c r="A81" s="39"/>
       <c r="B81" s="3" t="s">
         <v>190</v>
       </c>
@@ -13011,7 +13025,7 @@
       <c r="DF81" s="21"/>
     </row>
     <row r="82" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A82" s="42"/>
+      <c r="A82" s="39"/>
       <c r="B82" s="3" t="s">
         <v>191</v>
       </c>
@@ -13129,7 +13143,7 @@
       <c r="DF82" s="21"/>
     </row>
     <row r="83" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A83" s="42"/>
+      <c r="A83" s="39"/>
       <c r="B83" s="3" t="s">
         <v>192</v>
       </c>
@@ -13249,7 +13263,7 @@
       <c r="DF83" s="21"/>
     </row>
     <row r="84" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A84" s="42"/>
+      <c r="A84" s="39"/>
       <c r="B84" s="3" t="s">
         <v>139</v>
       </c>
@@ -13363,7 +13377,7 @@
       <c r="DF84" s="21"/>
     </row>
     <row r="85" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A85" s="42"/>
+      <c r="A85" s="39"/>
       <c r="B85" s="3" t="s">
         <v>193</v>
       </c>
@@ -13597,7 +13611,7 @@
       <c r="DF86" s="21"/>
     </row>
     <row r="87" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A87" s="37" t="s">
+      <c r="A87" s="32" t="s">
         <v>90</v>
       </c>
       <c r="B87" s="2" t="s">
@@ -13729,7 +13743,7 @@
       <c r="DF87" s="20"/>
     </row>
     <row r="88" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A88" s="38"/>
+      <c r="A88" s="33"/>
       <c r="B88" s="2" t="s">
         <v>189</v>
       </c>
@@ -13843,7 +13857,7 @@
       <c r="DF88" s="20"/>
     </row>
     <row r="89" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A89" s="38"/>
+      <c r="A89" s="33"/>
       <c r="B89" s="2" t="s">
         <v>141</v>
       </c>
@@ -13961,7 +13975,7 @@
       <c r="DF89" s="20"/>
     </row>
     <row r="90" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A90" s="38"/>
+      <c r="A90" s="33"/>
       <c r="B90" s="2" t="s">
         <v>142</v>
       </c>
@@ -14091,7 +14105,7 @@
       <c r="DF90" s="20"/>
     </row>
     <row r="91" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A91" s="34" t="s">
+      <c r="A91" s="30" t="s">
         <v>91</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -14209,7 +14223,7 @@
       <c r="DF91" s="21"/>
     </row>
     <row r="92" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A92" s="35"/>
+      <c r="A92" s="31"/>
       <c r="B92" s="3" t="s">
         <v>196</v>
       </c>
@@ -14325,7 +14339,7 @@
       <c r="DF92" s="21"/>
     </row>
     <row r="93" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A93" s="35"/>
+      <c r="A93" s="31"/>
       <c r="B93" s="3" t="s">
         <v>197</v>
       </c>
@@ -14441,7 +14455,7 @@
       <c r="DF93" s="21"/>
     </row>
     <row r="94" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A94" s="35"/>
+      <c r="A94" s="31"/>
       <c r="B94" s="3" t="s">
         <v>198</v>
       </c>
@@ -14555,7 +14569,7 @@
       <c r="DF94" s="21"/>
     </row>
     <row r="95" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A95" s="35"/>
+      <c r="A95" s="31"/>
       <c r="B95" s="3" t="s">
         <v>199</v>
       </c>
@@ -14671,7 +14685,7 @@
       <c r="DF95" s="21"/>
     </row>
     <row r="96" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A96" s="40"/>
+      <c r="A96" s="34"/>
       <c r="B96" s="3" t="s">
         <v>189</v>
       </c>
@@ -14785,7 +14799,7 @@
       <c r="DF96" s="21"/>
     </row>
     <row r="97" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A97" s="37" t="s">
+      <c r="A97" s="32" t="s">
         <v>92</v>
       </c>
       <c r="B97" s="2" t="s">
@@ -14907,7 +14921,7 @@
       <c r="DF97" s="20"/>
     </row>
     <row r="98" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A98" s="38"/>
+      <c r="A98" s="33"/>
       <c r="B98" s="2" t="s">
         <v>200</v>
       </c>
@@ -15027,7 +15041,7 @@
       <c r="DF98" s="20"/>
     </row>
     <row r="99" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A99" s="34" t="s">
+      <c r="A99" s="30" t="s">
         <v>93</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -15163,7 +15177,7 @@
       <c r="DF99" s="21"/>
     </row>
     <row r="100" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="40"/>
+      <c r="A100" s="34"/>
       <c r="B100" s="3" t="s">
         <v>201</v>
       </c>
@@ -15297,7 +15311,7 @@
       <c r="DF100" s="21"/>
     </row>
     <row r="101" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="37" t="s">
+      <c r="A101" s="32" t="s">
         <v>94</v>
       </c>
       <c r="B101" s="2" t="s">
@@ -15415,7 +15429,7 @@
       <c r="DF101" s="20"/>
     </row>
     <row r="102" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A102" s="38"/>
+      <c r="A102" s="33"/>
       <c r="B102" s="2" t="s">
         <v>202</v>
       </c>
@@ -15531,7 +15545,7 @@
       <c r="DF102" s="20"/>
     </row>
     <row r="103" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A103" s="38"/>
+      <c r="A103" s="33"/>
       <c r="B103" s="2" t="s">
         <v>203</v>
       </c>
@@ -15647,7 +15661,7 @@
       <c r="DF103" s="20"/>
     </row>
     <row r="104" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A104" s="34" t="s">
+      <c r="A104" s="30" t="s">
         <v>95</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -15773,7 +15787,7 @@
       <c r="DF104" s="21"/>
     </row>
     <row r="105" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A105" s="35"/>
+      <c r="A105" s="31"/>
       <c r="B105" s="3" t="s">
         <v>205</v>
       </c>
@@ -15897,7 +15911,7 @@
       <c r="DF105" s="21"/>
     </row>
     <row r="106" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A106" s="35"/>
+      <c r="A106" s="31"/>
       <c r="B106" s="3" t="s">
         <v>206</v>
       </c>
@@ -16015,7 +16029,7 @@
       <c r="DF106" s="21"/>
     </row>
     <row r="107" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A107" s="35"/>
+      <c r="A107" s="31"/>
       <c r="B107" s="3" t="s">
         <v>431</v>
       </c>
@@ -16129,7 +16143,7 @@
       <c r="DF107" s="21"/>
     </row>
     <row r="108" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A108" s="40"/>
+      <c r="A108" s="34"/>
       <c r="B108" s="3" t="s">
         <v>77</v>
       </c>
@@ -16243,7 +16257,7 @@
       <c r="DF108" s="21"/>
     </row>
     <row r="109" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A109" s="37" t="s">
+      <c r="A109" s="32" t="s">
         <v>96</v>
       </c>
       <c r="B109" s="2" t="s">
@@ -16385,7 +16399,7 @@
       <c r="DF109" s="20"/>
     </row>
     <row r="110" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A110" s="38"/>
+      <c r="A110" s="33"/>
       <c r="B110" s="2" t="s">
         <v>207</v>
       </c>
@@ -16529,7 +16543,7 @@
       <c r="DF110" s="20"/>
     </row>
     <row r="111" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A111" s="38"/>
+      <c r="A111" s="33"/>
       <c r="B111" s="2" t="s">
         <v>208</v>
       </c>
@@ -16653,7 +16667,7 @@
       <c r="DF111" s="20"/>
     </row>
     <row r="112" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A112" s="38"/>
+      <c r="A112" s="33"/>
       <c r="B112" s="2" t="s">
         <v>209</v>
       </c>
@@ -16785,7 +16799,7 @@
       <c r="DF112" s="20"/>
     </row>
     <row r="113" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A113" s="38"/>
+      <c r="A113" s="33"/>
       <c r="B113" s="2" t="s">
         <v>210</v>
       </c>
@@ -16913,7 +16927,7 @@
       <c r="DF113" s="20"/>
     </row>
     <row r="114" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A114" s="38"/>
+      <c r="A114" s="33"/>
       <c r="B114" s="2" t="s">
         <v>211</v>
       </c>
@@ -17033,7 +17047,7 @@
       <c r="DF114" s="20"/>
     </row>
     <row r="115" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="34" t="s">
+      <c r="A115" s="30" t="s">
         <v>97</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -17151,7 +17165,7 @@
       <c r="DF115" s="21"/>
     </row>
     <row r="116" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A116" s="35"/>
+      <c r="A116" s="31"/>
       <c r="B116" s="3" t="s">
         <v>213</v>
       </c>
@@ -17267,7 +17281,7 @@
       <c r="DF116" s="21"/>
     </row>
     <row r="117" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A117" s="37" t="s">
+      <c r="A117" s="32" t="s">
         <v>98</v>
       </c>
       <c r="B117" s="2" t="s">
@@ -17387,7 +17401,7 @@
       <c r="DF117" s="20"/>
     </row>
     <row r="118" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A118" s="38"/>
+      <c r="A118" s="33"/>
       <c r="B118" s="2" t="s">
         <v>204</v>
       </c>
@@ -17501,7 +17515,7 @@
       <c r="DF118" s="20"/>
     </row>
     <row r="119" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A119" s="38"/>
+      <c r="A119" s="33"/>
       <c r="B119" s="2" t="s">
         <v>141</v>
       </c>
@@ -17615,7 +17629,7 @@
       <c r="DF119" s="20"/>
     </row>
     <row r="120" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A120" s="38"/>
+      <c r="A120" s="33"/>
       <c r="B120" s="2" t="s">
         <v>214</v>
       </c>
@@ -17731,7 +17745,7 @@
       <c r="DF120" s="20"/>
     </row>
     <row r="121" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A121" s="41" t="s">
+      <c r="A121" s="38" t="s">
         <v>99</v>
       </c>
       <c r="B121" s="3" t="s">
@@ -17849,7 +17863,7 @@
       <c r="DF121" s="21"/>
     </row>
     <row r="122" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A122" s="42"/>
+      <c r="A122" s="39"/>
       <c r="B122" s="3" t="s">
         <v>147</v>
       </c>
@@ -17963,7 +17977,7 @@
       <c r="DF122" s="21"/>
     </row>
     <row r="123" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A123" s="42"/>
+      <c r="A123" s="39"/>
       <c r="B123" s="3" t="s">
         <v>216</v>
       </c>
@@ -18193,7 +18207,7 @@
       <c r="DF124" s="21"/>
     </row>
     <row r="125" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A125" s="48" t="s">
+      <c r="A125" s="35" t="s">
         <v>100</v>
       </c>
       <c r="B125" s="2" t="s">
@@ -18317,7 +18331,7 @@
       <c r="DF125" s="20"/>
     </row>
     <row r="126" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A126" s="49"/>
+      <c r="A126" s="36"/>
       <c r="B126" s="2" t="s">
         <v>217</v>
       </c>
@@ -18439,7 +18453,7 @@
       <c r="DF126" s="20"/>
     </row>
     <row r="127" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="50"/>
+      <c r="A127" s="37"/>
       <c r="B127" s="2" t="s">
         <v>212</v>
       </c>
@@ -18557,7 +18571,7 @@
       <c r="DF127" s="20"/>
     </row>
     <row r="128" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A128" s="41" t="s">
+      <c r="A128" s="38" t="s">
         <v>102</v>
       </c>
       <c r="B128" s="3" t="s">
@@ -18675,7 +18689,7 @@
       <c r="DF128" s="21"/>
     </row>
     <row r="129" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A129" s="42"/>
+      <c r="A129" s="39"/>
       <c r="B129" s="3" t="s">
         <v>142</v>
       </c>
@@ -18791,7 +18805,7 @@
       <c r="DF129" s="21"/>
     </row>
     <row r="130" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A130" s="42"/>
+      <c r="A130" s="39"/>
       <c r="B130" s="3" t="s">
         <v>141</v>
       </c>
@@ -19023,7 +19037,7 @@
       <c r="DF131" s="21"/>
     </row>
     <row r="132" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A132" s="37" t="s">
+      <c r="A132" s="32" t="s">
         <v>101</v>
       </c>
       <c r="B132" s="2" t="s">
@@ -19143,7 +19157,7 @@
       <c r="DF132" s="20"/>
     </row>
     <row r="133" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A133" s="38"/>
+      <c r="A133" s="33"/>
       <c r="B133" s="2" t="s">
         <v>221</v>
       </c>
@@ -19261,7 +19275,7 @@
       <c r="DF133" s="20"/>
     </row>
     <row r="134" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A134" s="34" t="s">
+      <c r="A134" s="30" t="s">
         <v>103</v>
       </c>
       <c r="B134" s="3" t="s">
@@ -19393,7 +19407,7 @@
       <c r="DF134" s="21"/>
     </row>
     <row r="135" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A135" s="35"/>
+      <c r="A135" s="31"/>
       <c r="B135" s="3" t="s">
         <v>223</v>
       </c>
@@ -19515,7 +19529,7 @@
       <c r="DF135" s="21"/>
     </row>
     <row r="136" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A136" s="35"/>
+      <c r="A136" s="31"/>
       <c r="B136" s="3" t="s">
         <v>210</v>
       </c>
@@ -19641,7 +19655,7 @@
       <c r="DF136" s="21"/>
     </row>
     <row r="137" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A137" s="35"/>
+      <c r="A137" s="31"/>
       <c r="B137" s="3" t="s">
         <v>224</v>
       </c>
@@ -19761,7 +19775,7 @@
       <c r="DF137" s="21"/>
     </row>
     <row r="138" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A138" s="35"/>
+      <c r="A138" s="31"/>
       <c r="B138" s="3" t="s">
         <v>225</v>
       </c>
@@ -19879,7 +19893,7 @@
       <c r="DF138" s="21"/>
     </row>
     <row r="139" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A139" s="37" t="s">
+      <c r="A139" s="32" t="s">
         <v>104</v>
       </c>
       <c r="B139" s="2" t="s">
@@ -20003,7 +20017,7 @@
       <c r="DF139" s="20"/>
     </row>
     <row r="140" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A140" s="38"/>
+      <c r="A140" s="33"/>
       <c r="B140" s="2" t="s">
         <v>227</v>
       </c>
@@ -20125,7 +20139,7 @@
       <c r="DF140" s="20"/>
     </row>
     <row r="141" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A141" s="38"/>
+      <c r="A141" s="33"/>
       <c r="B141" s="2" t="s">
         <v>228</v>
       </c>
@@ -20247,7 +20261,7 @@
       <c r="DF141" s="20"/>
     </row>
     <row r="142" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A142" s="38"/>
+      <c r="A142" s="33"/>
       <c r="B142" s="2" t="s">
         <v>229</v>
       </c>
@@ -20369,141 +20383,141 @@
       <c r="DF142" s="20"/>
     </row>
     <row r="143" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="44"/>
+      <c r="A143" s="23"/>
       <c r="B143" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C143" s="26" t="s">
+      <c r="C143" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D143" s="24"/>
-      <c r="E143" s="24"/>
-      <c r="F143" s="25"/>
-      <c r="G143" s="27" t="s">
+      <c r="D143" s="26"/>
+      <c r="E143" s="26"/>
+      <c r="F143" s="27"/>
+      <c r="G143" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H143" s="28"/>
-      <c r="I143" s="28"/>
-      <c r="J143" s="27" t="s">
+      <c r="H143" s="29"/>
+      <c r="I143" s="29"/>
+      <c r="J143" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K143" s="28"/>
-      <c r="L143" s="28"/>
-      <c r="M143" s="28"/>
-      <c r="N143" s="28"/>
-      <c r="O143" s="28"/>
-      <c r="P143" s="28"/>
-      <c r="Q143" s="28"/>
-      <c r="R143" s="28"/>
-      <c r="S143" s="28"/>
-      <c r="T143" s="28"/>
-      <c r="U143" s="28"/>
-      <c r="V143" s="28"/>
-      <c r="W143" s="28"/>
-      <c r="X143" s="28"/>
-      <c r="Y143" s="27" t="s">
+      <c r="K143" s="29"/>
+      <c r="L143" s="29"/>
+      <c r="M143" s="29"/>
+      <c r="N143" s="29"/>
+      <c r="O143" s="29"/>
+      <c r="P143" s="29"/>
+      <c r="Q143" s="29"/>
+      <c r="R143" s="29"/>
+      <c r="S143" s="29"/>
+      <c r="T143" s="29"/>
+      <c r="U143" s="29"/>
+      <c r="V143" s="29"/>
+      <c r="W143" s="29"/>
+      <c r="X143" s="29"/>
+      <c r="Y143" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z143" s="28"/>
-      <c r="AA143" s="28"/>
-      <c r="AB143" s="28"/>
-      <c r="AC143" s="28"/>
-      <c r="AD143" s="28"/>
-      <c r="AE143" s="28"/>
-      <c r="AF143" s="28"/>
-      <c r="AG143" s="28"/>
-      <c r="AH143" s="28"/>
-      <c r="AI143" s="28"/>
-      <c r="AJ143" s="28"/>
-      <c r="AK143" s="28"/>
-      <c r="AL143" s="28"/>
-      <c r="AM143" s="28"/>
-      <c r="AN143" s="28"/>
-      <c r="AO143" s="28"/>
-      <c r="AP143" s="28"/>
-      <c r="AQ143" s="29" t="s">
+      <c r="Z143" s="29"/>
+      <c r="AA143" s="29"/>
+      <c r="AB143" s="29"/>
+      <c r="AC143" s="29"/>
+      <c r="AD143" s="29"/>
+      <c r="AE143" s="29"/>
+      <c r="AF143" s="29"/>
+      <c r="AG143" s="29"/>
+      <c r="AH143" s="29"/>
+      <c r="AI143" s="29"/>
+      <c r="AJ143" s="29"/>
+      <c r="AK143" s="29"/>
+      <c r="AL143" s="29"/>
+      <c r="AM143" s="29"/>
+      <c r="AN143" s="29"/>
+      <c r="AO143" s="29"/>
+      <c r="AP143" s="29"/>
+      <c r="AQ143" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR143" s="30"/>
-      <c r="AS143" s="30"/>
-      <c r="AT143" s="30"/>
-      <c r="AU143" s="30"/>
-      <c r="AV143" s="30"/>
-      <c r="AW143" s="30"/>
-      <c r="AX143" s="30"/>
-      <c r="AY143" s="30"/>
-      <c r="AZ143" s="30"/>
-      <c r="BA143" s="31"/>
-      <c r="BB143" s="29" t="s">
+      <c r="AR143" s="46"/>
+      <c r="AS143" s="46"/>
+      <c r="AT143" s="46"/>
+      <c r="AU143" s="46"/>
+      <c r="AV143" s="46"/>
+      <c r="AW143" s="46"/>
+      <c r="AX143" s="46"/>
+      <c r="AY143" s="46"/>
+      <c r="AZ143" s="46"/>
+      <c r="BA143" s="47"/>
+      <c r="BB143" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC143" s="30"/>
-      <c r="BD143" s="30"/>
-      <c r="BE143" s="30"/>
-      <c r="BF143" s="30"/>
-      <c r="BG143" s="30"/>
-      <c r="BH143" s="30"/>
-      <c r="BI143" s="30"/>
-      <c r="BJ143" s="30"/>
-      <c r="BK143" s="30"/>
-      <c r="BL143" s="30"/>
-      <c r="BM143" s="30"/>
-      <c r="BN143" s="30"/>
-      <c r="BO143" s="30"/>
-      <c r="BP143" s="31"/>
-      <c r="BQ143" s="32" t="s">
+      <c r="BC143" s="46"/>
+      <c r="BD143" s="46"/>
+      <c r="BE143" s="46"/>
+      <c r="BF143" s="46"/>
+      <c r="BG143" s="46"/>
+      <c r="BH143" s="46"/>
+      <c r="BI143" s="46"/>
+      <c r="BJ143" s="46"/>
+      <c r="BK143" s="46"/>
+      <c r="BL143" s="46"/>
+      <c r="BM143" s="46"/>
+      <c r="BN143" s="46"/>
+      <c r="BO143" s="46"/>
+      <c r="BP143" s="47"/>
+      <c r="BQ143" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR143" s="33"/>
-      <c r="BS143" s="33"/>
-      <c r="BT143" s="33"/>
-      <c r="BU143" s="23" t="s">
+      <c r="BR143" s="49"/>
+      <c r="BS143" s="49"/>
+      <c r="BT143" s="49"/>
+      <c r="BU143" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV143" s="24"/>
-      <c r="BW143" s="24"/>
-      <c r="BX143" s="24"/>
-      <c r="BY143" s="24"/>
-      <c r="BZ143" s="24"/>
-      <c r="CA143" s="24"/>
-      <c r="CB143" s="24"/>
-      <c r="CC143" s="24"/>
-      <c r="CD143" s="24"/>
-      <c r="CE143" s="24"/>
-      <c r="CF143" s="24"/>
-      <c r="CG143" s="24"/>
-      <c r="CH143" s="24"/>
-      <c r="CI143" s="24"/>
-      <c r="CJ143" s="24"/>
-      <c r="CK143" s="24"/>
-      <c r="CL143" s="25"/>
-      <c r="CM143" s="23" t="s">
+      <c r="BV143" s="26"/>
+      <c r="BW143" s="26"/>
+      <c r="BX143" s="26"/>
+      <c r="BY143" s="26"/>
+      <c r="BZ143" s="26"/>
+      <c r="CA143" s="26"/>
+      <c r="CB143" s="26"/>
+      <c r="CC143" s="26"/>
+      <c r="CD143" s="26"/>
+      <c r="CE143" s="26"/>
+      <c r="CF143" s="26"/>
+      <c r="CG143" s="26"/>
+      <c r="CH143" s="26"/>
+      <c r="CI143" s="26"/>
+      <c r="CJ143" s="26"/>
+      <c r="CK143" s="26"/>
+      <c r="CL143" s="27"/>
+      <c r="CM143" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN143" s="24"/>
-      <c r="CO143" s="24"/>
-      <c r="CP143" s="24"/>
-      <c r="CQ143" s="24"/>
-      <c r="CR143" s="24"/>
-      <c r="CS143" s="24"/>
-      <c r="CT143" s="24"/>
-      <c r="CU143" s="24"/>
-      <c r="CV143" s="25"/>
-      <c r="CW143" s="23" t="s">
+      <c r="CN143" s="26"/>
+      <c r="CO143" s="26"/>
+      <c r="CP143" s="26"/>
+      <c r="CQ143" s="26"/>
+      <c r="CR143" s="26"/>
+      <c r="CS143" s="26"/>
+      <c r="CT143" s="26"/>
+      <c r="CU143" s="26"/>
+      <c r="CV143" s="27"/>
+      <c r="CW143" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX143" s="24"/>
-      <c r="CY143" s="24"/>
-      <c r="CZ143" s="24"/>
-      <c r="DA143" s="24"/>
-      <c r="DB143" s="24"/>
-      <c r="DC143" s="24"/>
-      <c r="DD143" s="24"/>
-      <c r="DE143" s="24"/>
-      <c r="DF143" s="25"/>
+      <c r="CX143" s="26"/>
+      <c r="CY143" s="26"/>
+      <c r="CZ143" s="26"/>
+      <c r="DA143" s="26"/>
+      <c r="DB143" s="26"/>
+      <c r="DC143" s="26"/>
+      <c r="DD143" s="26"/>
+      <c r="DE143" s="26"/>
+      <c r="DF143" s="27"/>
     </row>
     <row r="144" spans="1:110" ht="56.25" x14ac:dyDescent="0.15">
-      <c r="A144" s="45"/>
+      <c r="A144" s="24"/>
       <c r="B144" s="12" t="s">
         <v>2</v>
       </c>
@@ -21165,7 +21179,7 @@
       </c>
     </row>
     <row r="146" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A146" s="34" t="s">
+      <c r="A146" s="30" t="s">
         <v>105</v>
       </c>
       <c r="B146" s="3" t="s">
@@ -21281,7 +21295,7 @@
       <c r="DF146" s="21"/>
     </row>
     <row r="147" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A147" s="35"/>
+      <c r="A147" s="31"/>
       <c r="B147" s="3" t="s">
         <v>127</v>
       </c>
@@ -21395,7 +21409,7 @@
       <c r="DF147" s="21"/>
     </row>
     <row r="148" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A148" s="37" t="s">
+      <c r="A148" s="32" t="s">
         <v>106</v>
       </c>
       <c r="B148" s="2" t="s">
@@ -21513,7 +21527,7 @@
       <c r="DF148" s="20"/>
     </row>
     <row r="149" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A149" s="38"/>
+      <c r="A149" s="33"/>
       <c r="B149" s="2" t="s">
         <v>142</v>
       </c>
@@ -21629,7 +21643,7 @@
       <c r="DF149" s="20"/>
     </row>
     <row r="150" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A150" s="38"/>
+      <c r="A150" s="33"/>
       <c r="B150" s="2" t="s">
         <v>226</v>
       </c>
@@ -21743,7 +21757,7 @@
       <c r="DF150" s="20"/>
     </row>
     <row r="151" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A151" s="38"/>
+      <c r="A151" s="33"/>
       <c r="B151" s="2" t="s">
         <v>232</v>
       </c>
@@ -21857,7 +21871,7 @@
       <c r="DF151" s="20"/>
     </row>
     <row r="152" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A152" s="38"/>
+      <c r="A152" s="33"/>
       <c r="B152" s="2" t="s">
         <v>230</v>
       </c>
@@ -21971,7 +21985,7 @@
       <c r="DF152" s="20"/>
     </row>
     <row r="153" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A153" s="34" t="s">
+      <c r="A153" s="30" t="s">
         <v>107</v>
       </c>
       <c r="B153" s="3" t="s">
@@ -22091,7 +22105,7 @@
       <c r="DF153" s="21"/>
     </row>
     <row r="154" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A154" s="35"/>
+      <c r="A154" s="31"/>
       <c r="B154" s="3" t="s">
         <v>77</v>
       </c>
@@ -22209,7 +22223,7 @@
       <c r="DF154" s="21"/>
     </row>
     <row r="155" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A155" s="35"/>
+      <c r="A155" s="31"/>
       <c r="B155" s="3" t="s">
         <v>220</v>
       </c>
@@ -22327,7 +22341,7 @@
       <c r="DF155" s="21"/>
     </row>
     <row r="156" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A156" s="37" t="s">
+      <c r="A156" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B156" s="2" t="s">
@@ -22447,7 +22461,7 @@
       <c r="DF156" s="20"/>
     </row>
     <row r="157" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A157" s="38"/>
+      <c r="A157" s="33"/>
       <c r="B157" s="2" t="s">
         <v>139</v>
       </c>
@@ -22565,7 +22579,7 @@
       <c r="DF157" s="20"/>
     </row>
     <row r="158" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A158" s="38"/>
+      <c r="A158" s="33"/>
       <c r="B158" s="2" t="s">
         <v>189</v>
       </c>
@@ -22683,7 +22697,7 @@
       <c r="DF158" s="20"/>
     </row>
     <row r="159" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A159" s="39"/>
+      <c r="A159" s="42"/>
       <c r="B159" s="2" t="s">
         <v>233</v>
       </c>
@@ -22801,7 +22815,7 @@
       <c r="DF159" s="20"/>
     </row>
     <row r="160" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A160" s="34" t="s">
+      <c r="A160" s="30" t="s">
         <v>109</v>
       </c>
       <c r="B160" s="3" t="s">
@@ -22921,7 +22935,7 @@
       <c r="DF160" s="21"/>
     </row>
     <row r="161" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A161" s="35"/>
+      <c r="A161" s="31"/>
       <c r="B161" s="3" t="s">
         <v>149</v>
       </c>
@@ -23037,7 +23051,7 @@
       <c r="DF161" s="21"/>
     </row>
     <row r="162" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A162" s="35"/>
+      <c r="A162" s="31"/>
       <c r="B162" s="3" t="s">
         <v>194</v>
       </c>
@@ -23153,7 +23167,7 @@
       <c r="DF162" s="21"/>
     </row>
     <row r="163" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A163" s="35"/>
+      <c r="A163" s="31"/>
       <c r="B163" s="3" t="s">
         <v>235</v>
       </c>
@@ -23271,7 +23285,7 @@
       <c r="DF163" s="21"/>
     </row>
     <row r="164" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A164" s="40"/>
+      <c r="A164" s="34"/>
       <c r="B164" s="3" t="s">
         <v>142</v>
       </c>
@@ -23389,7 +23403,7 @@
       <c r="DF164" s="21"/>
     </row>
     <row r="165" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A165" s="37" t="s">
+      <c r="A165" s="32" t="s">
         <v>110</v>
       </c>
       <c r="B165" s="2" t="s">
@@ -23507,7 +23521,7 @@
       <c r="DF165" s="20"/>
     </row>
     <row r="166" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A166" s="38"/>
+      <c r="A166" s="33"/>
       <c r="B166" s="2" t="s">
         <v>237</v>
       </c>
@@ -23623,7 +23637,7 @@
       <c r="DF166" s="20"/>
     </row>
     <row r="167" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A167" s="38"/>
+      <c r="A167" s="33"/>
       <c r="B167" s="2" t="s">
         <v>139</v>
       </c>
@@ -23739,7 +23753,7 @@
       <c r="DF167" s="20"/>
     </row>
     <row r="168" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A168" s="41" t="s">
+      <c r="A168" s="38" t="s">
         <v>111</v>
       </c>
       <c r="B168" s="3" t="s">
@@ -23857,7 +23871,7 @@
       <c r="DF168" s="21"/>
     </row>
     <row r="169" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A169" s="42"/>
+      <c r="A169" s="39"/>
       <c r="B169" s="3" t="s">
         <v>239</v>
       </c>
@@ -23973,7 +23987,7 @@
       <c r="DF169" s="21"/>
     </row>
     <row r="170" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A170" s="42"/>
+      <c r="A170" s="39"/>
       <c r="B170" s="3" t="s">
         <v>236</v>
       </c>
@@ -24205,7 +24219,7 @@
       <c r="DF171" s="21"/>
     </row>
     <row r="172" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A172" s="37" t="s">
+      <c r="A172" s="32" t="s">
         <v>112</v>
       </c>
       <c r="B172" s="2" t="s">
@@ -24331,7 +24345,7 @@
       <c r="DF172" s="20"/>
     </row>
     <row r="173" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A173" s="38"/>
+      <c r="A173" s="33"/>
       <c r="B173" s="2" t="s">
         <v>247</v>
       </c>
@@ -24453,7 +24467,7 @@
       <c r="DF173" s="20"/>
     </row>
     <row r="174" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A174" s="38"/>
+      <c r="A174" s="33"/>
       <c r="B174" s="2" t="s">
         <v>219</v>
       </c>
@@ -24569,7 +24583,7 @@
       <c r="DF174" s="20"/>
     </row>
     <row r="175" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A175" s="34" t="s">
+      <c r="A175" s="30" t="s">
         <v>113</v>
       </c>
       <c r="B175" s="3" t="s">
@@ -24695,7 +24709,7 @@
       <c r="DF175" s="21"/>
     </row>
     <row r="176" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A176" s="35"/>
+      <c r="A176" s="31"/>
       <c r="B176" s="3" t="s">
         <v>245</v>
       </c>
@@ -24811,7 +24825,7 @@
       <c r="DF176" s="21"/>
     </row>
     <row r="177" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A177" s="35"/>
+      <c r="A177" s="31"/>
       <c r="B177" s="3" t="s">
         <v>141</v>
       </c>
@@ -24931,7 +24945,7 @@
       <c r="DF177" s="21"/>
     </row>
     <row r="178" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A178" s="35"/>
+      <c r="A178" s="31"/>
       <c r="B178" s="3" t="s">
         <v>142</v>
       </c>
@@ -25053,7 +25067,7 @@
       <c r="DF178" s="21"/>
     </row>
     <row r="179" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A179" s="37" t="s">
+      <c r="A179" s="32" t="s">
         <v>114</v>
       </c>
       <c r="B179" s="2" t="s">
@@ -25177,7 +25191,7 @@
       <c r="DF179" s="20"/>
     </row>
     <row r="180" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A180" s="38"/>
+      <c r="A180" s="33"/>
       <c r="B180" s="2" t="s">
         <v>242</v>
       </c>
@@ -25295,7 +25309,7 @@
       <c r="DF180" s="20"/>
     </row>
     <row r="181" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A181" s="38"/>
+      <c r="A181" s="33"/>
       <c r="B181" s="2" t="s">
         <v>243</v>
       </c>
@@ -25413,7 +25427,7 @@
       <c r="DF181" s="20"/>
     </row>
     <row r="182" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A182" s="38"/>
+      <c r="A182" s="33"/>
       <c r="B182" s="2" t="s">
         <v>244</v>
       </c>
@@ -25531,7 +25545,7 @@
       <c r="DF182" s="20"/>
     </row>
     <row r="183" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A183" s="39"/>
+      <c r="A183" s="42"/>
       <c r="B183" s="2" t="s">
         <v>245</v>
       </c>
@@ -25647,7 +25661,7 @@
       <c r="DF183" s="20"/>
     </row>
     <row r="184" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A184" s="41" t="s">
+      <c r="A184" s="38" t="s">
         <v>115</v>
       </c>
       <c r="B184" s="3" t="s">
@@ -25889,7 +25903,7 @@
       <c r="DF185" s="21"/>
     </row>
     <row r="186" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A186" s="37" t="s">
+      <c r="A186" s="32" t="s">
         <v>116</v>
       </c>
       <c r="B186" s="2" t="s">
@@ -25946,7 +25960,9 @@
       <c r="AU186" s="20"/>
       <c r="AV186" s="20"/>
       <c r="AW186" s="20"/>
-      <c r="AX186" s="20"/>
+      <c r="AX186" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="AY186" s="20" t="s">
         <v>429</v>
       </c>
@@ -26015,7 +26031,7 @@
       <c r="DF186" s="20"/>
     </row>
     <row r="187" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A187" s="38"/>
+      <c r="A187" s="33"/>
       <c r="B187" s="2" t="s">
         <v>248</v>
       </c>
@@ -26066,7 +26082,9 @@
       <c r="AU187" s="20"/>
       <c r="AV187" s="20"/>
       <c r="AW187" s="20"/>
-      <c r="AX187" s="20"/>
+      <c r="AX187" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AY187" s="20" t="s">
         <v>429</v>
       </c>
@@ -26135,7 +26153,7 @@
       <c r="DF187" s="20"/>
     </row>
     <row r="188" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A188" s="34" t="s">
+      <c r="A188" s="30" t="s">
         <v>117</v>
       </c>
       <c r="B188" s="3" t="s">
@@ -26192,7 +26210,9 @@
       <c r="AU188" s="21"/>
       <c r="AV188" s="21"/>
       <c r="AW188" s="21"/>
-      <c r="AX188" s="21"/>
+      <c r="AX188" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="AY188" s="21" t="s">
         <v>429</v>
       </c>
@@ -26259,7 +26279,7 @@
       <c r="DF188" s="21"/>
     </row>
     <row r="189" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A189" s="35"/>
+      <c r="A189" s="31"/>
       <c r="B189" s="3" t="s">
         <v>162</v>
       </c>
@@ -26310,7 +26330,9 @@
       <c r="AU189" s="21"/>
       <c r="AV189" s="21"/>
       <c r="AW189" s="21"/>
-      <c r="AX189" s="21"/>
+      <c r="AX189" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AY189" s="21" t="s">
         <v>429</v>
       </c>
@@ -26375,7 +26397,7 @@
       <c r="DF189" s="21"/>
     </row>
     <row r="190" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A190" s="35"/>
+      <c r="A190" s="31"/>
       <c r="B190" s="3" t="s">
         <v>133</v>
       </c>
@@ -26426,7 +26448,9 @@
       <c r="AU190" s="21"/>
       <c r="AV190" s="21"/>
       <c r="AW190" s="21"/>
-      <c r="AX190" s="21"/>
+      <c r="AX190" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AY190" s="21" t="s">
         <v>425</v>
       </c>
@@ -26493,7 +26517,7 @@
       <c r="DF190" s="21"/>
     </row>
     <row r="191" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A191" s="46" t="s">
+      <c r="A191" s="50" t="s">
         <v>118</v>
       </c>
       <c r="B191" s="2" t="s">
@@ -26550,7 +26574,9 @@
       <c r="AU191" s="20"/>
       <c r="AV191" s="20"/>
       <c r="AW191" s="20"/>
-      <c r="AX191" s="20"/>
+      <c r="AX191" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AY191" s="20" t="s">
         <v>429</v>
       </c>
@@ -26617,7 +26643,7 @@
       <c r="DF191" s="20"/>
     </row>
     <row r="192" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A192" s="47"/>
+      <c r="A192" s="51"/>
       <c r="B192" s="2" t="s">
         <v>249</v>
       </c>
@@ -26668,7 +26694,9 @@
       <c r="AU192" s="20"/>
       <c r="AV192" s="20"/>
       <c r="AW192" s="20"/>
-      <c r="AX192" s="20"/>
+      <c r="AX192" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AY192" s="20" t="s">
         <v>425</v>
       </c>
@@ -26733,7 +26761,7 @@
       <c r="DF192" s="20"/>
     </row>
     <row r="193" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A193" s="47"/>
+      <c r="A193" s="51"/>
       <c r="B193" s="2" t="s">
         <v>167</v>
       </c>
@@ -26784,7 +26812,9 @@
       <c r="AU193" s="20"/>
       <c r="AV193" s="20"/>
       <c r="AW193" s="20"/>
-      <c r="AX193" s="20"/>
+      <c r="AX193" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AY193" s="20" t="s">
         <v>425</v>
       </c>
@@ -26849,141 +26879,141 @@
       <c r="DF193" s="20"/>
     </row>
     <row r="194" spans="1:110" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A194" s="44"/>
+      <c r="A194" s="23"/>
       <c r="B194" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C194" s="26" t="s">
+      <c r="C194" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D194" s="24"/>
-      <c r="E194" s="24"/>
-      <c r="F194" s="25"/>
-      <c r="G194" s="27" t="s">
+      <c r="D194" s="26"/>
+      <c r="E194" s="26"/>
+      <c r="F194" s="27"/>
+      <c r="G194" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="H194" s="28"/>
-      <c r="I194" s="28"/>
-      <c r="J194" s="27" t="s">
+      <c r="H194" s="29"/>
+      <c r="I194" s="29"/>
+      <c r="J194" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="K194" s="28"/>
-      <c r="L194" s="28"/>
-      <c r="M194" s="28"/>
-      <c r="N194" s="28"/>
-      <c r="O194" s="28"/>
-      <c r="P194" s="28"/>
-      <c r="Q194" s="28"/>
-      <c r="R194" s="28"/>
-      <c r="S194" s="28"/>
-      <c r="T194" s="28"/>
-      <c r="U194" s="28"/>
-      <c r="V194" s="28"/>
-      <c r="W194" s="28"/>
-      <c r="X194" s="28"/>
-      <c r="Y194" s="27" t="s">
+      <c r="K194" s="29"/>
+      <c r="L194" s="29"/>
+      <c r="M194" s="29"/>
+      <c r="N194" s="29"/>
+      <c r="O194" s="29"/>
+      <c r="P194" s="29"/>
+      <c r="Q194" s="29"/>
+      <c r="R194" s="29"/>
+      <c r="S194" s="29"/>
+      <c r="T194" s="29"/>
+      <c r="U194" s="29"/>
+      <c r="V194" s="29"/>
+      <c r="W194" s="29"/>
+      <c r="X194" s="29"/>
+      <c r="Y194" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="Z194" s="28"/>
-      <c r="AA194" s="28"/>
-      <c r="AB194" s="28"/>
-      <c r="AC194" s="28"/>
-      <c r="AD194" s="28"/>
-      <c r="AE194" s="28"/>
-      <c r="AF194" s="28"/>
-      <c r="AG194" s="28"/>
-      <c r="AH194" s="28"/>
-      <c r="AI194" s="28"/>
-      <c r="AJ194" s="28"/>
-      <c r="AK194" s="28"/>
-      <c r="AL194" s="28"/>
-      <c r="AM194" s="28"/>
-      <c r="AN194" s="28"/>
-      <c r="AO194" s="28"/>
-      <c r="AP194" s="28"/>
-      <c r="AQ194" s="29" t="s">
+      <c r="Z194" s="29"/>
+      <c r="AA194" s="29"/>
+      <c r="AB194" s="29"/>
+      <c r="AC194" s="29"/>
+      <c r="AD194" s="29"/>
+      <c r="AE194" s="29"/>
+      <c r="AF194" s="29"/>
+      <c r="AG194" s="29"/>
+      <c r="AH194" s="29"/>
+      <c r="AI194" s="29"/>
+      <c r="AJ194" s="29"/>
+      <c r="AK194" s="29"/>
+      <c r="AL194" s="29"/>
+      <c r="AM194" s="29"/>
+      <c r="AN194" s="29"/>
+      <c r="AO194" s="29"/>
+      <c r="AP194" s="29"/>
+      <c r="AQ194" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="AR194" s="30"/>
-      <c r="AS194" s="30"/>
-      <c r="AT194" s="30"/>
-      <c r="AU194" s="30"/>
-      <c r="AV194" s="30"/>
-      <c r="AW194" s="30"/>
-      <c r="AX194" s="30"/>
-      <c r="AY194" s="30"/>
-      <c r="AZ194" s="30"/>
-      <c r="BA194" s="31"/>
-      <c r="BB194" s="29" t="s">
+      <c r="AR194" s="46"/>
+      <c r="AS194" s="46"/>
+      <c r="AT194" s="46"/>
+      <c r="AU194" s="46"/>
+      <c r="AV194" s="46"/>
+      <c r="AW194" s="46"/>
+      <c r="AX194" s="46"/>
+      <c r="AY194" s="46"/>
+      <c r="AZ194" s="46"/>
+      <c r="BA194" s="47"/>
+      <c r="BB194" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BC194" s="30"/>
-      <c r="BD194" s="30"/>
-      <c r="BE194" s="30"/>
-      <c r="BF194" s="30"/>
-      <c r="BG194" s="30"/>
-      <c r="BH194" s="30"/>
-      <c r="BI194" s="30"/>
-      <c r="BJ194" s="30"/>
-      <c r="BK194" s="30"/>
-      <c r="BL194" s="30"/>
-      <c r="BM194" s="30"/>
-      <c r="BN194" s="30"/>
-      <c r="BO194" s="30"/>
-      <c r="BP194" s="31"/>
-      <c r="BQ194" s="32" t="s">
+      <c r="BC194" s="46"/>
+      <c r="BD194" s="46"/>
+      <c r="BE194" s="46"/>
+      <c r="BF194" s="46"/>
+      <c r="BG194" s="46"/>
+      <c r="BH194" s="46"/>
+      <c r="BI194" s="46"/>
+      <c r="BJ194" s="46"/>
+      <c r="BK194" s="46"/>
+      <c r="BL194" s="46"/>
+      <c r="BM194" s="46"/>
+      <c r="BN194" s="46"/>
+      <c r="BO194" s="46"/>
+      <c r="BP194" s="47"/>
+      <c r="BQ194" s="48" t="s">
         <v>66</v>
       </c>
-      <c r="BR194" s="33"/>
-      <c r="BS194" s="33"/>
-      <c r="BT194" s="33"/>
-      <c r="BU194" s="23" t="s">
+      <c r="BR194" s="49"/>
+      <c r="BS194" s="49"/>
+      <c r="BT194" s="49"/>
+      <c r="BU194" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="BV194" s="24"/>
-      <c r="BW194" s="24"/>
-      <c r="BX194" s="24"/>
-      <c r="BY194" s="24"/>
-      <c r="BZ194" s="24"/>
-      <c r="CA194" s="24"/>
-      <c r="CB194" s="24"/>
-      <c r="CC194" s="24"/>
-      <c r="CD194" s="24"/>
-      <c r="CE194" s="24"/>
-      <c r="CF194" s="24"/>
-      <c r="CG194" s="24"/>
-      <c r="CH194" s="24"/>
-      <c r="CI194" s="24"/>
-      <c r="CJ194" s="24"/>
-      <c r="CK194" s="24"/>
-      <c r="CL194" s="25"/>
-      <c r="CM194" s="23" t="s">
+      <c r="BV194" s="26"/>
+      <c r="BW194" s="26"/>
+      <c r="BX194" s="26"/>
+      <c r="BY194" s="26"/>
+      <c r="BZ194" s="26"/>
+      <c r="CA194" s="26"/>
+      <c r="CB194" s="26"/>
+      <c r="CC194" s="26"/>
+      <c r="CD194" s="26"/>
+      <c r="CE194" s="26"/>
+      <c r="CF194" s="26"/>
+      <c r="CG194" s="26"/>
+      <c r="CH194" s="26"/>
+      <c r="CI194" s="26"/>
+      <c r="CJ194" s="26"/>
+      <c r="CK194" s="26"/>
+      <c r="CL194" s="27"/>
+      <c r="CM194" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="CN194" s="24"/>
-      <c r="CO194" s="24"/>
-      <c r="CP194" s="24"/>
-      <c r="CQ194" s="24"/>
-      <c r="CR194" s="24"/>
-      <c r="CS194" s="24"/>
-      <c r="CT194" s="24"/>
-      <c r="CU194" s="24"/>
-      <c r="CV194" s="25"/>
-      <c r="CW194" s="23" t="s">
+      <c r="CN194" s="26"/>
+      <c r="CO194" s="26"/>
+      <c r="CP194" s="26"/>
+      <c r="CQ194" s="26"/>
+      <c r="CR194" s="26"/>
+      <c r="CS194" s="26"/>
+      <c r="CT194" s="26"/>
+      <c r="CU194" s="26"/>
+      <c r="CV194" s="27"/>
+      <c r="CW194" s="44" t="s">
         <v>404</v>
       </c>
-      <c r="CX194" s="24"/>
-      <c r="CY194" s="24"/>
-      <c r="CZ194" s="24"/>
-      <c r="DA194" s="24"/>
-      <c r="DB194" s="24"/>
-      <c r="DC194" s="24"/>
-      <c r="DD194" s="24"/>
-      <c r="DE194" s="24"/>
-      <c r="DF194" s="25"/>
+      <c r="CX194" s="26"/>
+      <c r="CY194" s="26"/>
+      <c r="CZ194" s="26"/>
+      <c r="DA194" s="26"/>
+      <c r="DB194" s="26"/>
+      <c r="DC194" s="26"/>
+      <c r="DD194" s="26"/>
+      <c r="DE194" s="26"/>
+      <c r="DF194" s="27"/>
     </row>
     <row r="195" spans="1:110" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A195" s="45"/>
+      <c r="A195" s="24"/>
       <c r="B195" s="12" t="s">
         <v>2</v>
       </c>
@@ -27645,7 +27675,7 @@
       </c>
     </row>
     <row r="197" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A197" s="37" t="s">
+      <c r="A197" s="32" t="s">
         <v>119</v>
       </c>
       <c r="B197" s="2" t="s">
@@ -27700,7 +27730,9 @@
       <c r="AU197" s="20"/>
       <c r="AV197" s="20"/>
       <c r="AW197" s="20"/>
-      <c r="AX197" s="20"/>
+      <c r="AX197" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AY197" s="20" t="s">
         <v>425</v>
       </c>
@@ -27767,7 +27799,7 @@
       <c r="DF197" s="20"/>
     </row>
     <row r="198" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A198" s="38"/>
+      <c r="A198" s="33"/>
       <c r="B198" s="2" t="s">
         <v>250</v>
       </c>
@@ -27820,7 +27852,9 @@
       <c r="AU198" s="20"/>
       <c r="AV198" s="20"/>
       <c r="AW198" s="20"/>
-      <c r="AX198" s="20"/>
+      <c r="AX198" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AY198" s="20" t="s">
         <v>425</v>
       </c>
@@ -27887,7 +27921,7 @@
       <c r="DF198" s="20"/>
     </row>
     <row r="199" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A199" s="34" t="s">
+      <c r="A199" s="30" t="s">
         <v>120</v>
       </c>
       <c r="B199" s="3" t="s">
@@ -28005,7 +28039,7 @@
       <c r="DF199" s="21"/>
     </row>
     <row r="200" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A200" s="35"/>
+      <c r="A200" s="31"/>
       <c r="B200" s="3" t="s">
         <v>251</v>
       </c>
@@ -28123,7 +28157,7 @@
       <c r="DF200" s="21"/>
     </row>
     <row r="201" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A201" s="37" t="s">
+      <c r="A201" s="32" t="s">
         <v>121</v>
       </c>
       <c r="B201" s="2" t="s">
@@ -28243,7 +28277,7 @@
       <c r="DF201" s="20"/>
     </row>
     <row r="202" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A202" s="38"/>
+      <c r="A202" s="33"/>
       <c r="B202" s="2" t="s">
         <v>182</v>
       </c>
@@ -28361,7 +28395,7 @@
       <c r="DF202" s="20"/>
     </row>
     <row r="203" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A203" s="38"/>
+      <c r="A203" s="33"/>
       <c r="B203" s="2" t="s">
         <v>181</v>
       </c>
@@ -28479,7 +28513,7 @@
       <c r="DF203" s="20"/>
     </row>
     <row r="204" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A204" s="34" t="s">
+      <c r="A204" s="30" t="s">
         <v>122</v>
       </c>
       <c r="B204" s="3" t="s">
@@ -28603,7 +28637,7 @@
       <c r="DF204" s="21"/>
     </row>
     <row r="205" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A205" s="35"/>
+      <c r="A205" s="31"/>
       <c r="B205" s="3" t="s">
         <v>253</v>
       </c>
@@ -28725,7 +28759,7 @@
       <c r="DF205" s="21"/>
     </row>
     <row r="206" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A206" s="35"/>
+      <c r="A206" s="31"/>
       <c r="B206" s="3" t="s">
         <v>254</v>
       </c>
@@ -28845,7 +28879,7 @@
       <c r="DF206" s="21"/>
     </row>
     <row r="207" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A207" s="35"/>
+      <c r="A207" s="31"/>
       <c r="B207" s="3" t="s">
         <v>255</v>
       </c>
@@ -28965,7 +28999,7 @@
       <c r="DF207" s="21"/>
     </row>
     <row r="208" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A208" s="37" t="s">
+      <c r="A208" s="32" t="s">
         <v>123</v>
       </c>
       <c r="B208" s="2" t="s">
@@ -29089,7 +29123,7 @@
       <c r="DF208" s="20"/>
     </row>
     <row r="209" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A209" s="38"/>
+      <c r="A209" s="33"/>
       <c r="B209" s="2" t="s">
         <v>257</v>
       </c>
@@ -29209,7 +29243,7 @@
       <c r="DF209" s="20"/>
     </row>
     <row r="210" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A210" s="38"/>
+      <c r="A210" s="33"/>
       <c r="B210" s="2" t="s">
         <v>258</v>
       </c>
@@ -29325,7 +29359,7 @@
       <c r="DF210" s="20"/>
     </row>
     <row r="211" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A211" s="34" t="s">
+      <c r="A211" s="30" t="s">
         <v>124</v>
       </c>
       <c r="B211" s="3" t="s">
@@ -29449,7 +29483,7 @@
       <c r="DF211" s="21"/>
     </row>
     <row r="212" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A212" s="35"/>
+      <c r="A212" s="31"/>
       <c r="B212" s="3" t="s">
         <v>256</v>
       </c>
@@ -29565,7 +29599,7 @@
       <c r="DF212" s="21"/>
     </row>
     <row r="213" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A213" s="35"/>
+      <c r="A213" s="31"/>
       <c r="B213" s="3" t="s">
         <v>142</v>
       </c>
@@ -29685,7 +29719,7 @@
       <c r="DF213" s="21"/>
     </row>
     <row r="214" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A214" s="35"/>
+      <c r="A214" s="31"/>
       <c r="B214" s="3" t="s">
         <v>141</v>
       </c>
@@ -29799,7 +29833,7 @@
       <c r="DF214" s="21"/>
     </row>
     <row r="215" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A215" s="35"/>
+      <c r="A215" s="31"/>
       <c r="B215" s="3" t="s">
         <v>222</v>
       </c>
@@ -29913,7 +29947,7 @@
       <c r="DF215" s="21"/>
     </row>
     <row r="216" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A216" s="37" t="s">
+      <c r="A216" s="32" t="s">
         <v>125</v>
       </c>
       <c r="B216" s="2" t="s">
@@ -30029,7 +30063,7 @@
       <c r="DF216" s="20"/>
     </row>
     <row r="217" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A217" s="38"/>
+      <c r="A217" s="33"/>
       <c r="B217" s="2" t="s">
         <v>260</v>
       </c>
@@ -30143,7 +30177,7 @@
       <c r="DF217" s="20"/>
     </row>
     <row r="218" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A218" s="34" t="s">
+      <c r="A218" s="30" t="s">
         <v>126</v>
       </c>
       <c r="B218" s="3" t="s">
@@ -30259,7 +30293,7 @@
       <c r="DF218" s="21"/>
     </row>
     <row r="219" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A219" s="35"/>
+      <c r="A219" s="31"/>
       <c r="B219" s="3" t="s">
         <v>272</v>
       </c>
@@ -30373,7 +30407,7 @@
       <c r="DF219" s="21"/>
     </row>
     <row r="220" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A220" s="35"/>
+      <c r="A220" s="31"/>
       <c r="B220" s="3" t="s">
         <v>273</v>
       </c>
@@ -30487,7 +30521,7 @@
       <c r="DF220" s="21"/>
     </row>
     <row r="221" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A221" s="37" t="s">
+      <c r="A221" s="32" t="s">
         <v>127</v>
       </c>
       <c r="B221" s="2" t="s">
@@ -30605,7 +30639,7 @@
       <c r="DF221" s="20"/>
     </row>
     <row r="222" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A222" s="38"/>
+      <c r="A222" s="33"/>
       <c r="B222" s="2" t="s">
         <v>271</v>
       </c>
@@ -30721,7 +30755,7 @@
       <c r="DF222" s="20"/>
     </row>
     <row r="223" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A223" s="34" t="s">
+      <c r="A223" s="30" t="s">
         <v>128</v>
       </c>
       <c r="B223" s="3" t="s">
@@ -30769,10 +30803,18 @@
       <c r="AN223" s="21"/>
       <c r="AO223" s="21"/>
       <c r="AP223" s="21"/>
-      <c r="AQ223" s="21"/>
-      <c r="AR223" s="21"/>
-      <c r="AS223" s="21"/>
-      <c r="AT223" s="21"/>
+      <c r="AQ223" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="AR223" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="AS223" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="AT223" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AU223" s="21"/>
       <c r="AV223" s="21"/>
       <c r="AW223" s="21"/>
@@ -30839,7 +30881,7 @@
       <c r="DF223" s="21"/>
     </row>
     <row r="224" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A224" s="35"/>
+      <c r="A224" s="31"/>
       <c r="B224" s="3" t="s">
         <v>269</v>
       </c>
@@ -30889,10 +30931,14 @@
       <c r="AN224" s="21"/>
       <c r="AO224" s="21"/>
       <c r="AP224" s="21"/>
-      <c r="AQ224" s="21"/>
+      <c r="AQ224" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="AR224" s="21"/>
       <c r="AS224" s="21"/>
-      <c r="AT224" s="21"/>
+      <c r="AT224" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="AU224" s="21"/>
       <c r="AV224" s="21"/>
       <c r="AW224" s="21"/>
@@ -30959,7 +31005,7 @@
       <c r="DF224" s="21"/>
     </row>
     <row r="225" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A225" s="35"/>
+      <c r="A225" s="31"/>
       <c r="B225" s="3" t="s">
         <v>270</v>
       </c>
@@ -31007,10 +31053,16 @@
       <c r="AN225" s="21"/>
       <c r="AO225" s="21"/>
       <c r="AP225" s="21"/>
-      <c r="AQ225" s="21"/>
-      <c r="AR225" s="21"/>
+      <c r="AQ225" s="21" t="s">
+        <v>429</v>
+      </c>
+      <c r="AR225" s="21" t="s">
+        <v>425</v>
+      </c>
       <c r="AS225" s="21"/>
-      <c r="AT225" s="21"/>
+      <c r="AT225" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="AU225" s="21"/>
       <c r="AV225" s="21"/>
       <c r="AW225" s="21"/>
@@ -31077,7 +31129,7 @@
       <c r="DF225" s="21"/>
     </row>
     <row r="226" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A226" s="35"/>
+      <c r="A226" s="31"/>
       <c r="B226" s="3" t="s">
         <v>266</v>
       </c>
@@ -31125,10 +31177,14 @@
       <c r="AN226" s="21"/>
       <c r="AO226" s="21"/>
       <c r="AP226" s="21"/>
-      <c r="AQ226" s="21"/>
+      <c r="AQ226" s="21" t="s">
+        <v>429</v>
+      </c>
       <c r="AR226" s="21"/>
       <c r="AS226" s="21"/>
-      <c r="AT226" s="21"/>
+      <c r="AT226" s="21" t="s">
+        <v>430</v>
+      </c>
       <c r="AU226" s="21"/>
       <c r="AV226" s="21"/>
       <c r="AW226" s="21"/>
@@ -31195,7 +31251,7 @@
       <c r="DF226" s="21"/>
     </row>
     <row r="227" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A227" s="37" t="s">
+      <c r="A227" s="32" t="s">
         <v>129</v>
       </c>
       <c r="B227" s="2" t="s">
@@ -31241,13 +31297,19 @@
       <c r="AN227" s="20"/>
       <c r="AO227" s="20"/>
       <c r="AP227" s="20"/>
-      <c r="AQ227" s="20"/>
+      <c r="AQ227" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="AR227" s="20"/>
       <c r="AS227" s="20"/>
-      <c r="AT227" s="20"/>
+      <c r="AT227" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AU227" s="20"/>
       <c r="AV227" s="20"/>
-      <c r="AW227" s="20"/>
+      <c r="AW227" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="AX227" s="20"/>
       <c r="AY227" s="20"/>
       <c r="AZ227" s="20"/>
@@ -31311,7 +31373,7 @@
       <c r="DF227" s="20"/>
     </row>
     <row r="228" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A228" s="38"/>
+      <c r="A228" s="33"/>
       <c r="B228" s="2" t="s">
         <v>267</v>
       </c>
@@ -31355,13 +31417,19 @@
       <c r="AN228" s="20"/>
       <c r="AO228" s="20"/>
       <c r="AP228" s="20"/>
-      <c r="AQ228" s="20"/>
+      <c r="AQ228" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AR228" s="20"/>
       <c r="AS228" s="20"/>
-      <c r="AT228" s="20"/>
+      <c r="AT228" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="AU228" s="20"/>
       <c r="AV228" s="20"/>
-      <c r="AW228" s="20"/>
+      <c r="AW228" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="AX228" s="20"/>
       <c r="AY228" s="20"/>
       <c r="AZ228" s="20"/>
@@ -31425,7 +31493,7 @@
       <c r="DF228" s="20"/>
     </row>
     <row r="229" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A229" s="38"/>
+      <c r="A229" s="33"/>
       <c r="B229" s="2" t="s">
         <v>268</v>
       </c>
@@ -31469,13 +31537,19 @@
       <c r="AN229" s="20"/>
       <c r="AO229" s="20"/>
       <c r="AP229" s="20"/>
-      <c r="AQ229" s="20"/>
+      <c r="AQ229" s="20" t="s">
+        <v>425</v>
+      </c>
       <c r="AR229" s="20"/>
       <c r="AS229" s="20"/>
-      <c r="AT229" s="20"/>
+      <c r="AT229" s="20" t="s">
+        <v>430</v>
+      </c>
       <c r="AU229" s="20"/>
       <c r="AV229" s="20"/>
-      <c r="AW229" s="20"/>
+      <c r="AW229" s="20" t="s">
+        <v>429</v>
+      </c>
       <c r="AX229" s="20"/>
       <c r="AY229" s="20"/>
       <c r="AZ229" s="20"/>
@@ -31539,7 +31613,7 @@
       <c r="DF229" s="20"/>
     </row>
     <row r="230" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A230" s="34" t="s">
+      <c r="A230" s="30" t="s">
         <v>130</v>
       </c>
       <c r="B230" s="3" t="s">
@@ -31655,7 +31729,7 @@
       <c r="DF230" s="21"/>
     </row>
     <row r="231" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A231" s="35"/>
+      <c r="A231" s="31"/>
       <c r="B231" s="3" t="s">
         <v>262</v>
       </c>
@@ -31769,7 +31843,7 @@
       <c r="DF231" s="21"/>
     </row>
     <row r="232" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A232" s="35"/>
+      <c r="A232" s="31"/>
       <c r="B232" s="3" t="s">
         <v>263</v>
       </c>
@@ -31883,7 +31957,7 @@
       <c r="DF232" s="21"/>
     </row>
     <row r="233" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A233" s="37" t="s">
+      <c r="A233" s="32" t="s">
         <v>131</v>
       </c>
       <c r="B233" s="2" t="s">
@@ -32005,7 +32079,7 @@
       <c r="DF233" s="20"/>
     </row>
     <row r="234" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A234" s="38"/>
+      <c r="A234" s="33"/>
       <c r="B234" s="2" t="s">
         <v>139</v>
       </c>
@@ -32121,7 +32195,7 @@
       <c r="DF234" s="20"/>
     </row>
     <row r="235" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A235" s="34" t="s">
+      <c r="A235" s="30" t="s">
         <v>132</v>
       </c>
       <c r="B235" s="3" t="s">
@@ -32243,7 +32317,7 @@
       <c r="DF235" s="21"/>
     </row>
     <row r="236" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A236" s="35"/>
+      <c r="A236" s="31"/>
       <c r="B236" s="3" t="s">
         <v>141</v>
       </c>
@@ -32361,7 +32435,7 @@
       <c r="DF236" s="21"/>
     </row>
     <row r="237" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A237" s="35"/>
+      <c r="A237" s="31"/>
       <c r="B237" s="3" t="s">
         <v>264</v>
       </c>
@@ -32477,7 +32551,7 @@
       <c r="DF237" s="21"/>
     </row>
     <row r="238" spans="1:110" ht="6" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A238" s="36"/>
+      <c r="A238" s="52"/>
       <c r="B238" s="3" t="s">
         <v>142</v>
       </c>
@@ -32596,50 +32670,45 @@
     </row>
   </sheetData>
   <mergeCells count="107">
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="C1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="J1:X1"/>
-    <mergeCell ref="Y1:AP1"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A32"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A38:A41"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A11:A14"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="A62:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A52"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A58"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A101:A103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="A109:A114"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A117:A120"/>
-    <mergeCell ref="A80:A86"/>
-    <mergeCell ref="A87:A90"/>
-    <mergeCell ref="A91:A96"/>
-    <mergeCell ref="A97:A98"/>
-    <mergeCell ref="A99:A100"/>
-    <mergeCell ref="A139:A142"/>
-    <mergeCell ref="C143:F143"/>
-    <mergeCell ref="G143:I143"/>
-    <mergeCell ref="J143:X143"/>
-    <mergeCell ref="A121:A124"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="A128:A131"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="CW1:DF1"/>
+    <mergeCell ref="CW143:DF143"/>
+    <mergeCell ref="CW194:DF194"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="J73:X73"/>
+    <mergeCell ref="Y73:AP73"/>
+    <mergeCell ref="AQ73:BA73"/>
+    <mergeCell ref="BB73:BP73"/>
+    <mergeCell ref="BQ73:BT73"/>
+    <mergeCell ref="BU73:CL73"/>
+    <mergeCell ref="CM73:CV73"/>
+    <mergeCell ref="CW73:DF73"/>
+    <mergeCell ref="CM194:CV194"/>
+    <mergeCell ref="AQ1:BA1"/>
+    <mergeCell ref="BB1:BP1"/>
+    <mergeCell ref="BQ1:BT1"/>
+    <mergeCell ref="BU1:CL1"/>
+    <mergeCell ref="CM1:CV1"/>
+    <mergeCell ref="BU194:CL194"/>
+    <mergeCell ref="A235:A238"/>
+    <mergeCell ref="A221:A222"/>
+    <mergeCell ref="A223:A226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="A230:A232"/>
+    <mergeCell ref="A233:A234"/>
+    <mergeCell ref="A208:A210"/>
+    <mergeCell ref="A211:A215"/>
+    <mergeCell ref="A216:A217"/>
+    <mergeCell ref="A218:A220"/>
+    <mergeCell ref="A188:A190"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="A199:A200"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A204:A207"/>
+    <mergeCell ref="Y194:AP194"/>
+    <mergeCell ref="AQ194:BA194"/>
+    <mergeCell ref="BB194:BP194"/>
+    <mergeCell ref="BQ194:BT194"/>
     <mergeCell ref="A156:A159"/>
     <mergeCell ref="A160:A164"/>
     <mergeCell ref="A165:A167"/>
@@ -32664,45 +32733,50 @@
     <mergeCell ref="A179:A183"/>
     <mergeCell ref="A184:A185"/>
     <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A188:A190"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="A199:A200"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A204:A207"/>
-    <mergeCell ref="Y194:AP194"/>
-    <mergeCell ref="AQ194:BA194"/>
-    <mergeCell ref="BB194:BP194"/>
-    <mergeCell ref="BQ194:BT194"/>
-    <mergeCell ref="A235:A238"/>
-    <mergeCell ref="A221:A222"/>
-    <mergeCell ref="A223:A226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="A230:A232"/>
-    <mergeCell ref="A233:A234"/>
-    <mergeCell ref="A208:A210"/>
-    <mergeCell ref="A211:A215"/>
-    <mergeCell ref="A216:A217"/>
-    <mergeCell ref="A218:A220"/>
-    <mergeCell ref="CW1:DF1"/>
-    <mergeCell ref="CW143:DF143"/>
-    <mergeCell ref="CW194:DF194"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="J73:X73"/>
-    <mergeCell ref="Y73:AP73"/>
-    <mergeCell ref="AQ73:BA73"/>
-    <mergeCell ref="BB73:BP73"/>
-    <mergeCell ref="BQ73:BT73"/>
-    <mergeCell ref="BU73:CL73"/>
-    <mergeCell ref="CM73:CV73"/>
-    <mergeCell ref="CW73:DF73"/>
-    <mergeCell ref="CM194:CV194"/>
-    <mergeCell ref="AQ1:BA1"/>
-    <mergeCell ref="BB1:BP1"/>
-    <mergeCell ref="BQ1:BT1"/>
-    <mergeCell ref="BU1:CL1"/>
-    <mergeCell ref="CM1:CV1"/>
-    <mergeCell ref="BU194:CL194"/>
+    <mergeCell ref="A139:A142"/>
+    <mergeCell ref="C143:F143"/>
+    <mergeCell ref="G143:I143"/>
+    <mergeCell ref="J143:X143"/>
+    <mergeCell ref="A121:A124"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="A128:A131"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="A134:A138"/>
+    <mergeCell ref="A101:A103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A109:A114"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A117:A120"/>
+    <mergeCell ref="A80:A86"/>
+    <mergeCell ref="A87:A90"/>
+    <mergeCell ref="A91:A96"/>
+    <mergeCell ref="A97:A98"/>
+    <mergeCell ref="A99:A100"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A76:A77"/>
+    <mergeCell ref="A78:A79"/>
+    <mergeCell ref="A62:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A52"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A58"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:X1"/>
+    <mergeCell ref="Y1:AP1"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A32"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="A36:A37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="40" orientation="portrait" r:id="rId1"/>

</xml_diff>